<commit_message>
Fix default delivery test
</commit_message>
<xml_diff>
--- a/config/default/forms/app/delivery.xlsx
+++ b/config/default/forms/app/delivery.xlsx
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="744">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -2986,14 +2986,14 @@
   <dimension ref="A1:AJ301"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C234" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="K36" activeCellId="0" sqref="K36"/>
+      <selection pane="bottomLeft" activeCell="A234" activeCellId="0" sqref="A234"/>
+      <selection pane="bottomRight" activeCell="J269" activeCellId="0" sqref="J269"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.29"/>
@@ -9494,9 +9494,7 @@
       <c r="G142" s="25"/>
       <c r="H142" s="25"/>
       <c r="I142" s="25"/>
-      <c r="J142" s="26" t="s">
-        <v>102</v>
-      </c>
+      <c r="J142" s="26"/>
       <c r="K142" s="26" t="s">
         <v>288</v>
       </c>
@@ -9636,9 +9634,7 @@
       <c r="G145" s="25"/>
       <c r="H145" s="25"/>
       <c r="I145" s="25"/>
-      <c r="J145" s="26" t="s">
-        <v>102</v>
-      </c>
+      <c r="J145" s="26"/>
       <c r="K145" s="26"/>
       <c r="L145" s="26"/>
       <c r="M145" s="26"/>
@@ -16903,7 +16899,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="2" style="0" width="45.86"/>
@@ -20216,7 +20212,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.57"/>
@@ -20274,7 +20270,7 @@
       </c>
       <c r="C2" s="59" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2021-08-31  8-32</v>
+        <v>2021-09-02  10-00</v>
       </c>
       <c r="D2" s="60" t="s">
         <v>649</v>
@@ -20330,7 +20326,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="2" style="0" width="45.86"/>

</xml_diff>

<commit_message>
Reset default delivery form
</commit_message>
<xml_diff>
--- a/config/default/forms/app/delivery.xlsx
+++ b/config/default/forms/app/delivery.xlsx
@@ -375,7 +375,7 @@
     <t xml:space="preserve">patient_age_in_years</t>
   </si>
   <si>
-    <t xml:space="preserve">floor( difference-in-months( date(../inputs/contact/date_of_birth), today() ) div 12 )</t>
+    <t xml:space="preserve">floor( difference-in-months( ../inputs/contact/date_of_birth, today() ) div 12 )</t>
   </si>
   <si>
     <t xml:space="preserve">patient_uuid</t>
@@ -515,7 +515,7 @@
     <t xml:space="preserve">Date of death</t>
   </si>
   <si>
-    <t xml:space="preserve">decimal-date-time(.) &lt;= floor(decimal-date-time(today())) and difference-in-months( date(.), today() ) &lt; 1</t>
+    <t xml:space="preserve">decimal-date-time(.) &lt;= floor(decimal-date-time(today())) and difference-in-months( ., today() ) &lt; 1</t>
   </si>
   <si>
     <t xml:space="preserve">Date cannot be in the future and older than a month from today.</t>
@@ -2986,16 +2986,16 @@
   <dimension ref="A1:AJ301"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C234" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C275" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A234" activeCellId="0" sqref="A234"/>
-      <selection pane="bottomRight" activeCell="J269" activeCellId="0" sqref="J269"/>
+      <selection pane="bottomLeft" activeCell="A275" activeCellId="0" sqref="A275"/>
+      <selection pane="bottomRight" activeCell="J310" activeCellId="0" sqref="J310"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.29"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="4" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="0" width="8.71"/>
@@ -3007,7 +3007,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="32.71"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="20" min="15" style="0" width="25.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="73.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="30.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="30.01"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="29" min="24" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="31" style="0" width="29.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="49"/>
@@ -16899,7 +16899,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="2" style="0" width="45.86"/>
@@ -20212,9 +20212,9 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.57"/>
   </cols>
@@ -20270,7 +20270,7 @@
       </c>
       <c r="C2" s="59" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2021-09-02  10-00</v>
+        <v>2021-09-08  9-19</v>
       </c>
       <c r="D2" s="60" t="s">
         <v>649</v>
@@ -20318,7 +20318,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W1000"/>
+  <dimension ref="A1:W75"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -20326,7 +20326,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="2" style="0" width="45.86"/>

</xml_diff>

<commit_message>
Update default app forms to pass validation
</commit_message>
<xml_diff>
--- a/config/default/forms/app/delivery.xlsx
+++ b/config/default/forms/app/delivery.xlsx
@@ -1448,7 +1448,7 @@
   <si>
     <t xml:space="preserve">selected(../../condition/woman_outcome, 'alive_well') or
 selected(../../condition/woman_outcome, 'alive_unwell') or
-../delivery_outcome/babies_alive_num &gt; 0 or
+../../delivery_outcome/babies_alive_num &gt; 0 or
 ../../pnc_visits/pnc_visits_additional != ''</t>
   </si>
   <si>
@@ -2417,10 +2417,10 @@
   <numFmts count="1">
     <numFmt numFmtId="160" formatCode="dd\-mm\-yyyy\ hh\-mm\-ss"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <name val="Arial"/>
-      <color indexed="64"/>
+      <color theme="1"/>
       <sz val="10.000000"/>
     </font>
     <font>
@@ -2443,29 +2443,16 @@
     </font>
     <font>
       <name val="Arial"/>
-      <color indexed="64"/>
-      <sz val="11.000000"/>
-    </font>
-    <font>
-      <name val="Arial"/>
       <sz val="11.000000"/>
     </font>
     <font>
       <name val="Arial"/>
       <b/>
-      <color indexed="64"/>
-      <sz val="10.000000"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <b/>
-      <color indexed="64"/>
       <sz val="11.000000"/>
     </font>
     <font>
       <name val="Calibri"/>
       <b/>
-      <color indexed="64"/>
       <sz val="11.000000"/>
     </font>
   </fonts>
@@ -2586,7 +2573,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="65">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -2735,38 +2722,38 @@
       <alignment horizontal="left"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="6" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="0">
+    <xf fontId="5" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="7" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="7" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="2" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="7" fillId="13" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="2" fillId="13" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="7" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="2" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="7" fillId="14" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="2" fillId="14" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="7" fillId="15" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="2" fillId="15" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="7" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="2" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="7" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="2" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
@@ -2774,14 +2761,14 @@
       <alignment horizontal="left"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
+    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
       <protection hidden="0" locked="1"/>
     </xf>
@@ -2793,45 +2780,38 @@
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
     <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="9" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="7" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="9" fillId="13" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="7" fillId="13" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="9" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="7" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="9" fillId="14" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="7" fillId="14" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="9" fillId="15" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="7" fillId="15" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="9" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="7" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="9" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="7" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
-      <alignment wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
@@ -2860,7 +2840,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName=" " id="{7340FC0C-B4EF-7CF6-D8BF-479DF1898AC4}"/>
+  <person displayName=" " id="{16F6E003-524F-F17E-22FB-BCB874643EBA}"/>
 </personList>
 </file>
 
@@ -3276,7 +3256,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="U266" personId="{7340FC0C-B4EF-7CF6-D8BF-479DF1898AC4}" id="{0024000F-00D4-40FA-8C20-0081001200D2}" done="0">
+  <threadedComment ref="U266" personId="{16F6E003-524F-F17E-22FB-BCB874643EBA}" id="{0024000F-00D4-40FA-8C20-0081001200D2}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org is there a reason we are using .. instead of ${} for these? It would be more consistent if we could use $
 _Assigned to you_
 -Michael Kohn
@@ -3298,7 +3278,7 @@
 -Michael Kohn
 </text>
   </threadedComment>
-  <threadedComment ref="U294" personId="{7340FC0C-B4EF-7CF6-D8BF-479DF1898AC4}" id="{00800045-00BB-493D-B802-00C800B500C8}" done="0">
+  <threadedComment ref="U294" personId="{16F6E003-524F-F17E-22FB-BCB874643EBA}" id="{00800045-00BB-493D-B802-00C800B500C8}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org in some of the other forms i see this as ../../patient_id instead, not sure if it matters but feel like we should be consistent. I can update it based on your input. Also not sure why some of the ones below have ../../inputs and this one is ../inputs.
 _Assigned to you_
 -Michael Kohn
@@ -3311,7 +3291,7 @@
 -Michael Kohn
 </text>
   </threadedComment>
-  <threadedComment ref="U298" personId="{7340FC0C-B4EF-7CF6-D8BF-479DF1898AC4}" id="{00660081-00F5-41A0-8991-00C6004C00A7}" done="0">
+  <threadedComment ref="U298" personId="{16F6E003-524F-F17E-22FB-BCB874643EBA}" id="{00660081-00F5-41A0-8991-00C6004C00A7}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org in other forms there is a calculate field called pregnancy_uuid_ctx. To be consistent, it feels like we should either add that calculate field to this form and use that for this calculation, or update the other forms to use the "instance('contact-summary'......)" notation. I'd actually prefer to update the other forms to use the "instance('contact-summary'....)" notation because in general i was trying to avoid referencing those top level calculate fields in the data section (there are exceptions). Do you have a preference?
 _Assigned to you_
 -Michael Kohn
@@ -3321,7 +3301,7 @@
 -Marc Abbyad
 </text>
   </threadedComment>
-  <threadedComment ref="AI1" personId="{7340FC0C-B4EF-7CF6-D8BF-479DF1898AC4}" id="{00A000D4-0058-42D9-AAD4-004A00F70029}" done="0">
+  <threadedComment ref="AI1" personId="{16F6E003-524F-F17E-22FB-BCB874643EBA}" id="{00A000D4-0058-42D9-AAD4-004A00F70029}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org just FYI i moved these "instance" columns to be after the cht::notes column so that all forms have the same columns in the same order up to AH. Personally I'd probably prefer that all forms have the same exact columns in the same order, even if not all columns are needed for that form.
 _Assigned to you_
 -Michael Kohn
@@ -17222,7 +17202,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{002700AA-00D7-4C35-98DB-000A00E800DF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{007A00F1-00AD-49F4-BF2A-0051005A007F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -17231,7 +17211,7 @@
           </x14:formula2>
           <xm:sqref>J2:J43 J45:J291 J293:J301</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00ED00F2-0002-4BC3-8FEF-000E00F1006F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00DF006E-0053-4943-954A-00EB0094006F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -20625,7 +20605,7 @@
       </c>
       <c r="C2" s="53" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-06-14 15-07</v>
+        <v xml:space="preserve">2022-08-19 15-13</v>
       </c>
       <c r="D2" s="54" t="s">
         <v>649</v>
@@ -20634,7 +20614,7 @@
         <v>491</v>
       </c>
       <c r="F2" s="55"/>
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="55" t="s">
         <v>650</v>
       </c>
       <c r="H2" s="55"/>
@@ -20690,25 +20670,25 @@
       <c r="B1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="G1" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="62" t="s">
+      <c r="H1" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="63" t="s">
+      <c r="I1" s="62" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="55"/>
@@ -20727,960 +20707,960 @@
       <c r="W1" s="55"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="63" t="s">
         <v>585</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="63" t="s">
         <v>586</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="64"/>
-      <c r="U2" s="64"/>
-      <c r="V2" s="64"/>
-      <c r="W2" s="64"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="63"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="63" t="s">
         <v>585</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="63" t="s">
         <v>138</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="63" t="s">
         <v>587</v>
       </c>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="63"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="63"/>
+      <c r="U3" s="63"/>
+      <c r="V3" s="63"/>
+      <c r="W3" s="63"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="64"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
-      <c r="O4" s="64"/>
-      <c r="P4" s="64"/>
-      <c r="Q4" s="64"/>
-      <c r="R4" s="64"/>
-      <c r="S4" s="64"/>
-      <c r="T4" s="64"/>
-      <c r="U4" s="64"/>
-      <c r="V4" s="64"/>
-      <c r="W4" s="64"/>
+      <c r="A4" s="63"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="63"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="63"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="63"/>
+      <c r="T4" s="63"/>
+      <c r="U4" s="63"/>
+      <c r="V4" s="63"/>
+      <c r="W4" s="63"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="63" t="s">
         <v>651</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="63" t="s">
         <v>652</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="63" t="s">
         <v>653</v>
       </c>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="64"/>
-      <c r="N5" s="64"/>
-      <c r="O5" s="64"/>
-      <c r="P5" s="64"/>
-      <c r="Q5" s="64"/>
-      <c r="R5" s="64"/>
-      <c r="S5" s="64"/>
-      <c r="T5" s="64"/>
-      <c r="U5" s="64"/>
-      <c r="V5" s="64"/>
-      <c r="W5" s="64"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="63"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="63"/>
+      <c r="U5" s="63"/>
+      <c r="V5" s="63"/>
+      <c r="W5" s="63"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="63" t="s">
         <v>651</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="63" t="s">
         <v>654</v>
       </c>
-      <c r="C6" s="64" t="s">
+      <c r="C6" s="63" t="s">
         <v>655</v>
       </c>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="64"/>
-      <c r="N6" s="64"/>
-      <c r="O6" s="64"/>
-      <c r="P6" s="64"/>
-      <c r="Q6" s="64"/>
-      <c r="R6" s="64"/>
-      <c r="S6" s="64"/>
-      <c r="T6" s="64"/>
-      <c r="U6" s="64"/>
-      <c r="V6" s="64"/>
-      <c r="W6" s="64"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="63"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
+      <c r="V6" s="63"/>
+      <c r="W6" s="63"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="63" t="s">
         <v>651</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="63" t="s">
         <v>656</v>
       </c>
-      <c r="C7" s="64" t="s">
+      <c r="C7" s="63" t="s">
         <v>657</v>
       </c>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="64"/>
-      <c r="M7" s="64"/>
-      <c r="N7" s="64"/>
-      <c r="O7" s="64"/>
-      <c r="P7" s="64"/>
-      <c r="Q7" s="64"/>
-      <c r="R7" s="64"/>
-      <c r="S7" s="64"/>
-      <c r="T7" s="64"/>
-      <c r="U7" s="64"/>
-      <c r="V7" s="64"/>
-      <c r="W7" s="64"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="63"/>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="63"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="63"/>
+      <c r="W7" s="63"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="63" t="s">
         <v>651</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="63" t="s">
         <v>658</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="63" t="s">
         <v>659</v>
       </c>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="64"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="64"/>
-      <c r="N8" s="64"/>
-      <c r="O8" s="64"/>
-      <c r="P8" s="64"/>
-      <c r="Q8" s="64"/>
-      <c r="R8" s="64"/>
-      <c r="S8" s="64"/>
-      <c r="T8" s="64"/>
-      <c r="U8" s="64"/>
-      <c r="V8" s="64"/>
-      <c r="W8" s="64"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63"/>
+      <c r="N8" s="63"/>
+      <c r="O8" s="63"/>
+      <c r="P8" s="63"/>
+      <c r="Q8" s="63"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="63"/>
+      <c r="U8" s="63"/>
+      <c r="V8" s="63"/>
+      <c r="W8" s="63"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="63" t="s">
         <v>651</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="63" t="s">
         <v>660</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" s="63" t="s">
         <v>661</v>
       </c>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="64"/>
-      <c r="N9" s="64"/>
-      <c r="O9" s="64"/>
-      <c r="P9" s="64"/>
-      <c r="Q9" s="64"/>
-      <c r="R9" s="64"/>
-      <c r="S9" s="64"/>
-      <c r="T9" s="64"/>
-      <c r="U9" s="64"/>
-      <c r="V9" s="64"/>
-      <c r="W9" s="64"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="63"/>
+      <c r="P9" s="63"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="63"/>
+      <c r="V9" s="63"/>
+      <c r="W9" s="63"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="64"/>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="64"/>
-      <c r="N10" s="64"/>
-      <c r="O10" s="64"/>
-      <c r="P10" s="64"/>
-      <c r="Q10" s="64"/>
-      <c r="R10" s="64"/>
-      <c r="S10" s="64"/>
-      <c r="T10" s="64"/>
-      <c r="U10" s="64"/>
-      <c r="V10" s="64"/>
-      <c r="W10" s="64"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="63"/>
+      <c r="P10" s="63"/>
+      <c r="Q10" s="63"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="63"/>
+      <c r="U10" s="63"/>
+      <c r="V10" s="63"/>
+      <c r="W10" s="63"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="63" t="s">
         <v>662</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="63" t="s">
         <v>663</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="63" t="s">
         <v>664</v>
       </c>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="64"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="64"/>
-      <c r="N11" s="64"/>
-      <c r="O11" s="64"/>
-      <c r="P11" s="64"/>
-      <c r="Q11" s="64"/>
-      <c r="R11" s="64"/>
-      <c r="S11" s="64"/>
-      <c r="T11" s="64"/>
-      <c r="U11" s="64"/>
-      <c r="V11" s="64"/>
-      <c r="W11" s="64"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="63"/>
+      <c r="N11" s="63"/>
+      <c r="O11" s="63"/>
+      <c r="P11" s="63"/>
+      <c r="Q11" s="63"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="63"/>
+      <c r="T11" s="63"/>
+      <c r="U11" s="63"/>
+      <c r="V11" s="63"/>
+      <c r="W11" s="63"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="63" t="s">
         <v>662</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="63" t="s">
         <v>665</v>
       </c>
-      <c r="C12" s="64" t="s">
+      <c r="C12" s="63" t="s">
         <v>666</v>
       </c>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="64"/>
-      <c r="K12" s="64"/>
-      <c r="L12" s="64"/>
-      <c r="M12" s="64"/>
-      <c r="N12" s="64"/>
-      <c r="O12" s="64"/>
-      <c r="P12" s="64"/>
-      <c r="Q12" s="64"/>
-      <c r="R12" s="64"/>
-      <c r="S12" s="64"/>
-      <c r="T12" s="64"/>
-      <c r="U12" s="64"/>
-      <c r="V12" s="64"/>
-      <c r="W12" s="64"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="63"/>
+      <c r="P12" s="63"/>
+      <c r="Q12" s="63"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="63"/>
+      <c r="V12" s="63"/>
+      <c r="W12" s="63"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="64" t="s">
+      <c r="A13" s="63" t="s">
         <v>662</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="63" t="s">
         <v>667</v>
       </c>
-      <c r="C13" s="64" t="s">
+      <c r="C13" s="63" t="s">
         <v>668</v>
       </c>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="64"/>
-      <c r="M13" s="64"/>
-      <c r="N13" s="64"/>
-      <c r="O13" s="64"/>
-      <c r="P13" s="64"/>
-      <c r="Q13" s="64"/>
-      <c r="R13" s="64"/>
-      <c r="S13" s="64"/>
-      <c r="T13" s="64"/>
-      <c r="U13" s="64"/>
-      <c r="V13" s="64"/>
-      <c r="W13" s="64"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="63"/>
+      <c r="O13" s="63"/>
+      <c r="P13" s="63"/>
+      <c r="Q13" s="63"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="63"/>
+      <c r="U13" s="63"/>
+      <c r="V13" s="63"/>
+      <c r="W13" s="63"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="64" t="s">
+      <c r="A14" s="63" t="s">
         <v>662</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="63" t="s">
         <v>669</v>
       </c>
-      <c r="C14" s="64" t="s">
+      <c r="C14" s="63" t="s">
         <v>670</v>
       </c>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="64"/>
-      <c r="J14" s="64"/>
-      <c r="K14" s="64"/>
-      <c r="L14" s="64"/>
-      <c r="M14" s="64"/>
-      <c r="N14" s="64"/>
-      <c r="O14" s="64"/>
-      <c r="P14" s="64"/>
-      <c r="Q14" s="64"/>
-      <c r="R14" s="64"/>
-      <c r="S14" s="64"/>
-      <c r="T14" s="64"/>
-      <c r="U14" s="64"/>
-      <c r="V14" s="64"/>
-      <c r="W14" s="64"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="63"/>
+      <c r="N14" s="63"/>
+      <c r="O14" s="63"/>
+      <c r="P14" s="63"/>
+      <c r="Q14" s="63"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="63"/>
+      <c r="U14" s="63"/>
+      <c r="V14" s="63"/>
+      <c r="W14" s="63"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="64" t="s">
+      <c r="A15" s="63" t="s">
         <v>662</v>
       </c>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="63" t="s">
         <v>671</v>
       </c>
-      <c r="C15" s="64" t="s">
+      <c r="C15" s="63" t="s">
         <v>672</v>
       </c>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="64"/>
-      <c r="N15" s="64"/>
-      <c r="O15" s="64"/>
-      <c r="P15" s="64"/>
-      <c r="Q15" s="64"/>
-      <c r="R15" s="64"/>
-      <c r="S15" s="64"/>
-      <c r="T15" s="64"/>
-      <c r="U15" s="64"/>
-      <c r="V15" s="64"/>
-      <c r="W15" s="64"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="63"/>
+      <c r="O15" s="63"/>
+      <c r="P15" s="63"/>
+      <c r="Q15" s="63"/>
+      <c r="R15" s="63"/>
+      <c r="S15" s="63"/>
+      <c r="T15" s="63"/>
+      <c r="U15" s="63"/>
+      <c r="V15" s="63"/>
+      <c r="W15" s="63"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="63" t="s">
         <v>662</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="63" t="s">
         <v>673</v>
       </c>
-      <c r="C16" s="64" t="s">
+      <c r="C16" s="63" t="s">
         <v>674</v>
       </c>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="64"/>
-      <c r="I16" s="64"/>
-      <c r="J16" s="64"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="64"/>
-      <c r="M16" s="64"/>
-      <c r="N16" s="64"/>
-      <c r="O16" s="64"/>
-      <c r="P16" s="64"/>
-      <c r="Q16" s="64"/>
-      <c r="R16" s="64"/>
-      <c r="S16" s="64"/>
-      <c r="T16" s="64"/>
-      <c r="U16" s="64"/>
-      <c r="V16" s="64"/>
-      <c r="W16" s="64"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="63"/>
+      <c r="L16" s="63"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="63"/>
+      <c r="O16" s="63"/>
+      <c r="P16" s="63"/>
+      <c r="Q16" s="63"/>
+      <c r="R16" s="63"/>
+      <c r="S16" s="63"/>
+      <c r="T16" s="63"/>
+      <c r="U16" s="63"/>
+      <c r="V16" s="63"/>
+      <c r="W16" s="63"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="64"/>
-      <c r="B17" s="64"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="64"/>
-      <c r="J17" s="64"/>
-      <c r="K17" s="64"/>
-      <c r="L17" s="64"/>
-      <c r="M17" s="64"/>
-      <c r="N17" s="64"/>
-      <c r="O17" s="64"/>
-      <c r="P17" s="64"/>
-      <c r="Q17" s="64"/>
-      <c r="R17" s="64"/>
-      <c r="S17" s="64"/>
-      <c r="T17" s="64"/>
-      <c r="U17" s="64"/>
-      <c r="V17" s="64"/>
-      <c r="W17" s="64"/>
+      <c r="A17" s="63"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="63"/>
+      <c r="O17" s="63"/>
+      <c r="P17" s="63"/>
+      <c r="Q17" s="63"/>
+      <c r="R17" s="63"/>
+      <c r="S17" s="63"/>
+      <c r="T17" s="63"/>
+      <c r="U17" s="63"/>
+      <c r="V17" s="63"/>
+      <c r="W17" s="63"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="64" t="s">
+      <c r="A18" s="63" t="s">
         <v>675</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="63" t="s">
         <v>663</v>
       </c>
-      <c r="C18" s="64" t="s">
+      <c r="C18" s="63" t="s">
         <v>664</v>
       </c>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="64"/>
-      <c r="L18" s="64"/>
-      <c r="M18" s="64"/>
-      <c r="N18" s="64"/>
-      <c r="O18" s="64"/>
-      <c r="P18" s="64"/>
-      <c r="Q18" s="64"/>
-      <c r="R18" s="64"/>
-      <c r="S18" s="64"/>
-      <c r="T18" s="64"/>
-      <c r="U18" s="64"/>
-      <c r="V18" s="64"/>
-      <c r="W18" s="64"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="63"/>
+      <c r="N18" s="63"/>
+      <c r="O18" s="63"/>
+      <c r="P18" s="63"/>
+      <c r="Q18" s="63"/>
+      <c r="R18" s="63"/>
+      <c r="S18" s="63"/>
+      <c r="T18" s="63"/>
+      <c r="U18" s="63"/>
+      <c r="V18" s="63"/>
+      <c r="W18" s="63"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="64" t="s">
+      <c r="A19" s="63" t="s">
         <v>675</v>
       </c>
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="63" t="s">
         <v>665</v>
       </c>
-      <c r="C19" s="64" t="s">
+      <c r="C19" s="63" t="s">
         <v>666</v>
       </c>
-      <c r="D19" s="64"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="64"/>
-      <c r="H19" s="64"/>
-      <c r="I19" s="64"/>
-      <c r="J19" s="64"/>
-      <c r="K19" s="64"/>
-      <c r="L19" s="64"/>
-      <c r="M19" s="64"/>
-      <c r="N19" s="64"/>
-      <c r="O19" s="64"/>
-      <c r="P19" s="64"/>
-      <c r="Q19" s="64"/>
-      <c r="R19" s="64"/>
-      <c r="S19" s="64"/>
-      <c r="T19" s="64"/>
-      <c r="U19" s="64"/>
-      <c r="V19" s="64"/>
-      <c r="W19" s="64"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="63"/>
+      <c r="O19" s="63"/>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="63"/>
+      <c r="R19" s="63"/>
+      <c r="S19" s="63"/>
+      <c r="T19" s="63"/>
+      <c r="U19" s="63"/>
+      <c r="V19" s="63"/>
+      <c r="W19" s="63"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="64" t="s">
+      <c r="A20" s="63" t="s">
         <v>675</v>
       </c>
-      <c r="B20" s="64" t="s">
+      <c r="B20" s="63" t="s">
         <v>667</v>
       </c>
-      <c r="C20" s="64" t="s">
+      <c r="C20" s="63" t="s">
         <v>668</v>
       </c>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
-      <c r="J20" s="64"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="64"/>
-      <c r="M20" s="64"/>
-      <c r="N20" s="64"/>
-      <c r="O20" s="64"/>
-      <c r="P20" s="64"/>
-      <c r="Q20" s="64"/>
-      <c r="R20" s="64"/>
-      <c r="S20" s="64"/>
-      <c r="T20" s="64"/>
-      <c r="U20" s="64"/>
-      <c r="V20" s="64"/>
-      <c r="W20" s="64"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="63"/>
+      <c r="P20" s="63"/>
+      <c r="Q20" s="63"/>
+      <c r="R20" s="63"/>
+      <c r="S20" s="63"/>
+      <c r="T20" s="63"/>
+      <c r="U20" s="63"/>
+      <c r="V20" s="63"/>
+      <c r="W20" s="63"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="64" t="s">
+      <c r="A21" s="63" t="s">
         <v>675</v>
       </c>
-      <c r="B21" s="64" t="s">
+      <c r="B21" s="63" t="s">
         <v>669</v>
       </c>
-      <c r="C21" s="64" t="s">
+      <c r="C21" s="63" t="s">
         <v>670</v>
       </c>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="64"/>
-      <c r="J21" s="64"/>
-      <c r="K21" s="64"/>
-      <c r="L21" s="64"/>
-      <c r="M21" s="64"/>
-      <c r="N21" s="64"/>
-      <c r="O21" s="64"/>
-      <c r="P21" s="64"/>
-      <c r="Q21" s="64"/>
-      <c r="R21" s="64"/>
-      <c r="S21" s="64"/>
-      <c r="T21" s="64"/>
-      <c r="U21" s="64"/>
-      <c r="V21" s="64"/>
-      <c r="W21" s="64"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="63"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="63"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="63"/>
+      <c r="L21" s="63"/>
+      <c r="M21" s="63"/>
+      <c r="N21" s="63"/>
+      <c r="O21" s="63"/>
+      <c r="P21" s="63"/>
+      <c r="Q21" s="63"/>
+      <c r="R21" s="63"/>
+      <c r="S21" s="63"/>
+      <c r="T21" s="63"/>
+      <c r="U21" s="63"/>
+      <c r="V21" s="63"/>
+      <c r="W21" s="63"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="64" t="s">
+      <c r="A22" s="63" t="s">
         <v>675</v>
       </c>
-      <c r="B22" s="64" t="s">
+      <c r="B22" s="63" t="s">
         <v>673</v>
       </c>
-      <c r="C22" s="64" t="s">
+      <c r="C22" s="63" t="s">
         <v>674</v>
       </c>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="64"/>
-      <c r="K22" s="64"/>
-      <c r="L22" s="64"/>
-      <c r="M22" s="64"/>
-      <c r="N22" s="64"/>
-      <c r="O22" s="64"/>
-      <c r="P22" s="64"/>
-      <c r="Q22" s="64"/>
-      <c r="R22" s="64"/>
-      <c r="S22" s="64"/>
-      <c r="T22" s="64"/>
-      <c r="U22" s="64"/>
-      <c r="V22" s="64"/>
-      <c r="W22" s="64"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="63"/>
+      <c r="J22" s="63"/>
+      <c r="K22" s="63"/>
+      <c r="L22" s="63"/>
+      <c r="M22" s="63"/>
+      <c r="N22" s="63"/>
+      <c r="O22" s="63"/>
+      <c r="P22" s="63"/>
+      <c r="Q22" s="63"/>
+      <c r="R22" s="63"/>
+      <c r="S22" s="63"/>
+      <c r="T22" s="63"/>
+      <c r="U22" s="63"/>
+      <c r="V22" s="63"/>
+      <c r="W22" s="63"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="64" t="s">
+      <c r="A23" s="63" t="s">
         <v>675</v>
       </c>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="63" t="s">
         <v>676</v>
       </c>
-      <c r="C23" s="64" t="s">
+      <c r="C23" s="63" t="s">
         <v>677</v>
       </c>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="64"/>
-      <c r="J23" s="64"/>
-      <c r="K23" s="64"/>
-      <c r="L23" s="64"/>
-      <c r="M23" s="64"/>
-      <c r="N23" s="64"/>
-      <c r="O23" s="64"/>
-      <c r="P23" s="64"/>
-      <c r="Q23" s="64"/>
-      <c r="R23" s="64"/>
-      <c r="S23" s="64"/>
-      <c r="T23" s="64"/>
-      <c r="U23" s="64"/>
-      <c r="V23" s="64"/>
-      <c r="W23" s="64"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="63"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="63"/>
+      <c r="M23" s="63"/>
+      <c r="N23" s="63"/>
+      <c r="O23" s="63"/>
+      <c r="P23" s="63"/>
+      <c r="Q23" s="63"/>
+      <c r="R23" s="63"/>
+      <c r="S23" s="63"/>
+      <c r="T23" s="63"/>
+      <c r="U23" s="63"/>
+      <c r="V23" s="63"/>
+      <c r="W23" s="63"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="64"/>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="64"/>
-      <c r="G24" s="64"/>
-      <c r="H24" s="64"/>
-      <c r="I24" s="64"/>
-      <c r="J24" s="64"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="64"/>
-      <c r="M24" s="64"/>
-      <c r="N24" s="64"/>
-      <c r="O24" s="64"/>
-      <c r="P24" s="64"/>
-      <c r="Q24" s="64"/>
-      <c r="R24" s="64"/>
-      <c r="S24" s="64"/>
-      <c r="T24" s="64"/>
-      <c r="U24" s="64"/>
-      <c r="V24" s="64"/>
-      <c r="W24" s="64"/>
+      <c r="A24" s="63"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="63"/>
+      <c r="G24" s="63"/>
+      <c r="H24" s="63"/>
+      <c r="I24" s="63"/>
+      <c r="J24" s="63"/>
+      <c r="K24" s="63"/>
+      <c r="L24" s="63"/>
+      <c r="M24" s="63"/>
+      <c r="N24" s="63"/>
+      <c r="O24" s="63"/>
+      <c r="P24" s="63"/>
+      <c r="Q24" s="63"/>
+      <c r="R24" s="63"/>
+      <c r="S24" s="63"/>
+      <c r="T24" s="63"/>
+      <c r="U24" s="63"/>
+      <c r="V24" s="63"/>
+      <c r="W24" s="63"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="64" t="s">
+      <c r="A25" s="63" t="s">
         <v>678</v>
       </c>
-      <c r="B25" s="64" t="s">
+      <c r="B25" s="63" t="s">
         <v>679</v>
       </c>
-      <c r="C25" s="64" t="s">
+      <c r="C25" s="63" t="s">
         <v>680</v>
       </c>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="64"/>
-      <c r="H25" s="64"/>
-      <c r="I25" s="64"/>
-      <c r="J25" s="64"/>
-      <c r="K25" s="64"/>
-      <c r="L25" s="64"/>
-      <c r="M25" s="64"/>
-      <c r="N25" s="64"/>
-      <c r="O25" s="64"/>
-      <c r="P25" s="64"/>
-      <c r="Q25" s="64"/>
-      <c r="R25" s="64"/>
-      <c r="S25" s="64"/>
-      <c r="T25" s="64"/>
-      <c r="U25" s="64"/>
-      <c r="V25" s="64"/>
-      <c r="W25" s="64"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="63"/>
+      <c r="J25" s="63"/>
+      <c r="K25" s="63"/>
+      <c r="L25" s="63"/>
+      <c r="M25" s="63"/>
+      <c r="N25" s="63"/>
+      <c r="O25" s="63"/>
+      <c r="P25" s="63"/>
+      <c r="Q25" s="63"/>
+      <c r="R25" s="63"/>
+      <c r="S25" s="63"/>
+      <c r="T25" s="63"/>
+      <c r="U25" s="63"/>
+      <c r="V25" s="63"/>
+      <c r="W25" s="63"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="64" t="s">
+      <c r="A26" s="63" t="s">
         <v>678</v>
       </c>
-      <c r="B26" s="64" t="s">
+      <c r="B26" s="63" t="s">
         <v>681</v>
       </c>
-      <c r="C26" s="64" t="s">
+      <c r="C26" s="63" t="s">
         <v>682</v>
       </c>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="64"/>
-      <c r="I26" s="64"/>
-      <c r="J26" s="64"/>
-      <c r="K26" s="64"/>
-      <c r="L26" s="64"/>
-      <c r="M26" s="64"/>
-      <c r="N26" s="64"/>
-      <c r="O26" s="64"/>
-      <c r="P26" s="64"/>
-      <c r="Q26" s="64"/>
-      <c r="R26" s="64"/>
-      <c r="S26" s="64"/>
-      <c r="T26" s="64"/>
-      <c r="U26" s="64"/>
-      <c r="V26" s="64"/>
-      <c r="W26" s="64"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="63"/>
+      <c r="J26" s="63"/>
+      <c r="K26" s="63"/>
+      <c r="L26" s="63"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="63"/>
+      <c r="O26" s="63"/>
+      <c r="P26" s="63"/>
+      <c r="Q26" s="63"/>
+      <c r="R26" s="63"/>
+      <c r="S26" s="63"/>
+      <c r="T26" s="63"/>
+      <c r="U26" s="63"/>
+      <c r="V26" s="63"/>
+      <c r="W26" s="63"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="64" t="s">
+      <c r="A27" s="63" t="s">
         <v>678</v>
       </c>
-      <c r="B27" s="64" t="s">
+      <c r="B27" s="63" t="s">
         <v>683</v>
       </c>
-      <c r="C27" s="64" t="s">
+      <c r="C27" s="63" t="s">
         <v>684</v>
       </c>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="64"/>
-      <c r="I27" s="64"/>
-      <c r="J27" s="64"/>
-      <c r="K27" s="64"/>
-      <c r="L27" s="64"/>
-      <c r="M27" s="64"/>
-      <c r="N27" s="64"/>
-      <c r="O27" s="64"/>
-      <c r="P27" s="64"/>
-      <c r="Q27" s="64"/>
-      <c r="R27" s="64"/>
-      <c r="S27" s="64"/>
-      <c r="T27" s="64"/>
-      <c r="U27" s="64"/>
-      <c r="V27" s="64"/>
-      <c r="W27" s="64"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="63"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="63"/>
+      <c r="P27" s="63"/>
+      <c r="Q27" s="63"/>
+      <c r="R27" s="63"/>
+      <c r="S27" s="63"/>
+      <c r="T27" s="63"/>
+      <c r="U27" s="63"/>
+      <c r="V27" s="63"/>
+      <c r="W27" s="63"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="64" t="s">
+      <c r="A28" s="63" t="s">
         <v>678</v>
       </c>
-      <c r="B28" s="64" t="s">
+      <c r="B28" s="63" t="s">
         <v>685</v>
       </c>
-      <c r="C28" s="64" t="s">
+      <c r="C28" s="63" t="s">
         <v>686</v>
       </c>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="64"/>
-      <c r="I28" s="64"/>
-      <c r="J28" s="64"/>
-      <c r="K28" s="64"/>
-      <c r="L28" s="64"/>
-      <c r="M28" s="64"/>
-      <c r="N28" s="64"/>
-      <c r="O28" s="64"/>
-      <c r="P28" s="64"/>
-      <c r="Q28" s="64"/>
-      <c r="R28" s="64"/>
-      <c r="S28" s="64"/>
-      <c r="T28" s="64"/>
-      <c r="U28" s="64"/>
-      <c r="V28" s="64"/>
-      <c r="W28" s="64"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="63"/>
+      <c r="J28" s="63"/>
+      <c r="K28" s="63"/>
+      <c r="L28" s="63"/>
+      <c r="M28" s="63"/>
+      <c r="N28" s="63"/>
+      <c r="O28" s="63"/>
+      <c r="P28" s="63"/>
+      <c r="Q28" s="63"/>
+      <c r="R28" s="63"/>
+      <c r="S28" s="63"/>
+      <c r="T28" s="63"/>
+      <c r="U28" s="63"/>
+      <c r="V28" s="63"/>
+      <c r="W28" s="63"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="64" t="s">
+      <c r="A29" s="63" t="s">
         <v>678</v>
       </c>
-      <c r="B29" s="64" t="s">
+      <c r="B29" s="63" t="s">
         <v>598</v>
       </c>
-      <c r="C29" s="64" t="s">
+      <c r="C29" s="63" t="s">
         <v>599</v>
       </c>
-      <c r="D29" s="64"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="64"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="64"/>
-      <c r="I29" s="64"/>
-      <c r="J29" s="64"/>
-      <c r="K29" s="64"/>
-      <c r="L29" s="64"/>
-      <c r="M29" s="64"/>
-      <c r="N29" s="64"/>
-      <c r="O29" s="64"/>
-      <c r="P29" s="64"/>
-      <c r="Q29" s="64"/>
-      <c r="R29" s="64"/>
-      <c r="S29" s="64"/>
-      <c r="T29" s="64"/>
-      <c r="U29" s="64"/>
-      <c r="V29" s="64"/>
-      <c r="W29" s="64"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="63"/>
+      <c r="J29" s="63"/>
+      <c r="K29" s="63"/>
+      <c r="L29" s="63"/>
+      <c r="M29" s="63"/>
+      <c r="N29" s="63"/>
+      <c r="O29" s="63"/>
+      <c r="P29" s="63"/>
+      <c r="Q29" s="63"/>
+      <c r="R29" s="63"/>
+      <c r="S29" s="63"/>
+      <c r="T29" s="63"/>
+      <c r="U29" s="63"/>
+      <c r="V29" s="63"/>
+      <c r="W29" s="63"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="64"/>
-      <c r="B30" s="64"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="64"/>
-      <c r="J30" s="64"/>
-      <c r="K30" s="64"/>
-      <c r="L30" s="64"/>
-      <c r="M30" s="64"/>
-      <c r="N30" s="64"/>
-      <c r="O30" s="64"/>
-      <c r="P30" s="64"/>
-      <c r="Q30" s="64"/>
-      <c r="R30" s="64"/>
-      <c r="S30" s="64"/>
-      <c r="T30" s="64"/>
-      <c r="U30" s="64"/>
-      <c r="V30" s="64"/>
-      <c r="W30" s="64"/>
+      <c r="A30" s="63"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="63"/>
+      <c r="K30" s="63"/>
+      <c r="L30" s="63"/>
+      <c r="M30" s="63"/>
+      <c r="N30" s="63"/>
+      <c r="O30" s="63"/>
+      <c r="P30" s="63"/>
+      <c r="Q30" s="63"/>
+      <c r="R30" s="63"/>
+      <c r="S30" s="63"/>
+      <c r="T30" s="63"/>
+      <c r="U30" s="63"/>
+      <c r="V30" s="63"/>
+      <c r="W30" s="63"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="64" t="s">
+      <c r="A31" s="63" t="s">
         <v>687</v>
       </c>
-      <c r="B31" s="64" t="s">
+      <c r="B31" s="63" t="s">
         <v>688</v>
       </c>
-      <c r="C31" s="64" t="s">
+      <c r="C31" s="63" t="s">
         <v>586</v>
       </c>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="64"/>
-      <c r="I31" s="64"/>
-      <c r="J31" s="64"/>
-      <c r="K31" s="64"/>
-      <c r="L31" s="64"/>
-      <c r="M31" s="64"/>
-      <c r="N31" s="64"/>
-      <c r="O31" s="64"/>
-      <c r="P31" s="64"/>
-      <c r="Q31" s="64"/>
-      <c r="R31" s="64"/>
-      <c r="S31" s="64"/>
-      <c r="T31" s="64"/>
-      <c r="U31" s="64"/>
-      <c r="V31" s="64"/>
-      <c r="W31" s="64"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="63"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="63"/>
+      <c r="K31" s="63"/>
+      <c r="L31" s="63"/>
+      <c r="M31" s="63"/>
+      <c r="N31" s="63"/>
+      <c r="O31" s="63"/>
+      <c r="P31" s="63"/>
+      <c r="Q31" s="63"/>
+      <c r="R31" s="63"/>
+      <c r="S31" s="63"/>
+      <c r="T31" s="63"/>
+      <c r="U31" s="63"/>
+      <c r="V31" s="63"/>
+      <c r="W31" s="63"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="64" t="s">
+      <c r="A32" s="63" t="s">
         <v>687</v>
       </c>
-      <c r="B32" s="64" t="s">
+      <c r="B32" s="63" t="s">
         <v>689</v>
       </c>
-      <c r="C32" s="64" t="s">
+      <c r="C32" s="63" t="s">
         <v>587</v>
       </c>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="64"/>
-      <c r="J32" s="64"/>
-      <c r="K32" s="64"/>
-      <c r="L32" s="64"/>
-      <c r="M32" s="64"/>
-      <c r="N32" s="64"/>
-      <c r="O32" s="64"/>
-      <c r="P32" s="64"/>
-      <c r="Q32" s="64"/>
-      <c r="R32" s="64"/>
-      <c r="S32" s="64"/>
-      <c r="T32" s="64"/>
-      <c r="U32" s="64"/>
-      <c r="V32" s="64"/>
-      <c r="W32" s="64"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="63"/>
+      <c r="O32" s="63"/>
+      <c r="P32" s="63"/>
+      <c r="Q32" s="63"/>
+      <c r="R32" s="63"/>
+      <c r="S32" s="63"/>
+      <c r="T32" s="63"/>
+      <c r="U32" s="63"/>
+      <c r="V32" s="63"/>
+      <c r="W32" s="63"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="64"/>
-      <c r="B33" s="64"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="64"/>
-      <c r="I33" s="64"/>
-      <c r="J33" s="64"/>
-      <c r="K33" s="64"/>
-      <c r="L33" s="64"/>
-      <c r="M33" s="64"/>
-      <c r="N33" s="64"/>
-      <c r="O33" s="64"/>
-      <c r="P33" s="64"/>
-      <c r="Q33" s="64"/>
-      <c r="R33" s="64"/>
-      <c r="S33" s="64"/>
-      <c r="T33" s="64"/>
-      <c r="U33" s="64"/>
-      <c r="V33" s="64"/>
-      <c r="W33" s="64"/>
+      <c r="A33" s="63"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="63"/>
+      <c r="M33" s="63"/>
+      <c r="N33" s="63"/>
+      <c r="O33" s="63"/>
+      <c r="P33" s="63"/>
+      <c r="Q33" s="63"/>
+      <c r="R33" s="63"/>
+      <c r="S33" s="63"/>
+      <c r="T33" s="63"/>
+      <c r="U33" s="63"/>
+      <c r="V33" s="63"/>
+      <c r="W33" s="63"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" t="s">
@@ -21838,25 +21818,25 @@
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="65" t="s">
+      <c r="A48" s="54" t="s">
         <v>703</v>
       </c>
-      <c r="B48" s="65" t="s">
+      <c r="B48" s="54" t="s">
         <v>704</v>
       </c>
-      <c r="C48" s="65" t="s">
+      <c r="C48" s="54" t="s">
         <v>705</v>
       </c>
-      <c r="D48" s="65"/>
-      <c r="E48" s="65"/>
-      <c r="F48" s="65"/>
-      <c r="G48" s="65"/>
-      <c r="H48" s="65"/>
-      <c r="I48" s="65"/>
-      <c r="J48" s="65"/>
-      <c r="K48" s="65"/>
-      <c r="L48" s="65"/>
-      <c r="M48" s="65"/>
+      <c r="D48" s="54"/>
+      <c r="E48" s="54"/>
+      <c r="F48" s="54"/>
+      <c r="G48" s="54"/>
+      <c r="H48" s="54"/>
+      <c r="I48" s="54"/>
+      <c r="J48" s="54"/>
+      <c r="K48" s="54"/>
+      <c r="L48" s="54"/>
+      <c r="M48" s="54"/>
       <c r="N48" s="55"/>
       <c r="O48" s="55"/>
       <c r="P48" s="55"/>
@@ -21869,25 +21849,25 @@
       <c r="W48" s="55"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="65" t="s">
+      <c r="A49" s="54" t="s">
         <v>703</v>
       </c>
-      <c r="B49" s="65" t="s">
+      <c r="B49" s="54" t="s">
         <v>706</v>
       </c>
-      <c r="C49" s="65" t="s">
+      <c r="C49" s="54" t="s">
         <v>707</v>
       </c>
-      <c r="D49" s="65"/>
-      <c r="E49" s="65"/>
-      <c r="F49" s="65"/>
-      <c r="G49" s="65"/>
-      <c r="H49" s="65"/>
-      <c r="I49" s="65"/>
-      <c r="J49" s="65"/>
-      <c r="K49" s="65"/>
-      <c r="L49" s="65"/>
-      <c r="M49" s="65"/>
+      <c r="D49" s="54"/>
+      <c r="E49" s="54"/>
+      <c r="F49" s="54"/>
+      <c r="G49" s="54"/>
+      <c r="H49" s="54"/>
+      <c r="I49" s="54"/>
+      <c r="J49" s="54"/>
+      <c r="K49" s="54"/>
+      <c r="L49" s="54"/>
+      <c r="M49" s="54"/>
       <c r="N49" s="55"/>
       <c r="O49" s="55"/>
       <c r="P49" s="55"/>
@@ -21966,46 +21946,46 @@
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="65" t="s">
+      <c r="A58" s="54" t="s">
         <v>719</v>
       </c>
-      <c r="B58" s="65" t="s">
+      <c r="B58" s="54" t="s">
         <v>720</v>
       </c>
-      <c r="C58" s="65" t="s">
+      <c r="C58" s="54" t="s">
         <v>721</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="65" t="s">
+      <c r="A59" s="54" t="s">
         <v>719</v>
       </c>
-      <c r="B59" s="65" t="s">
+      <c r="B59" s="54" t="s">
         <v>722</v>
       </c>
-      <c r="C59" s="65" t="s">
+      <c r="C59" s="54" t="s">
         <v>723</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="65" t="s">
+      <c r="A60" s="54" t="s">
         <v>719</v>
       </c>
-      <c r="B60" s="65" t="s">
+      <c r="B60" s="54" t="s">
         <v>724</v>
       </c>
-      <c r="C60" s="65" t="s">
+      <c r="C60" s="54" t="s">
         <v>725</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="65" t="s">
+      <c r="A61" s="54" t="s">
         <v>719</v>
       </c>
-      <c r="B61" s="65" t="s">
+      <c r="B61" s="54" t="s">
         <v>598</v>
       </c>
-      <c r="C61" s="65" t="s">
+      <c r="C61" s="54" t="s">
         <v>599</v>
       </c>
     </row>
@@ -22016,7 +21996,7 @@
       <c r="B63" s="55" t="s">
         <v>727</v>
       </c>
-      <c r="C63" s="65" t="s">
+      <c r="C63" s="54" t="s">
         <v>728</v>
       </c>
     </row>
@@ -22027,7 +22007,7 @@
       <c r="B64" s="55" t="s">
         <v>729</v>
       </c>
-      <c r="C64" s="65" t="s">
+      <c r="C64" s="54" t="s">
         <v>730</v>
       </c>
     </row>
@@ -22038,7 +22018,7 @@
       <c r="B65" s="55" t="s">
         <v>731</v>
       </c>
-      <c r="C65" s="65" t="s">
+      <c r="C65" s="54" t="s">
         <v>732</v>
       </c>
     </row>
@@ -22049,7 +22029,7 @@
       <c r="B66" s="55" t="s">
         <v>733</v>
       </c>
-      <c r="C66" s="65" t="s">
+      <c r="C66" s="54" t="s">
         <v>734</v>
       </c>
     </row>
@@ -22060,7 +22040,7 @@
       <c r="B67" s="55" t="s">
         <v>627</v>
       </c>
-      <c r="C67" s="65" t="s">
+      <c r="C67" s="54" t="s">
         <v>633</v>
       </c>
     </row>
@@ -22093,7 +22073,7 @@
       <c r="B72" t="s">
         <v>741</v>
       </c>
-      <c r="C72" s="66" t="s">
+      <c r="C72" s="64" t="s">
         <v>701</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add tests for delivery changes
</commit_message>
<xml_diff>
--- a/config/default/forms/app/delivery.xlsx
+++ b/config/default/forms/app/delivery.xlsx
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="743">
   <si>
     <t>type</t>
   </si>
@@ -1448,19 +1448,13 @@
   <si>
     <t xml:space="preserve">selected(../../condition/woman_outcome, 'alive_well') or
 selected(../../condition/woman_outcome, 'alive_unwell') or
-../../delivery_outcome/babies_alive_num &gt; 0 or
-../../pnc_visits/pnc_visits_additional != ''</t>
+../../delivery_outcome/babies_alive_num &gt; 0</t>
   </si>
   <si>
     <t>r_pnc_visits_completed</t>
   </si>
   <si>
     <t xml:space="preserve">PNC visits completed so far:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../condition/woman_outcome, 'alive_well') or
-selected(../../condition/woman_outcome, 'alive_unwell') or
-../../delivery_outcome/babies_alive_num &gt; 0</t>
   </si>
   <si>
     <t>r_pnc_visit_24hrs</t>
@@ -2840,7 +2834,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName=" " id="{16F6E003-524F-F17E-22FB-BCB874643EBA}"/>
+  <person displayName=" " id="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}"/>
 </personList>
 </file>
 
@@ -3256,7 +3250,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="U266" personId="{16F6E003-524F-F17E-22FB-BCB874643EBA}" id="{0024000F-00D4-40FA-8C20-0081001200D2}" done="0">
+  <threadedComment ref="U266" personId="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}" id="{0024000F-00D4-40FA-8C20-0081001200D2}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org is there a reason we are using .. instead of ${} for these? It would be more consistent if we could use $
 _Assigned to you_
 -Michael Kohn
@@ -3278,7 +3272,7 @@
 -Michael Kohn
 </text>
   </threadedComment>
-  <threadedComment ref="U294" personId="{16F6E003-524F-F17E-22FB-BCB874643EBA}" id="{00800045-00BB-493D-B802-00C800B500C8}" done="0">
+  <threadedComment ref="U294" personId="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}" id="{00800045-00BB-493D-B802-00C800B500C8}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org in some of the other forms i see this as ../../patient_id instead, not sure if it matters but feel like we should be consistent. I can update it based on your input. Also not sure why some of the ones below have ../../inputs and this one is ../inputs.
 _Assigned to you_
 -Michael Kohn
@@ -3291,7 +3285,7 @@
 -Michael Kohn
 </text>
   </threadedComment>
-  <threadedComment ref="U298" personId="{16F6E003-524F-F17E-22FB-BCB874643EBA}" id="{00660081-00F5-41A0-8991-00C6004C00A7}" done="0">
+  <threadedComment ref="U298" personId="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}" id="{00660081-00F5-41A0-8991-00C6004C00A7}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org in other forms there is a calculate field called pregnancy_uuid_ctx. To be consistent, it feels like we should either add that calculate field to this form and use that for this calculation, or update the other forms to use the "instance('contact-summary'......)" notation. I'd actually prefer to update the other forms to use the "instance('contact-summary'....)" notation because in general i was trying to avoid referencing those top level calculate fields in the data section (there are exceptions). Do you have a preference?
 _Assigned to you_
 -Michael Kohn
@@ -3301,7 +3295,7 @@
 -Marc Abbyad
 </text>
   </threadedComment>
-  <threadedComment ref="AI1" personId="{16F6E003-524F-F17E-22FB-BCB874643EBA}" id="{00A000D4-0058-42D9-AAD4-004A00F70029}" done="0">
+  <threadedComment ref="AI1" personId="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}" id="{00A000D4-0058-42D9-AAD4-004A00F70029}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org just FYI i moved these "instance" columns to be after the cht::notes column so that all forms have the same columns in the same order up to AH. Personally I'd probably prefer that all forms have the same exact columns in the same order, even if not all columns are needed for that form.
 _Assigned to you_
 -Michael Kohn
@@ -14127,7 +14121,7 @@
       <c r="I236" s="31"/>
       <c r="J236" s="31"/>
       <c r="K236" s="30" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="L236" s="31"/>
       <c r="M236" s="31"/>
@@ -14160,10 +14154,10 @@
         <v>106</v>
       </c>
       <c r="B237" s="29" t="s">
+        <v>429</v>
+      </c>
+      <c r="C237" s="30" t="s">
         <v>430</v>
-      </c>
-      <c r="C237" s="30" t="s">
-        <v>431</v>
       </c>
       <c r="D237" s="31"/>
       <c r="E237" s="31"/>
@@ -14173,7 +14167,7 @@
       <c r="I237" s="31"/>
       <c r="J237" s="31"/>
       <c r="K237" s="31" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L237" s="31" t="s">
         <v>384</v>
@@ -14208,10 +14202,10 @@
         <v>106</v>
       </c>
       <c r="B238" s="29" t="s">
+        <v>432</v>
+      </c>
+      <c r="C238" s="30" t="s">
         <v>433</v>
-      </c>
-      <c r="C238" s="30" t="s">
-        <v>434</v>
       </c>
       <c r="D238" s="31"/>
       <c r="E238" s="31"/>
@@ -14221,7 +14215,7 @@
       <c r="I238" s="31"/>
       <c r="J238" s="31"/>
       <c r="K238" s="31" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="L238" s="31" t="s">
         <v>384</v>
@@ -14256,10 +14250,10 @@
         <v>106</v>
       </c>
       <c r="B239" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="C239" s="30" t="s">
         <v>436</v>
-      </c>
-      <c r="C239" s="30" t="s">
-        <v>437</v>
       </c>
       <c r="D239" s="31"/>
       <c r="E239" s="31"/>
@@ -14269,7 +14263,7 @@
       <c r="I239" s="31"/>
       <c r="J239" s="31"/>
       <c r="K239" s="31" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="L239" s="31" t="s">
         <v>384</v>
@@ -14304,10 +14298,10 @@
         <v>106</v>
       </c>
       <c r="B240" s="29" t="s">
+        <v>438</v>
+      </c>
+      <c r="C240" s="30" t="s">
         <v>439</v>
-      </c>
-      <c r="C240" s="30" t="s">
-        <v>440</v>
       </c>
       <c r="D240" s="31"/>
       <c r="E240" s="31"/>
@@ -14317,7 +14311,7 @@
       <c r="I240" s="31"/>
       <c r="J240" s="31"/>
       <c r="K240" s="31" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L240" s="31" t="s">
         <v>384</v>
@@ -14352,10 +14346,10 @@
         <v>106</v>
       </c>
       <c r="B241" s="29" t="s">
+        <v>441</v>
+      </c>
+      <c r="C241" s="30" t="s">
         <v>442</v>
-      </c>
-      <c r="C241" s="30" t="s">
-        <v>443</v>
       </c>
       <c r="D241" s="31"/>
       <c r="E241" s="31"/>
@@ -14365,7 +14359,7 @@
       <c r="I241" s="31"/>
       <c r="J241" s="31"/>
       <c r="K241" s="30" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="L241" s="31" t="s">
         <v>384</v>
@@ -14400,10 +14394,10 @@
         <v>106</v>
       </c>
       <c r="B242" s="29" t="s">
+        <v>444</v>
+      </c>
+      <c r="C242" s="30" t="s">
         <v>445</v>
-      </c>
-      <c r="C242" s="30" t="s">
-        <v>446</v>
       </c>
       <c r="D242" s="31"/>
       <c r="E242" s="31"/>
@@ -14413,7 +14407,7 @@
       <c r="I242" s="31"/>
       <c r="J242" s="31"/>
       <c r="K242" s="31" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="L242" s="31"/>
       <c r="M242" s="31"/>
@@ -14446,10 +14440,10 @@
         <v>106</v>
       </c>
       <c r="B243" s="29" t="s">
+        <v>447</v>
+      </c>
+      <c r="C243" s="30" t="s">
         <v>448</v>
-      </c>
-      <c r="C243" s="30" t="s">
-        <v>449</v>
       </c>
       <c r="D243" s="31"/>
       <c r="E243" s="31"/>
@@ -14459,10 +14453,10 @@
       <c r="I243" s="31"/>
       <c r="J243" s="31"/>
       <c r="K243" s="30" t="s">
+        <v>449</v>
+      </c>
+      <c r="L243" s="30" t="s">
         <v>450</v>
-      </c>
-      <c r="L243" s="30" t="s">
-        <v>451</v>
       </c>
       <c r="M243" s="31"/>
       <c r="N243" s="31"/>
@@ -14494,10 +14488,10 @@
         <v>106</v>
       </c>
       <c r="B244" s="29" t="s">
+        <v>451</v>
+      </c>
+      <c r="C244" s="30" t="s">
         <v>452</v>
-      </c>
-      <c r="C244" s="30" t="s">
-        <v>453</v>
       </c>
       <c r="D244" s="31"/>
       <c r="E244" s="31"/>
@@ -14507,7 +14501,7 @@
       <c r="I244" s="31"/>
       <c r="J244" s="31"/>
       <c r="K244" s="30" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="L244" s="30"/>
       <c r="M244" s="31"/>
@@ -14540,7 +14534,7 @@
         <v>106</v>
       </c>
       <c r="B245" s="29" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C245" s="30" t="s">
         <v>413</v>
@@ -14588,10 +14582,10 @@
         <v>106</v>
       </c>
       <c r="B246" s="29" t="s">
+        <v>455</v>
+      </c>
+      <c r="C246" s="30" t="s">
         <v>456</v>
-      </c>
-      <c r="C246" s="30" t="s">
-        <v>457</v>
       </c>
       <c r="D246" s="31"/>
       <c r="E246" s="31"/>
@@ -14636,10 +14630,10 @@
         <v>106</v>
       </c>
       <c r="B247" s="29" t="s">
+        <v>457</v>
+      </c>
+      <c r="C247" s="30" t="s">
         <v>458</v>
-      </c>
-      <c r="C247" s="30" t="s">
-        <v>459</v>
       </c>
       <c r="D247" s="31"/>
       <c r="E247" s="31"/>
@@ -14649,7 +14643,7 @@
       <c r="I247" s="31"/>
       <c r="J247" s="31"/>
       <c r="K247" s="30" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="L247" s="31"/>
       <c r="M247" s="31"/>
@@ -14682,10 +14676,10 @@
         <v>106</v>
       </c>
       <c r="B248" s="29" t="s">
+        <v>459</v>
+      </c>
+      <c r="C248" s="30" t="s">
         <v>460</v>
-      </c>
-      <c r="C248" s="30" t="s">
-        <v>461</v>
       </c>
       <c r="D248" s="31"/>
       <c r="E248" s="31"/>
@@ -14695,7 +14689,7 @@
       <c r="I248" s="31"/>
       <c r="J248" s="31"/>
       <c r="K248" s="30" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="L248" s="31"/>
       <c r="M248" s="31"/>
@@ -14728,10 +14722,10 @@
         <v>106</v>
       </c>
       <c r="B249" s="29" t="s">
+        <v>461</v>
+      </c>
+      <c r="C249" s="30" t="s">
         <v>462</v>
-      </c>
-      <c r="C249" s="30" t="s">
-        <v>463</v>
       </c>
       <c r="D249" s="31"/>
       <c r="E249" s="31"/>
@@ -14744,7 +14738,7 @@
         <v>414</v>
       </c>
       <c r="L249" s="30" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="M249" s="31"/>
       <c r="N249" s="31"/>
@@ -14776,10 +14770,10 @@
         <v>106</v>
       </c>
       <c r="B250" s="29" t="s">
+        <v>464</v>
+      </c>
+      <c r="C250" s="30" t="s">
         <v>465</v>
-      </c>
-      <c r="C250" s="30" t="s">
-        <v>466</v>
       </c>
       <c r="D250" s="31"/>
       <c r="E250" s="31"/>
@@ -14822,10 +14816,10 @@
         <v>106</v>
       </c>
       <c r="B251" s="29" t="s">
+        <v>466</v>
+      </c>
+      <c r="C251" s="30" t="s">
         <v>467</v>
-      </c>
-      <c r="C251" s="30" t="s">
-        <v>468</v>
       </c>
       <c r="D251" s="31"/>
       <c r="E251" s="31"/>
@@ -14868,10 +14862,10 @@
         <v>106</v>
       </c>
       <c r="B252" s="29" t="s">
+        <v>468</v>
+      </c>
+      <c r="C252" s="30" t="s">
         <v>469</v>
-      </c>
-      <c r="C252" s="30" t="s">
-        <v>470</v>
       </c>
       <c r="D252" s="31"/>
       <c r="E252" s="31"/>
@@ -14881,7 +14875,7 @@
       <c r="I252" s="31"/>
       <c r="J252" s="31"/>
       <c r="K252" s="30" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="L252" s="30"/>
       <c r="M252" s="31"/>
@@ -14914,7 +14908,7 @@
         <v>36</v>
       </c>
       <c r="B253" s="29" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C253" s="30" t="s">
         <v>38</v>
@@ -14959,10 +14953,10 @@
     </row>
     <row r="254" ht="15.75" customHeight="1">
       <c r="A254" s="29" t="s">
+        <v>472</v>
+      </c>
+      <c r="B254" s="29" t="s">
         <v>473</v>
-      </c>
-      <c r="B254" s="29" t="s">
-        <v>474</v>
       </c>
       <c r="C254" s="30" t="s">
         <v>38</v>
@@ -14985,7 +14979,7 @@
       <c r="S254" s="30"/>
       <c r="T254" s="30"/>
       <c r="U254" s="30" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="V254" s="31"/>
       <c r="W254" s="30"/>
@@ -15008,7 +15002,7 @@
         <v>75</v>
       </c>
       <c r="B255" s="29" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C255" s="30" t="s">
         <v>38</v>
@@ -15031,7 +15025,7 @@
       <c r="S255" s="30"/>
       <c r="T255" s="30"/>
       <c r="U255" s="30" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="V255" s="31"/>
       <c r="W255" s="30"/>
@@ -15051,10 +15045,10 @@
     </row>
     <row r="256" ht="15.75" customHeight="1">
       <c r="A256" s="29" t="s">
+        <v>477</v>
+      </c>
+      <c r="B256" s="29" t="s">
         <v>478</v>
-      </c>
-      <c r="B256" s="29" t="s">
-        <v>479</v>
       </c>
       <c r="C256" s="30" t="s">
         <v>38</v>
@@ -15077,7 +15071,7 @@
       <c r="S256" s="30"/>
       <c r="T256" s="30"/>
       <c r="U256" s="30" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="V256" s="31"/>
       <c r="W256" s="30"/>
@@ -15100,7 +15094,7 @@
         <v>75</v>
       </c>
       <c r="B257" s="29" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C257" s="30" t="s">
         <v>38</v>
@@ -15123,7 +15117,7 @@
       <c r="S257" s="30"/>
       <c r="T257" s="30"/>
       <c r="U257" s="30" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="V257" s="31"/>
       <c r="W257" s="30"/>
@@ -15146,7 +15140,7 @@
         <v>130</v>
       </c>
       <c r="B258" s="29" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C258" s="30" t="s">
         <v>38</v>
@@ -15169,7 +15163,7 @@
       <c r="S258" s="31"/>
       <c r="T258" s="31"/>
       <c r="U258" s="30" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="V258" s="31"/>
       <c r="W258" s="31"/>
@@ -15192,7 +15186,7 @@
         <v>75</v>
       </c>
       <c r="B259" s="29" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C259" s="30" t="s">
         <v>38</v>
@@ -15215,7 +15209,7 @@
       <c r="S259" s="31"/>
       <c r="T259" s="31"/>
       <c r="U259" s="30" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="V259" s="31"/>
       <c r="W259" s="31"/>
@@ -15238,7 +15232,7 @@
         <v>130</v>
       </c>
       <c r="B260" s="29" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C260" s="30" t="s">
         <v>38</v>
@@ -15261,7 +15255,7 @@
       <c r="S260" s="31"/>
       <c r="T260" s="31"/>
       <c r="U260" s="30" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="V260" s="31"/>
       <c r="W260" s="31"/>
@@ -15284,7 +15278,7 @@
         <v>75</v>
       </c>
       <c r="B261" s="29" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C261" s="30" t="s">
         <v>38</v>
@@ -15307,7 +15301,7 @@
       <c r="S261" s="31"/>
       <c r="T261" s="31"/>
       <c r="U261" s="30" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="V261" s="31"/>
       <c r="W261" s="31"/>
@@ -15448,7 +15442,7 @@
         <v>36</v>
       </c>
       <c r="B265" s="33" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C265" s="34" t="s">
         <v>38</v>
@@ -15496,7 +15490,7 @@
         <v>75</v>
       </c>
       <c r="B266" s="33" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C266" s="40" t="s">
         <v>38</v>
@@ -15519,7 +15513,7 @@
       <c r="S266" s="34"/>
       <c r="T266" s="34"/>
       <c r="U266" s="37" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="V266" s="34"/>
       <c r="W266" s="34"/>
@@ -15534,7 +15528,7 @@
       <c r="AF266" s="37"/>
       <c r="AG266" s="37"/>
       <c r="AH266" s="37" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="AI266" s="37"/>
       <c r="AJ266" s="37"/>
@@ -15544,7 +15538,7 @@
         <v>75</v>
       </c>
       <c r="B267" s="33" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C267" s="40" t="s">
         <v>38</v>
@@ -15567,7 +15561,7 @@
       <c r="S267" s="34"/>
       <c r="T267" s="34"/>
       <c r="U267" s="37" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="V267" s="34"/>
       <c r="W267" s="34"/>
@@ -15582,7 +15576,7 @@
       <c r="AF267" s="37"/>
       <c r="AG267" s="37"/>
       <c r="AH267" s="37" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="AI267" s="37"/>
       <c r="AJ267" s="37"/>
@@ -15592,7 +15586,7 @@
         <v>75</v>
       </c>
       <c r="B268" s="33" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C268" s="40" t="s">
         <v>38</v>
@@ -15615,7 +15609,7 @@
       <c r="S268" s="34"/>
       <c r="T268" s="34"/>
       <c r="U268" s="37" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="V268" s="34"/>
       <c r="W268" s="34"/>
@@ -15630,7 +15624,7 @@
       <c r="AF268" s="37"/>
       <c r="AG268" s="37"/>
       <c r="AH268" s="37" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AI268" s="37"/>
       <c r="AJ268" s="37"/>
@@ -15640,7 +15634,7 @@
         <v>75</v>
       </c>
       <c r="B269" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C269" s="40" t="s">
         <v>38</v>
@@ -15663,7 +15657,7 @@
       <c r="S269" s="34"/>
       <c r="T269" s="34"/>
       <c r="U269" s="37" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="V269" s="34"/>
       <c r="W269" s="34"/>
@@ -15678,7 +15672,7 @@
       <c r="AF269" s="37"/>
       <c r="AG269" s="37"/>
       <c r="AH269" s="37" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="AI269" s="37"/>
       <c r="AJ269" s="37"/>
@@ -15688,7 +15682,7 @@
         <v>75</v>
       </c>
       <c r="B270" s="33" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C270" s="40" t="s">
         <v>38</v>
@@ -15711,7 +15705,7 @@
       <c r="S270" s="34"/>
       <c r="T270" s="34"/>
       <c r="U270" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="V270" s="34"/>
       <c r="W270" s="34"/>
@@ -15726,7 +15720,7 @@
       <c r="AF270" s="37"/>
       <c r="AG270" s="37"/>
       <c r="AH270" s="37" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="AI270" s="37"/>
       <c r="AJ270" s="37"/>
@@ -15736,7 +15730,7 @@
         <v>75</v>
       </c>
       <c r="B271" s="33" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C271" s="40" t="s">
         <v>38</v>
@@ -15759,7 +15753,7 @@
       <c r="S271" s="34"/>
       <c r="T271" s="34"/>
       <c r="U271" s="37" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="V271" s="34"/>
       <c r="W271" s="34"/>
@@ -15774,7 +15768,7 @@
       <c r="AF271" s="37"/>
       <c r="AG271" s="37"/>
       <c r="AH271" s="37" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AI271" s="37"/>
       <c r="AJ271" s="37"/>
@@ -15784,7 +15778,7 @@
         <v>75</v>
       </c>
       <c r="B272" s="33" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C272" s="40" t="s">
         <v>38</v>
@@ -15807,7 +15801,7 @@
       <c r="S272" s="34"/>
       <c r="T272" s="34"/>
       <c r="U272" s="37" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="V272" s="34"/>
       <c r="W272" s="34"/>
@@ -15822,7 +15816,7 @@
       <c r="AF272" s="37"/>
       <c r="AG272" s="37"/>
       <c r="AH272" s="37" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="AI272" s="37"/>
       <c r="AJ272" s="37"/>
@@ -15832,7 +15826,7 @@
         <v>75</v>
       </c>
       <c r="B273" s="33" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C273" s="40" t="s">
         <v>38</v>
@@ -15855,7 +15849,7 @@
       <c r="S273" s="34"/>
       <c r="T273" s="34"/>
       <c r="U273" s="37" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="V273" s="34"/>
       <c r="W273" s="34"/>
@@ -15870,7 +15864,7 @@
       <c r="AF273" s="37"/>
       <c r="AG273" s="37"/>
       <c r="AH273" s="37" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AI273" s="37"/>
       <c r="AJ273" s="37"/>
@@ -15880,7 +15874,7 @@
         <v>75</v>
       </c>
       <c r="B274" s="33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C274" s="40" t="s">
         <v>38</v>
@@ -15903,7 +15897,7 @@
       <c r="S274" s="34"/>
       <c r="T274" s="34"/>
       <c r="U274" s="37" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="V274" s="34"/>
       <c r="W274" s="34"/>
@@ -15918,7 +15912,7 @@
       <c r="AF274" s="37"/>
       <c r="AG274" s="37"/>
       <c r="AH274" s="37" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="AI274" s="37"/>
       <c r="AJ274" s="37"/>
@@ -15928,7 +15922,7 @@
         <v>75</v>
       </c>
       <c r="B275" s="33" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C275" s="40" t="s">
         <v>38</v>
@@ -15951,7 +15945,7 @@
       <c r="S275" s="34"/>
       <c r="T275" s="34"/>
       <c r="U275" s="37" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="V275" s="34"/>
       <c r="W275" s="34"/>
@@ -15966,7 +15960,7 @@
       <c r="AF275" s="37"/>
       <c r="AG275" s="37"/>
       <c r="AH275" s="37" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="AI275" s="37"/>
       <c r="AJ275" s="37"/>
@@ -15976,7 +15970,7 @@
         <v>75</v>
       </c>
       <c r="B276" s="33" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C276" s="40" t="s">
         <v>38</v>
@@ -15999,7 +15993,7 @@
       <c r="S276" s="34"/>
       <c r="T276" s="34"/>
       <c r="U276" s="37" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="V276" s="34"/>
       <c r="W276" s="34"/>
@@ -16014,7 +16008,7 @@
       <c r="AF276" s="37"/>
       <c r="AG276" s="37"/>
       <c r="AH276" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="AI276" s="37"/>
       <c r="AJ276" s="37"/>
@@ -16024,7 +16018,7 @@
         <v>75</v>
       </c>
       <c r="B277" s="33" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C277" s="40" t="s">
         <v>38</v>
@@ -16047,7 +16041,7 @@
       <c r="S277" s="34"/>
       <c r="T277" s="34"/>
       <c r="U277" s="37" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="V277" s="34"/>
       <c r="W277" s="34"/>
@@ -16062,7 +16056,7 @@
       <c r="AF277" s="37"/>
       <c r="AG277" s="37"/>
       <c r="AH277" s="37" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="AI277" s="37"/>
       <c r="AJ277" s="37"/>
@@ -16072,7 +16066,7 @@
         <v>75</v>
       </c>
       <c r="B278" s="33" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C278" s="40" t="s">
         <v>38</v>
@@ -16110,7 +16104,7 @@
       <c r="AF278" s="37"/>
       <c r="AG278" s="37"/>
       <c r="AH278" s="37" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="AI278" s="37"/>
       <c r="AJ278" s="37"/>
@@ -16120,7 +16114,7 @@
         <v>75</v>
       </c>
       <c r="B279" s="33" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C279" s="40" t="s">
         <v>38</v>
@@ -16158,7 +16152,7 @@
       <c r="AF279" s="37"/>
       <c r="AG279" s="37"/>
       <c r="AH279" s="37" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AI279" s="37"/>
       <c r="AJ279" s="37"/>
@@ -16168,7 +16162,7 @@
         <v>75</v>
       </c>
       <c r="B280" s="33" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C280" s="40" t="s">
         <v>38</v>
@@ -16191,7 +16185,7 @@
       <c r="S280" s="34"/>
       <c r="T280" s="34"/>
       <c r="U280" s="37" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="V280" s="34"/>
       <c r="W280" s="34"/>
@@ -16206,7 +16200,7 @@
       <c r="AF280" s="37"/>
       <c r="AG280" s="37"/>
       <c r="AH280" s="37" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AI280" s="37"/>
       <c r="AJ280" s="37"/>
@@ -16216,7 +16210,7 @@
         <v>75</v>
       </c>
       <c r="B281" s="33" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C281" s="40" t="s">
         <v>38</v>
@@ -16239,7 +16233,7 @@
       <c r="S281" s="34"/>
       <c r="T281" s="34"/>
       <c r="U281" s="37" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="V281" s="34"/>
       <c r="W281" s="34"/>
@@ -16254,7 +16248,7 @@
       <c r="AF281" s="37"/>
       <c r="AG281" s="37"/>
       <c r="AH281" s="37" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="AI281" s="37"/>
       <c r="AJ281" s="37"/>
@@ -16264,7 +16258,7 @@
         <v>75</v>
       </c>
       <c r="B282" s="33" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C282" s="40" t="s">
         <v>38</v>
@@ -16287,7 +16281,7 @@
       <c r="S282" s="34"/>
       <c r="T282" s="34"/>
       <c r="U282" s="37" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="V282" s="34"/>
       <c r="W282" s="34"/>
@@ -16302,7 +16296,7 @@
       <c r="AF282" s="37"/>
       <c r="AG282" s="37"/>
       <c r="AH282" s="37" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AI282" s="37"/>
       <c r="AJ282" s="37"/>
@@ -16312,7 +16306,7 @@
         <v>75</v>
       </c>
       <c r="B283" s="33" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C283" s="40" t="s">
         <v>38</v>
@@ -16335,7 +16329,7 @@
       <c r="S283" s="34"/>
       <c r="T283" s="34"/>
       <c r="U283" s="37" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="V283" s="34"/>
       <c r="W283" s="34"/>
@@ -16350,7 +16344,7 @@
       <c r="AF283" s="37"/>
       <c r="AG283" s="37"/>
       <c r="AH283" s="37" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="AI283" s="37"/>
       <c r="AJ283" s="37"/>
@@ -16360,7 +16354,7 @@
         <v>75</v>
       </c>
       <c r="B284" s="33" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C284" s="40" t="s">
         <v>38</v>
@@ -16383,7 +16377,7 @@
       <c r="S284" s="34"/>
       <c r="T284" s="34"/>
       <c r="U284" s="37" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="V284" s="34"/>
       <c r="W284" s="34"/>
@@ -16398,7 +16392,7 @@
       <c r="AF284" s="37"/>
       <c r="AG284" s="37"/>
       <c r="AH284" s="37" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="AI284" s="37"/>
       <c r="AJ284" s="37"/>
@@ -16408,7 +16402,7 @@
         <v>75</v>
       </c>
       <c r="B285" s="33" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C285" s="40" t="s">
         <v>38</v>
@@ -16431,7 +16425,7 @@
       <c r="S285" s="34"/>
       <c r="T285" s="34"/>
       <c r="U285" s="37" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="V285" s="34"/>
       <c r="W285" s="34"/>
@@ -16446,7 +16440,7 @@
       <c r="AF285" s="37"/>
       <c r="AG285" s="37"/>
       <c r="AH285" s="37" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AI285" s="37"/>
       <c r="AJ285" s="37"/>
@@ -16456,7 +16450,7 @@
         <v>75</v>
       </c>
       <c r="B286" s="33" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C286" s="40" t="s">
         <v>38</v>
@@ -16479,7 +16473,7 @@
       <c r="S286" s="34"/>
       <c r="T286" s="34"/>
       <c r="U286" s="37" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="V286" s="34"/>
       <c r="W286" s="34"/>
@@ -16494,7 +16488,7 @@
       <c r="AF286" s="37"/>
       <c r="AG286" s="37"/>
       <c r="AH286" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AI286" s="37"/>
       <c r="AJ286" s="37"/>
@@ -16504,7 +16498,7 @@
         <v>75</v>
       </c>
       <c r="B287" s="33" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C287" s="40" t="s">
         <v>38</v>
@@ -16527,7 +16521,7 @@
       <c r="S287" s="34"/>
       <c r="T287" s="34"/>
       <c r="U287" s="37" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="V287" s="34"/>
       <c r="W287" s="34"/>
@@ -16542,7 +16536,7 @@
       <c r="AF287" s="37"/>
       <c r="AG287" s="37"/>
       <c r="AH287" s="37" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="AI287" s="37"/>
       <c r="AJ287" s="37"/>
@@ -16552,7 +16546,7 @@
         <v>75</v>
       </c>
       <c r="B288" s="33" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C288" s="40" t="s">
         <v>38</v>
@@ -16575,7 +16569,7 @@
       <c r="S288" s="34"/>
       <c r="T288" s="34"/>
       <c r="U288" s="37" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="V288" s="34"/>
       <c r="W288" s="34"/>
@@ -16590,7 +16584,7 @@
       <c r="AF288" s="37"/>
       <c r="AG288" s="37"/>
       <c r="AH288" s="37" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AI288" s="37"/>
       <c r="AJ288" s="37"/>
@@ -16600,7 +16594,7 @@
         <v>75</v>
       </c>
       <c r="B289" s="33" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C289" s="40" t="s">
         <v>38</v>
@@ -16623,7 +16617,7 @@
       <c r="S289" s="34"/>
       <c r="T289" s="34"/>
       <c r="U289" s="37" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="V289" s="34"/>
       <c r="W289" s="34"/>
@@ -16638,7 +16632,7 @@
       <c r="AF289" s="37"/>
       <c r="AG289" s="37"/>
       <c r="AH289" s="37" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="AI289" s="37"/>
       <c r="AJ289" s="37"/>
@@ -16648,7 +16642,7 @@
         <v>75</v>
       </c>
       <c r="B290" s="33" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C290" s="40" t="s">
         <v>38</v>
@@ -16671,7 +16665,7 @@
       <c r="S290" s="34"/>
       <c r="T290" s="34"/>
       <c r="U290" s="37" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="V290" s="34"/>
       <c r="W290" s="34"/>
@@ -16686,7 +16680,7 @@
       <c r="AF290" s="37"/>
       <c r="AG290" s="37"/>
       <c r="AH290" s="37" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="AI290" s="37"/>
       <c r="AJ290" s="37"/>
@@ -16696,7 +16690,7 @@
         <v>75</v>
       </c>
       <c r="B291" s="33" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C291" s="40" t="s">
         <v>38</v>
@@ -16719,7 +16713,7 @@
       <c r="S291" s="34"/>
       <c r="T291" s="34"/>
       <c r="U291" s="37" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="V291" s="34"/>
       <c r="W291" s="34"/>
@@ -16734,7 +16728,7 @@
       <c r="AF291" s="37"/>
       <c r="AG291" s="37"/>
       <c r="AH291" s="37" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="AI291" s="37"/>
       <c r="AJ291" s="37"/>
@@ -16744,7 +16738,7 @@
         <v>36</v>
       </c>
       <c r="B292" s="33" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C292" s="40" t="s">
         <v>38</v>
@@ -16788,7 +16782,7 @@
         <v>75</v>
       </c>
       <c r="B293" s="33" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C293" s="40" t="s">
         <v>38</v>
@@ -16811,7 +16805,7 @@
       <c r="S293" s="34"/>
       <c r="T293" s="34"/>
       <c r="U293" s="40" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="V293" s="34"/>
       <c r="W293" s="34"/>
@@ -16826,7 +16820,7 @@
       <c r="AF293" s="37"/>
       <c r="AG293" s="37"/>
       <c r="AH293" s="40" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="AI293" s="37"/>
       <c r="AJ293" s="37"/>
@@ -16836,7 +16830,7 @@
         <v>75</v>
       </c>
       <c r="B294" s="33" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C294" s="40" t="s">
         <v>38</v>
@@ -16859,7 +16853,7 @@
       <c r="S294" s="34"/>
       <c r="T294" s="34"/>
       <c r="U294" s="40" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="V294" s="34"/>
       <c r="W294" s="34"/>
@@ -16884,7 +16878,7 @@
         <v>75</v>
       </c>
       <c r="B295" s="33" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C295" s="40" t="s">
         <v>38</v>
@@ -16907,7 +16901,7 @@
       <c r="S295" s="34"/>
       <c r="T295" s="34"/>
       <c r="U295" s="40" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="V295" s="34"/>
       <c r="W295" s="34"/>
@@ -16922,7 +16916,7 @@
       <c r="AF295" s="37"/>
       <c r="AG295" s="37"/>
       <c r="AH295" s="40" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="AI295" s="37"/>
       <c r="AJ295" s="37"/>
@@ -16932,7 +16926,7 @@
         <v>75</v>
       </c>
       <c r="B296" s="33" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C296" s="40" t="s">
         <v>38</v>
@@ -16955,7 +16949,7 @@
       <c r="S296" s="34"/>
       <c r="T296" s="34"/>
       <c r="U296" s="40" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="V296" s="34"/>
       <c r="W296" s="34"/>
@@ -16980,7 +16974,7 @@
         <v>75</v>
       </c>
       <c r="B297" s="33" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C297" s="40" t="s">
         <v>38</v>
@@ -17003,7 +16997,7 @@
       <c r="S297" s="34"/>
       <c r="T297" s="34"/>
       <c r="U297" s="40" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="V297" s="34"/>
       <c r="W297" s="34"/>
@@ -17018,7 +17012,7 @@
       <c r="AF297" s="37"/>
       <c r="AG297" s="37"/>
       <c r="AH297" s="40" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="AI297" s="37"/>
       <c r="AJ297" s="37"/>
@@ -17028,7 +17022,7 @@
         <v>75</v>
       </c>
       <c r="B298" s="33" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C298" s="40" t="s">
         <v>38</v>
@@ -17051,7 +17045,7 @@
       <c r="S298" s="34"/>
       <c r="T298" s="34"/>
       <c r="U298" s="37" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="V298" s="34"/>
       <c r="W298" s="34"/>
@@ -17066,7 +17060,7 @@
       <c r="AF298" s="37"/>
       <c r="AG298" s="37"/>
       <c r="AH298" s="40" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AI298" s="37"/>
       <c r="AJ298" s="37"/>
@@ -17076,7 +17070,7 @@
         <v>55</v>
       </c>
       <c r="B299" s="33" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C299" s="34"/>
       <c r="D299" s="35"/>
@@ -17118,7 +17112,7 @@
         <v>55</v>
       </c>
       <c r="B300" s="33" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C300" s="34"/>
       <c r="D300" s="35"/>
@@ -17202,7 +17196,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{007A00F1-00AD-49F4-BF2A-0051005A007F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00D3006B-00A8-468D-95F7-00F200E000EE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -17211,7 +17205,7 @@
           </x14:formula2>
           <xm:sqref>J2:J43 J45:J291 J293:J301</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00DF006E-0053-4943-954A-00EB0094006F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00CF0043-0030-41D2-91B1-001F00DE0047}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -17246,7 +17240,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="41" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B1" s="41" t="s">
         <v>1</v>
@@ -17273,7 +17267,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="49" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="K1" s="49"/>
       <c r="L1" s="49"/>
@@ -17293,13 +17287,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="49" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B2" s="49" t="s">
         <v>102</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -17326,13 +17320,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="49" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B3" s="49" t="s">
         <v>138</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -17386,13 +17380,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="49" t="s">
+        <v>587</v>
+      </c>
+      <c r="B5" s="49" t="s">
         <v>588</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="C5" s="10" t="s">
         <v>589</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>590</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -17419,13 +17413,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="49" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B6" s="49" t="s">
+        <v>590</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>591</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>592</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -17479,13 +17473,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="49" t="s">
+        <v>592</v>
+      </c>
+      <c r="B8" s="49" t="s">
         <v>593</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="C8" s="10" t="s">
         <v>594</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>595</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -17512,13 +17506,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="49" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B9" s="49" t="s">
+        <v>595</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>596</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>597</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -17545,13 +17539,13 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="49" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B10" s="49" t="s">
+        <v>597</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>598</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>599</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -17605,10 +17599,10 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="49" t="s">
+        <v>599</v>
+      </c>
+      <c r="B12" s="49" t="s">
         <v>600</v>
-      </c>
-      <c r="B12" s="49" t="s">
-        <v>601</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>382</v>
@@ -17638,10 +17632,10 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="49" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>386</v>
@@ -17671,10 +17665,10 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="49" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B14" s="49" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>389</v>
@@ -17731,10 +17725,10 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="49" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>382</v>
@@ -17764,10 +17758,10 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="49" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>386</v>
@@ -17824,13 +17818,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="49" t="s">
+        <v>604</v>
+      </c>
+      <c r="B19" s="49" t="s">
         <v>605</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="C19" s="49" t="s">
         <v>606</v>
-      </c>
-      <c r="C19" s="49" t="s">
-        <v>607</v>
       </c>
       <c r="D19" s="49"/>
       <c r="E19" s="49"/>
@@ -17857,13 +17851,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="49" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B20" s="49" t="s">
+        <v>607</v>
+      </c>
+      <c r="C20" s="49" t="s">
         <v>608</v>
-      </c>
-      <c r="C20" s="49" t="s">
-        <v>609</v>
       </c>
       <c r="D20" s="49"/>
       <c r="E20" s="49"/>
@@ -17890,13 +17884,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="49" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B21" s="49" t="s">
+        <v>597</v>
+      </c>
+      <c r="C21" s="49" t="s">
         <v>598</v>
-      </c>
-      <c r="C21" s="49" t="s">
-        <v>599</v>
       </c>
       <c r="D21" s="49"/>
       <c r="E21" s="49"/>
@@ -18052,10 +18046,10 @@
         <v>178</v>
       </c>
       <c r="B26" s="10" t="s">
+        <v>597</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>598</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>599</v>
       </c>
       <c r="D26" s="49"/>
       <c r="E26" s="49"/>
@@ -18279,10 +18273,10 @@
         <v>186</v>
       </c>
       <c r="B33" s="49" t="s">
+        <v>597</v>
+      </c>
+      <c r="C33" s="10" t="s">
         <v>598</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>599</v>
       </c>
       <c r="D33" s="49"/>
       <c r="E33" s="49"/>
@@ -18338,13 +18332,13 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="49" t="s">
+        <v>609</v>
+      </c>
+      <c r="B35" s="49" t="s">
         <v>610</v>
       </c>
-      <c r="B35" s="49" t="s">
+      <c r="C35" s="10" t="s">
         <v>611</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>612</v>
       </c>
       <c r="D35" s="49"/>
       <c r="E35" s="49"/>
@@ -18371,13 +18365,13 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="49" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B36" s="49" t="s">
+        <v>612</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>613</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>614</v>
       </c>
       <c r="D36" s="49"/>
       <c r="E36" s="49"/>
@@ -18431,13 +18425,13 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="49" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B38" s="49" t="s">
         <v>138</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D38" s="49"/>
       <c r="E38" s="49"/>
@@ -18464,13 +18458,13 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="49" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B39" s="49" t="s">
         <v>102</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D39" s="49"/>
       <c r="E39" s="49"/>
@@ -18524,13 +18518,13 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="49" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B41" s="49" t="s">
         <v>138</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D41" s="49"/>
       <c r="E41" s="49"/>
@@ -18557,13 +18551,13 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="49" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B42" s="49" t="s">
         <v>102</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D42" s="49"/>
       <c r="E42" s="49"/>
@@ -18617,13 +18611,13 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="49" t="s">
+        <v>619</v>
+      </c>
+      <c r="B44" s="49" t="s">
         <v>620</v>
       </c>
-      <c r="B44" s="49" t="s">
+      <c r="C44" s="10" t="s">
         <v>621</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>622</v>
       </c>
       <c r="D44" s="49"/>
       <c r="E44" s="49"/>
@@ -18650,13 +18644,13 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="49" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B45" s="49" t="s">
+        <v>622</v>
+      </c>
+      <c r="C45" s="10" t="s">
         <v>623</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>624</v>
       </c>
       <c r="D45" s="49"/>
       <c r="E45" s="49"/>
@@ -18683,13 +18677,13 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="49" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B46" s="49" t="s">
+        <v>624</v>
+      </c>
+      <c r="C46" s="10" t="s">
         <v>625</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>626</v>
       </c>
       <c r="D46" s="49"/>
       <c r="E46" s="49"/>
@@ -18716,13 +18710,13 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="49" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B47" s="49" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D47" s="49"/>
       <c r="E47" s="49"/>
@@ -18779,10 +18773,10 @@
         <v>352</v>
       </c>
       <c r="B49" s="49" t="s">
+        <v>627</v>
+      </c>
+      <c r="C49" s="49" t="s">
         <v>628</v>
-      </c>
-      <c r="C49" s="49" t="s">
-        <v>629</v>
       </c>
       <c r="D49" s="49"/>
       <c r="E49" s="49"/>
@@ -18814,10 +18808,10 @@
         <v>352</v>
       </c>
       <c r="B50" s="49" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D50" s="49"/>
       <c r="E50" s="49"/>
@@ -18849,10 +18843,10 @@
         <v>352</v>
       </c>
       <c r="B51" s="49" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D51" s="49"/>
       <c r="E51" s="49"/>
@@ -18884,10 +18878,10 @@
         <v>352</v>
       </c>
       <c r="B52" s="49" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D52" s="49"/>
       <c r="E52" s="49"/>
@@ -18919,10 +18913,10 @@
         <v>352</v>
       </c>
       <c r="B53" s="49" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D53" s="49"/>
       <c r="E53" s="49"/>
@@ -18978,13 +18972,13 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="49" t="s">
+        <v>633</v>
+      </c>
+      <c r="B55" s="49" t="s">
         <v>634</v>
       </c>
-      <c r="B55" s="49" t="s">
+      <c r="C55" s="10" t="s">
         <v>635</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>636</v>
       </c>
       <c r="D55" s="49"/>
       <c r="E55" s="49"/>
@@ -19011,13 +19005,13 @@
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="49" t="s">
+        <v>636</v>
+      </c>
+      <c r="B56" s="49" t="s">
         <v>637</v>
       </c>
-      <c r="B56" s="49" t="s">
+      <c r="C56" s="10" t="s">
         <v>638</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>639</v>
       </c>
       <c r="D56" s="49"/>
       <c r="E56" s="49"/>
@@ -20556,25 +20550,25 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="50" t="s">
+        <v>639</v>
+      </c>
+      <c r="B1" s="50" t="s">
         <v>640</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="C1" s="50" t="s">
         <v>641</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="D1" s="50" t="s">
         <v>642</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="E1" s="50" t="s">
         <v>643</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="F1" s="50" t="s">
         <v>644</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="G1" s="51" t="s">
         <v>645</v>
-      </c>
-      <c r="G1" s="51" t="s">
-        <v>646</v>
       </c>
       <c r="H1" s="50"/>
       <c r="I1" s="50"/>
@@ -20598,24 +20592,24 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="52" t="s">
+        <v>646</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>647</v>
-      </c>
-      <c r="B2" s="52" t="s">
-        <v>648</v>
       </c>
       <c r="C2" s="53" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-08-19 15-13</v>
+        <v xml:space="preserve">2022-08-23 13-48</v>
       </c>
       <c r="D2" s="54" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E2" s="54" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F2" s="55"/>
       <c r="G2" s="55" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="H2" s="55"/>
       <c r="I2" s="55"/>
@@ -20665,7 +20659,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="50" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B1" s="50" t="s">
         <v>1</v>
@@ -20708,13 +20702,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="63" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B2" s="63" t="s">
         <v>102</v>
       </c>
       <c r="C2" s="63" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D2" s="63"/>
       <c r="E2" s="63"/>
@@ -20739,13 +20733,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="63" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B3" s="63" t="s">
         <v>138</v>
       </c>
       <c r="C3" s="63" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D3" s="63"/>
       <c r="E3" s="63"/>
@@ -20795,13 +20789,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="63" t="s">
+        <v>650</v>
+      </c>
+      <c r="B5" s="63" t="s">
         <v>651</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="C5" s="63" t="s">
         <v>652</v>
-      </c>
-      <c r="C5" s="63" t="s">
-        <v>653</v>
       </c>
       <c r="D5" s="63"/>
       <c r="E5" s="63"/>
@@ -20826,13 +20820,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="63" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B6" s="63" t="s">
+        <v>653</v>
+      </c>
+      <c r="C6" s="63" t="s">
         <v>654</v>
-      </c>
-      <c r="C6" s="63" t="s">
-        <v>655</v>
       </c>
       <c r="D6" s="63"/>
       <c r="E6" s="63"/>
@@ -20857,13 +20851,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="63" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B7" s="63" t="s">
+        <v>655</v>
+      </c>
+      <c r="C7" s="63" t="s">
         <v>656</v>
-      </c>
-      <c r="C7" s="63" t="s">
-        <v>657</v>
       </c>
       <c r="D7" s="63"/>
       <c r="E7" s="63"/>
@@ -20888,13 +20882,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="63" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B8" s="63" t="s">
+        <v>657</v>
+      </c>
+      <c r="C8" s="63" t="s">
         <v>658</v>
-      </c>
-      <c r="C8" s="63" t="s">
-        <v>659</v>
       </c>
       <c r="D8" s="63"/>
       <c r="E8" s="63"/>
@@ -20919,13 +20913,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="63" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B9" s="63" t="s">
+        <v>659</v>
+      </c>
+      <c r="C9" s="63" t="s">
         <v>660</v>
-      </c>
-      <c r="C9" s="63" t="s">
-        <v>661</v>
       </c>
       <c r="D9" s="63"/>
       <c r="E9" s="63"/>
@@ -20975,13 +20969,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="63" t="s">
+        <v>661</v>
+      </c>
+      <c r="B11" s="63" t="s">
         <v>662</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="C11" s="63" t="s">
         <v>663</v>
-      </c>
-      <c r="C11" s="63" t="s">
-        <v>664</v>
       </c>
       <c r="D11" s="63"/>
       <c r="E11" s="63"/>
@@ -21006,13 +21000,13 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="63" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B12" s="63" t="s">
+        <v>664</v>
+      </c>
+      <c r="C12" s="63" t="s">
         <v>665</v>
-      </c>
-      <c r="C12" s="63" t="s">
-        <v>666</v>
       </c>
       <c r="D12" s="63"/>
       <c r="E12" s="63"/>
@@ -21037,13 +21031,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="63" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B13" s="63" t="s">
+        <v>666</v>
+      </c>
+      <c r="C13" s="63" t="s">
         <v>667</v>
-      </c>
-      <c r="C13" s="63" t="s">
-        <v>668</v>
       </c>
       <c r="D13" s="63"/>
       <c r="E13" s="63"/>
@@ -21068,13 +21062,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="63" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B14" s="63" t="s">
+        <v>668</v>
+      </c>
+      <c r="C14" s="63" t="s">
         <v>669</v>
-      </c>
-      <c r="C14" s="63" t="s">
-        <v>670</v>
       </c>
       <c r="D14" s="63"/>
       <c r="E14" s="63"/>
@@ -21099,13 +21093,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="63" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B15" s="63" t="s">
+        <v>670</v>
+      </c>
+      <c r="C15" s="63" t="s">
         <v>671</v>
-      </c>
-      <c r="C15" s="63" t="s">
-        <v>672</v>
       </c>
       <c r="D15" s="63"/>
       <c r="E15" s="63"/>
@@ -21130,13 +21124,13 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="63" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B16" s="63" t="s">
+        <v>672</v>
+      </c>
+      <c r="C16" s="63" t="s">
         <v>673</v>
-      </c>
-      <c r="C16" s="63" t="s">
-        <v>674</v>
       </c>
       <c r="D16" s="63"/>
       <c r="E16" s="63"/>
@@ -21186,13 +21180,13 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="63" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B18" s="63" t="s">
+        <v>662</v>
+      </c>
+      <c r="C18" s="63" t="s">
         <v>663</v>
-      </c>
-      <c r="C18" s="63" t="s">
-        <v>664</v>
       </c>
       <c r="D18" s="63"/>
       <c r="E18" s="63"/>
@@ -21217,13 +21211,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="63" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B19" s="63" t="s">
+        <v>664</v>
+      </c>
+      <c r="C19" s="63" t="s">
         <v>665</v>
-      </c>
-      <c r="C19" s="63" t="s">
-        <v>666</v>
       </c>
       <c r="D19" s="63"/>
       <c r="E19" s="63"/>
@@ -21248,13 +21242,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="63" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B20" s="63" t="s">
+        <v>666</v>
+      </c>
+      <c r="C20" s="63" t="s">
         <v>667</v>
-      </c>
-      <c r="C20" s="63" t="s">
-        <v>668</v>
       </c>
       <c r="D20" s="63"/>
       <c r="E20" s="63"/>
@@ -21279,13 +21273,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="63" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B21" s="63" t="s">
+        <v>668</v>
+      </c>
+      <c r="C21" s="63" t="s">
         <v>669</v>
-      </c>
-      <c r="C21" s="63" t="s">
-        <v>670</v>
       </c>
       <c r="D21" s="63"/>
       <c r="E21" s="63"/>
@@ -21310,13 +21304,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="63" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B22" s="63" t="s">
+        <v>672</v>
+      </c>
+      <c r="C22" s="63" t="s">
         <v>673</v>
-      </c>
-      <c r="C22" s="63" t="s">
-        <v>674</v>
       </c>
       <c r="D22" s="63"/>
       <c r="E22" s="63"/>
@@ -21341,13 +21335,13 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="63" t="s">
+        <v>674</v>
+      </c>
+      <c r="B23" s="63" t="s">
         <v>675</v>
       </c>
-      <c r="B23" s="63" t="s">
+      <c r="C23" s="63" t="s">
         <v>676</v>
-      </c>
-      <c r="C23" s="63" t="s">
-        <v>677</v>
       </c>
       <c r="D23" s="63"/>
       <c r="E23" s="63"/>
@@ -21397,13 +21391,13 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="63" t="s">
+        <v>677</v>
+      </c>
+      <c r="B25" s="63" t="s">
         <v>678</v>
       </c>
-      <c r="B25" s="63" t="s">
+      <c r="C25" s="63" t="s">
         <v>679</v>
-      </c>
-      <c r="C25" s="63" t="s">
-        <v>680</v>
       </c>
       <c r="D25" s="63"/>
       <c r="E25" s="63"/>
@@ -21428,13 +21422,13 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="63" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B26" s="63" t="s">
+        <v>680</v>
+      </c>
+      <c r="C26" s="63" t="s">
         <v>681</v>
-      </c>
-      <c r="C26" s="63" t="s">
-        <v>682</v>
       </c>
       <c r="D26" s="63"/>
       <c r="E26" s="63"/>
@@ -21459,13 +21453,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="63" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B27" s="63" t="s">
+        <v>682</v>
+      </c>
+      <c r="C27" s="63" t="s">
         <v>683</v>
-      </c>
-      <c r="C27" s="63" t="s">
-        <v>684</v>
       </c>
       <c r="D27" s="63"/>
       <c r="E27" s="63"/>
@@ -21490,13 +21484,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="63" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B28" s="63" t="s">
+        <v>684</v>
+      </c>
+      <c r="C28" s="63" t="s">
         <v>685</v>
-      </c>
-      <c r="C28" s="63" t="s">
-        <v>686</v>
       </c>
       <c r="D28" s="63"/>
       <c r="E28" s="63"/>
@@ -21521,13 +21515,13 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="63" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B29" s="63" t="s">
+        <v>597</v>
+      </c>
+      <c r="C29" s="63" t="s">
         <v>598</v>
-      </c>
-      <c r="C29" s="63" t="s">
-        <v>599</v>
       </c>
       <c r="D29" s="63"/>
       <c r="E29" s="63"/>
@@ -21577,13 +21571,13 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="63" t="s">
+        <v>686</v>
+      </c>
+      <c r="B31" s="63" t="s">
         <v>687</v>
       </c>
-      <c r="B31" s="63" t="s">
-        <v>688</v>
-      </c>
       <c r="C31" s="63" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D31" s="63"/>
       <c r="E31" s="63"/>
@@ -21608,13 +21602,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="63" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B32" s="63" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C32" s="63" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D32" s="63"/>
       <c r="E32" s="63"/>
@@ -21664,121 +21658,121 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" ref="B34:B47" si="0">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C34, "(", ""), ")", "")), " ", "_")</f>
         <v>combined_oral_contraceptives</v>
       </c>
       <c r="C34" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
         <v>progesterone_only_pills</v>
       </c>
       <c r="C35" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
         <v>injectibles</v>
       </c>
       <c r="C36" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
         <v>implants_1_rod</v>
       </c>
       <c r="C37" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
         <v>implants_2_rods</v>
       </c>
       <c r="C38" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
         <v>iud</v>
       </c>
       <c r="C39" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
         <v>condoms</v>
       </c>
       <c r="C40" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
         <v>tubal_ligation</v>
       </c>
       <c r="C41" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>cycle_beads</v>
       </c>
       <c r="C42" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B43" t="s">
+        <v>597</v>
+      </c>
+      <c r="C43" t="s">
         <v>598</v>
-      </c>
-      <c r="C43" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -21789,26 +21783,26 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
         <v>wants_to_get_pregnant</v>
       </c>
       <c r="C45" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
         <v>did_not_want_fp</v>
       </c>
       <c r="C46" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -21819,13 +21813,13 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="54" t="s">
+        <v>702</v>
+      </c>
+      <c r="B48" s="54" t="s">
         <v>703</v>
       </c>
-      <c r="B48" s="54" t="s">
+      <c r="C48" s="54" t="s">
         <v>704</v>
-      </c>
-      <c r="C48" s="54" t="s">
-        <v>705</v>
       </c>
       <c r="D48" s="54"/>
       <c r="E48" s="54"/>
@@ -21850,13 +21844,13 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="54" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B49" s="54" t="s">
+        <v>705</v>
+      </c>
+      <c r="C49" s="54" t="s">
         <v>706</v>
-      </c>
-      <c r="C49" s="54" t="s">
-        <v>707</v>
       </c>
       <c r="D49" s="54"/>
       <c r="E49" s="54"/>
@@ -21881,222 +21875,222 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" t="s">
+        <v>707</v>
+      </c>
+      <c r="B51" t="s">
         <v>708</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>709</v>
-      </c>
-      <c r="C51" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B52" t="s">
+        <v>710</v>
+      </c>
+      <c r="C52" t="s">
         <v>711</v>
-      </c>
-      <c r="C52" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B53" t="s">
+        <v>712</v>
+      </c>
+      <c r="C53" t="s">
         <v>713</v>
-      </c>
-      <c r="C53" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B54" t="s">
+        <v>714</v>
+      </c>
+      <c r="C54" t="s">
         <v>715</v>
-      </c>
-      <c r="C54" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B55" t="s">
+        <v>716</v>
+      </c>
+      <c r="C55" t="s">
         <v>717</v>
-      </c>
-      <c r="C55" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B56" t="s">
+        <v>597</v>
+      </c>
+      <c r="C56" t="s">
         <v>598</v>
-      </c>
-      <c r="C56" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="54" t="s">
+        <v>718</v>
+      </c>
+      <c r="B58" s="54" t="s">
         <v>719</v>
       </c>
-      <c r="B58" s="54" t="s">
+      <c r="C58" s="54" t="s">
         <v>720</v>
-      </c>
-      <c r="C58" s="54" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="54" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B59" s="54" t="s">
+        <v>721</v>
+      </c>
+      <c r="C59" s="54" t="s">
         <v>722</v>
-      </c>
-      <c r="C59" s="54" t="s">
-        <v>723</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="54" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B60" s="54" t="s">
+        <v>723</v>
+      </c>
+      <c r="C60" s="54" t="s">
         <v>724</v>
-      </c>
-      <c r="C60" s="54" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="54" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B61" s="54" t="s">
+        <v>597</v>
+      </c>
+      <c r="C61" s="54" t="s">
         <v>598</v>
-      </c>
-      <c r="C61" s="54" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="55" t="s">
+        <v>725</v>
+      </c>
+      <c r="B63" s="55" t="s">
         <v>726</v>
       </c>
-      <c r="B63" s="55" t="s">
+      <c r="C63" s="54" t="s">
         <v>727</v>
-      </c>
-      <c r="C63" s="54" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="55" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B64" s="55" t="s">
+        <v>728</v>
+      </c>
+      <c r="C64" s="54" t="s">
         <v>729</v>
-      </c>
-      <c r="C64" s="54" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="55" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B65" s="55" t="s">
+        <v>730</v>
+      </c>
+      <c r="C65" s="54" t="s">
         <v>731</v>
-      </c>
-      <c r="C65" s="54" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="55" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B66" s="55" t="s">
+        <v>732</v>
+      </c>
+      <c r="C66" s="54" t="s">
         <v>733</v>
-      </c>
-      <c r="C66" s="54" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="55" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B67" s="55" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C67" s="54" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" t="s">
+        <v>734</v>
+      </c>
+      <c r="B69" t="s">
         <v>735</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>736</v>
-      </c>
-      <c r="C69" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B70" t="s">
+        <v>737</v>
+      </c>
+      <c r="C70" t="s">
         <v>738</v>
-      </c>
-      <c r="C70" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" t="s">
+        <v>739</v>
+      </c>
+      <c r="B72" t="s">
         <v>740</v>
       </c>
-      <c r="B72" t="s">
-        <v>741</v>
-      </c>
       <c r="C72" s="64" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B73" t="s">
+        <v>741</v>
+      </c>
+      <c r="C73" t="s">
         <v>742</v>
-      </c>
-      <c r="C73" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B74" t="s">
+        <v>597</v>
+      </c>
+      <c r="C74" t="s">
         <v>598</v>
-      </c>
-      <c r="C74" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Update default/standard config forms to pass validation (#7739)
(cherry picked from commit 922ababb701511a23de495a4bddf1dd6ff4136bc)
</commit_message>
<xml_diff>
--- a/config/default/forms/app/delivery.xlsx
+++ b/config/default/forms/app/delivery.xlsx
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="743">
   <si>
     <t>type</t>
   </si>
@@ -1448,19 +1448,13 @@
   <si>
     <t xml:space="preserve">selected(../../condition/woman_outcome, 'alive_well') or
 selected(../../condition/woman_outcome, 'alive_unwell') or
-../delivery_outcome/babies_alive_num &gt; 0 or
-../../pnc_visits/pnc_visits_additional != ''</t>
+../../delivery_outcome/babies_alive_num &gt; 0</t>
   </si>
   <si>
     <t>r_pnc_visits_completed</t>
   </si>
   <si>
     <t xml:space="preserve">PNC visits completed so far:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../condition/woman_outcome, 'alive_well') or
-selected(../../condition/woman_outcome, 'alive_unwell') or
-../../delivery_outcome/babies_alive_num &gt; 0</t>
   </si>
   <si>
     <t>r_pnc_visit_24hrs</t>
@@ -2417,10 +2411,10 @@
   <numFmts count="1">
     <numFmt numFmtId="160" formatCode="dd\-mm\-yyyy\ hh\-mm\-ss"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <name val="Arial"/>
-      <color indexed="64"/>
+      <color theme="1"/>
       <sz val="10.000000"/>
     </font>
     <font>
@@ -2443,29 +2437,16 @@
     </font>
     <font>
       <name val="Arial"/>
-      <color indexed="64"/>
-      <sz val="11.000000"/>
-    </font>
-    <font>
-      <name val="Arial"/>
       <sz val="11.000000"/>
     </font>
     <font>
       <name val="Arial"/>
       <b/>
-      <color indexed="64"/>
-      <sz val="10.000000"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <b/>
-      <color indexed="64"/>
       <sz val="11.000000"/>
     </font>
     <font>
       <name val="Calibri"/>
       <b/>
-      <color indexed="64"/>
       <sz val="11.000000"/>
     </font>
   </fonts>
@@ -2586,7 +2567,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="65">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -2735,38 +2716,38 @@
       <alignment horizontal="left"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="6" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="0">
+    <xf fontId="5" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="7" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="7" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="2" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="7" fillId="13" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="2" fillId="13" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="7" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="2" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="7" fillId="14" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="2" fillId="14" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="7" fillId="15" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="2" fillId="15" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="7" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="2" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="7" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="2" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
@@ -2774,14 +2755,14 @@
       <alignment horizontal="left"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
+    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
       <protection hidden="0" locked="1"/>
     </xf>
@@ -2793,45 +2774,38 @@
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
     <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="9" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="7" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="9" fillId="13" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="7" fillId="13" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="9" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="7" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="9" fillId="14" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="7" fillId="14" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="9" fillId="15" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="7" fillId="15" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="9" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="7" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="9" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="7" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
-      <alignment wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
@@ -2860,7 +2834,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName=" " id="{7340FC0C-B4EF-7CF6-D8BF-479DF1898AC4}"/>
+  <person displayName=" " id="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}"/>
 </personList>
 </file>
 
@@ -3276,7 +3250,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="U266" personId="{7340FC0C-B4EF-7CF6-D8BF-479DF1898AC4}" id="{0024000F-00D4-40FA-8C20-0081001200D2}" done="0">
+  <threadedComment ref="U266" personId="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}" id="{0024000F-00D4-40FA-8C20-0081001200D2}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org is there a reason we are using .. instead of ${} for these? It would be more consistent if we could use $
 _Assigned to you_
 -Michael Kohn
@@ -3298,7 +3272,7 @@
 -Michael Kohn
 </text>
   </threadedComment>
-  <threadedComment ref="U294" personId="{7340FC0C-B4EF-7CF6-D8BF-479DF1898AC4}" id="{00800045-00BB-493D-B802-00C800B500C8}" done="0">
+  <threadedComment ref="U294" personId="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}" id="{00800045-00BB-493D-B802-00C800B500C8}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org in some of the other forms i see this as ../../patient_id instead, not sure if it matters but feel like we should be consistent. I can update it based on your input. Also not sure why some of the ones below have ../../inputs and this one is ../inputs.
 _Assigned to you_
 -Michael Kohn
@@ -3311,7 +3285,7 @@
 -Michael Kohn
 </text>
   </threadedComment>
-  <threadedComment ref="U298" personId="{7340FC0C-B4EF-7CF6-D8BF-479DF1898AC4}" id="{00660081-00F5-41A0-8991-00C6004C00A7}" done="0">
+  <threadedComment ref="U298" personId="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}" id="{00660081-00F5-41A0-8991-00C6004C00A7}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org in other forms there is a calculate field called pregnancy_uuid_ctx. To be consistent, it feels like we should either add that calculate field to this form and use that for this calculation, or update the other forms to use the "instance('contact-summary'......)" notation. I'd actually prefer to update the other forms to use the "instance('contact-summary'....)" notation because in general i was trying to avoid referencing those top level calculate fields in the data section (there are exceptions). Do you have a preference?
 _Assigned to you_
 -Michael Kohn
@@ -3321,7 +3295,7 @@
 -Marc Abbyad
 </text>
   </threadedComment>
-  <threadedComment ref="AI1" personId="{7340FC0C-B4EF-7CF6-D8BF-479DF1898AC4}" id="{00A000D4-0058-42D9-AAD4-004A00F70029}" done="0">
+  <threadedComment ref="AI1" personId="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}" id="{00A000D4-0058-42D9-AAD4-004A00F70029}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org just FYI i moved these "instance" columns to be after the cht::notes column so that all forms have the same columns in the same order up to AH. Personally I'd probably prefer that all forms have the same exact columns in the same order, even if not all columns are needed for that form.
 _Assigned to you_
 -Michael Kohn
@@ -14147,7 +14121,7 @@
       <c r="I236" s="31"/>
       <c r="J236" s="31"/>
       <c r="K236" s="30" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="L236" s="31"/>
       <c r="M236" s="31"/>
@@ -14180,10 +14154,10 @@
         <v>106</v>
       </c>
       <c r="B237" s="29" t="s">
+        <v>429</v>
+      </c>
+      <c r="C237" s="30" t="s">
         <v>430</v>
-      </c>
-      <c r="C237" s="30" t="s">
-        <v>431</v>
       </c>
       <c r="D237" s="31"/>
       <c r="E237" s="31"/>
@@ -14193,7 +14167,7 @@
       <c r="I237" s="31"/>
       <c r="J237" s="31"/>
       <c r="K237" s="31" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L237" s="31" t="s">
         <v>384</v>
@@ -14228,10 +14202,10 @@
         <v>106</v>
       </c>
       <c r="B238" s="29" t="s">
+        <v>432</v>
+      </c>
+      <c r="C238" s="30" t="s">
         <v>433</v>
-      </c>
-      <c r="C238" s="30" t="s">
-        <v>434</v>
       </c>
       <c r="D238" s="31"/>
       <c r="E238" s="31"/>
@@ -14241,7 +14215,7 @@
       <c r="I238" s="31"/>
       <c r="J238" s="31"/>
       <c r="K238" s="31" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="L238" s="31" t="s">
         <v>384</v>
@@ -14276,10 +14250,10 @@
         <v>106</v>
       </c>
       <c r="B239" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="C239" s="30" t="s">
         <v>436</v>
-      </c>
-      <c r="C239" s="30" t="s">
-        <v>437</v>
       </c>
       <c r="D239" s="31"/>
       <c r="E239" s="31"/>
@@ -14289,7 +14263,7 @@
       <c r="I239" s="31"/>
       <c r="J239" s="31"/>
       <c r="K239" s="31" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="L239" s="31" t="s">
         <v>384</v>
@@ -14324,10 +14298,10 @@
         <v>106</v>
       </c>
       <c r="B240" s="29" t="s">
+        <v>438</v>
+      </c>
+      <c r="C240" s="30" t="s">
         <v>439</v>
-      </c>
-      <c r="C240" s="30" t="s">
-        <v>440</v>
       </c>
       <c r="D240" s="31"/>
       <c r="E240" s="31"/>
@@ -14337,7 +14311,7 @@
       <c r="I240" s="31"/>
       <c r="J240" s="31"/>
       <c r="K240" s="31" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L240" s="31" t="s">
         <v>384</v>
@@ -14372,10 +14346,10 @@
         <v>106</v>
       </c>
       <c r="B241" s="29" t="s">
+        <v>441</v>
+      </c>
+      <c r="C241" s="30" t="s">
         <v>442</v>
-      </c>
-      <c r="C241" s="30" t="s">
-        <v>443</v>
       </c>
       <c r="D241" s="31"/>
       <c r="E241" s="31"/>
@@ -14385,7 +14359,7 @@
       <c r="I241" s="31"/>
       <c r="J241" s="31"/>
       <c r="K241" s="30" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="L241" s="31" t="s">
         <v>384</v>
@@ -14420,10 +14394,10 @@
         <v>106</v>
       </c>
       <c r="B242" s="29" t="s">
+        <v>444</v>
+      </c>
+      <c r="C242" s="30" t="s">
         <v>445</v>
-      </c>
-      <c r="C242" s="30" t="s">
-        <v>446</v>
       </c>
       <c r="D242" s="31"/>
       <c r="E242" s="31"/>
@@ -14433,7 +14407,7 @@
       <c r="I242" s="31"/>
       <c r="J242" s="31"/>
       <c r="K242" s="31" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="L242" s="31"/>
       <c r="M242" s="31"/>
@@ -14466,10 +14440,10 @@
         <v>106</v>
       </c>
       <c r="B243" s="29" t="s">
+        <v>447</v>
+      </c>
+      <c r="C243" s="30" t="s">
         <v>448</v>
-      </c>
-      <c r="C243" s="30" t="s">
-        <v>449</v>
       </c>
       <c r="D243" s="31"/>
       <c r="E243" s="31"/>
@@ -14479,10 +14453,10 @@
       <c r="I243" s="31"/>
       <c r="J243" s="31"/>
       <c r="K243" s="30" t="s">
+        <v>449</v>
+      </c>
+      <c r="L243" s="30" t="s">
         <v>450</v>
-      </c>
-      <c r="L243" s="30" t="s">
-        <v>451</v>
       </c>
       <c r="M243" s="31"/>
       <c r="N243" s="31"/>
@@ -14514,10 +14488,10 @@
         <v>106</v>
       </c>
       <c r="B244" s="29" t="s">
+        <v>451</v>
+      </c>
+      <c r="C244" s="30" t="s">
         <v>452</v>
-      </c>
-      <c r="C244" s="30" t="s">
-        <v>453</v>
       </c>
       <c r="D244" s="31"/>
       <c r="E244" s="31"/>
@@ -14527,7 +14501,7 @@
       <c r="I244" s="31"/>
       <c r="J244" s="31"/>
       <c r="K244" s="30" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="L244" s="30"/>
       <c r="M244" s="31"/>
@@ -14560,7 +14534,7 @@
         <v>106</v>
       </c>
       <c r="B245" s="29" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C245" s="30" t="s">
         <v>413</v>
@@ -14608,10 +14582,10 @@
         <v>106</v>
       </c>
       <c r="B246" s="29" t="s">
+        <v>455</v>
+      </c>
+      <c r="C246" s="30" t="s">
         <v>456</v>
-      </c>
-      <c r="C246" s="30" t="s">
-        <v>457</v>
       </c>
       <c r="D246" s="31"/>
       <c r="E246" s="31"/>
@@ -14656,10 +14630,10 @@
         <v>106</v>
       </c>
       <c r="B247" s="29" t="s">
+        <v>457</v>
+      </c>
+      <c r="C247" s="30" t="s">
         <v>458</v>
-      </c>
-      <c r="C247" s="30" t="s">
-        <v>459</v>
       </c>
       <c r="D247" s="31"/>
       <c r="E247" s="31"/>
@@ -14669,7 +14643,7 @@
       <c r="I247" s="31"/>
       <c r="J247" s="31"/>
       <c r="K247" s="30" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="L247" s="31"/>
       <c r="M247" s="31"/>
@@ -14702,10 +14676,10 @@
         <v>106</v>
       </c>
       <c r="B248" s="29" t="s">
+        <v>459</v>
+      </c>
+      <c r="C248" s="30" t="s">
         <v>460</v>
-      </c>
-      <c r="C248" s="30" t="s">
-        <v>461</v>
       </c>
       <c r="D248" s="31"/>
       <c r="E248" s="31"/>
@@ -14715,7 +14689,7 @@
       <c r="I248" s="31"/>
       <c r="J248" s="31"/>
       <c r="K248" s="30" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="L248" s="31"/>
       <c r="M248" s="31"/>
@@ -14748,10 +14722,10 @@
         <v>106</v>
       </c>
       <c r="B249" s="29" t="s">
+        <v>461</v>
+      </c>
+      <c r="C249" s="30" t="s">
         <v>462</v>
-      </c>
-      <c r="C249" s="30" t="s">
-        <v>463</v>
       </c>
       <c r="D249" s="31"/>
       <c r="E249" s="31"/>
@@ -14764,7 +14738,7 @@
         <v>414</v>
       </c>
       <c r="L249" s="30" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="M249" s="31"/>
       <c r="N249" s="31"/>
@@ -14796,10 +14770,10 @@
         <v>106</v>
       </c>
       <c r="B250" s="29" t="s">
+        <v>464</v>
+      </c>
+      <c r="C250" s="30" t="s">
         <v>465</v>
-      </c>
-      <c r="C250" s="30" t="s">
-        <v>466</v>
       </c>
       <c r="D250" s="31"/>
       <c r="E250" s="31"/>
@@ -14842,10 +14816,10 @@
         <v>106</v>
       </c>
       <c r="B251" s="29" t="s">
+        <v>466</v>
+      </c>
+      <c r="C251" s="30" t="s">
         <v>467</v>
-      </c>
-      <c r="C251" s="30" t="s">
-        <v>468</v>
       </c>
       <c r="D251" s="31"/>
       <c r="E251" s="31"/>
@@ -14888,10 +14862,10 @@
         <v>106</v>
       </c>
       <c r="B252" s="29" t="s">
+        <v>468</v>
+      </c>
+      <c r="C252" s="30" t="s">
         <v>469</v>
-      </c>
-      <c r="C252" s="30" t="s">
-        <v>470</v>
       </c>
       <c r="D252" s="31"/>
       <c r="E252" s="31"/>
@@ -14901,7 +14875,7 @@
       <c r="I252" s="31"/>
       <c r="J252" s="31"/>
       <c r="K252" s="30" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="L252" s="30"/>
       <c r="M252" s="31"/>
@@ -14934,7 +14908,7 @@
         <v>36</v>
       </c>
       <c r="B253" s="29" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C253" s="30" t="s">
         <v>38</v>
@@ -14979,10 +14953,10 @@
     </row>
     <row r="254" ht="15.75" customHeight="1">
       <c r="A254" s="29" t="s">
+        <v>472</v>
+      </c>
+      <c r="B254" s="29" t="s">
         <v>473</v>
-      </c>
-      <c r="B254" s="29" t="s">
-        <v>474</v>
       </c>
       <c r="C254" s="30" t="s">
         <v>38</v>
@@ -15005,7 +14979,7 @@
       <c r="S254" s="30"/>
       <c r="T254" s="30"/>
       <c r="U254" s="30" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="V254" s="31"/>
       <c r="W254" s="30"/>
@@ -15028,7 +15002,7 @@
         <v>75</v>
       </c>
       <c r="B255" s="29" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C255" s="30" t="s">
         <v>38</v>
@@ -15051,7 +15025,7 @@
       <c r="S255" s="30"/>
       <c r="T255" s="30"/>
       <c r="U255" s="30" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="V255" s="31"/>
       <c r="W255" s="30"/>
@@ -15071,10 +15045,10 @@
     </row>
     <row r="256" ht="15.75" customHeight="1">
       <c r="A256" s="29" t="s">
+        <v>477</v>
+      </c>
+      <c r="B256" s="29" t="s">
         <v>478</v>
-      </c>
-      <c r="B256" s="29" t="s">
-        <v>479</v>
       </c>
       <c r="C256" s="30" t="s">
         <v>38</v>
@@ -15097,7 +15071,7 @@
       <c r="S256" s="30"/>
       <c r="T256" s="30"/>
       <c r="U256" s="30" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="V256" s="31"/>
       <c r="W256" s="30"/>
@@ -15120,7 +15094,7 @@
         <v>75</v>
       </c>
       <c r="B257" s="29" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C257" s="30" t="s">
         <v>38</v>
@@ -15143,7 +15117,7 @@
       <c r="S257" s="30"/>
       <c r="T257" s="30"/>
       <c r="U257" s="30" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="V257" s="31"/>
       <c r="W257" s="30"/>
@@ -15166,7 +15140,7 @@
         <v>130</v>
       </c>
       <c r="B258" s="29" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C258" s="30" t="s">
         <v>38</v>
@@ -15189,7 +15163,7 @@
       <c r="S258" s="31"/>
       <c r="T258" s="31"/>
       <c r="U258" s="30" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="V258" s="31"/>
       <c r="W258" s="31"/>
@@ -15212,7 +15186,7 @@
         <v>75</v>
       </c>
       <c r="B259" s="29" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C259" s="30" t="s">
         <v>38</v>
@@ -15235,7 +15209,7 @@
       <c r="S259" s="31"/>
       <c r="T259" s="31"/>
       <c r="U259" s="30" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="V259" s="31"/>
       <c r="W259" s="31"/>
@@ -15258,7 +15232,7 @@
         <v>130</v>
       </c>
       <c r="B260" s="29" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C260" s="30" t="s">
         <v>38</v>
@@ -15281,7 +15255,7 @@
       <c r="S260" s="31"/>
       <c r="T260" s="31"/>
       <c r="U260" s="30" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="V260" s="31"/>
       <c r="W260" s="31"/>
@@ -15304,7 +15278,7 @@
         <v>75</v>
       </c>
       <c r="B261" s="29" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C261" s="30" t="s">
         <v>38</v>
@@ -15327,7 +15301,7 @@
       <c r="S261" s="31"/>
       <c r="T261" s="31"/>
       <c r="U261" s="30" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="V261" s="31"/>
       <c r="W261" s="31"/>
@@ -15468,7 +15442,7 @@
         <v>36</v>
       </c>
       <c r="B265" s="33" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C265" s="34" t="s">
         <v>38</v>
@@ -15516,7 +15490,7 @@
         <v>75</v>
       </c>
       <c r="B266" s="33" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C266" s="40" t="s">
         <v>38</v>
@@ -15539,7 +15513,7 @@
       <c r="S266" s="34"/>
       <c r="T266" s="34"/>
       <c r="U266" s="37" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="V266" s="34"/>
       <c r="W266" s="34"/>
@@ -15554,7 +15528,7 @@
       <c r="AF266" s="37"/>
       <c r="AG266" s="37"/>
       <c r="AH266" s="37" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="AI266" s="37"/>
       <c r="AJ266" s="37"/>
@@ -15564,7 +15538,7 @@
         <v>75</v>
       </c>
       <c r="B267" s="33" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C267" s="40" t="s">
         <v>38</v>
@@ -15587,7 +15561,7 @@
       <c r="S267" s="34"/>
       <c r="T267" s="34"/>
       <c r="U267" s="37" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="V267" s="34"/>
       <c r="W267" s="34"/>
@@ -15602,7 +15576,7 @@
       <c r="AF267" s="37"/>
       <c r="AG267" s="37"/>
       <c r="AH267" s="37" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="AI267" s="37"/>
       <c r="AJ267" s="37"/>
@@ -15612,7 +15586,7 @@
         <v>75</v>
       </c>
       <c r="B268" s="33" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C268" s="40" t="s">
         <v>38</v>
@@ -15635,7 +15609,7 @@
       <c r="S268" s="34"/>
       <c r="T268" s="34"/>
       <c r="U268" s="37" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="V268" s="34"/>
       <c r="W268" s="34"/>
@@ -15650,7 +15624,7 @@
       <c r="AF268" s="37"/>
       <c r="AG268" s="37"/>
       <c r="AH268" s="37" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AI268" s="37"/>
       <c r="AJ268" s="37"/>
@@ -15660,7 +15634,7 @@
         <v>75</v>
       </c>
       <c r="B269" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C269" s="40" t="s">
         <v>38</v>
@@ -15683,7 +15657,7 @@
       <c r="S269" s="34"/>
       <c r="T269" s="34"/>
       <c r="U269" s="37" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="V269" s="34"/>
       <c r="W269" s="34"/>
@@ -15698,7 +15672,7 @@
       <c r="AF269" s="37"/>
       <c r="AG269" s="37"/>
       <c r="AH269" s="37" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="AI269" s="37"/>
       <c r="AJ269" s="37"/>
@@ -15708,7 +15682,7 @@
         <v>75</v>
       </c>
       <c r="B270" s="33" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C270" s="40" t="s">
         <v>38</v>
@@ -15731,7 +15705,7 @@
       <c r="S270" s="34"/>
       <c r="T270" s="34"/>
       <c r="U270" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="V270" s="34"/>
       <c r="W270" s="34"/>
@@ -15746,7 +15720,7 @@
       <c r="AF270" s="37"/>
       <c r="AG270" s="37"/>
       <c r="AH270" s="37" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="AI270" s="37"/>
       <c r="AJ270" s="37"/>
@@ -15756,7 +15730,7 @@
         <v>75</v>
       </c>
       <c r="B271" s="33" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C271" s="40" t="s">
         <v>38</v>
@@ -15779,7 +15753,7 @@
       <c r="S271" s="34"/>
       <c r="T271" s="34"/>
       <c r="U271" s="37" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="V271" s="34"/>
       <c r="W271" s="34"/>
@@ -15794,7 +15768,7 @@
       <c r="AF271" s="37"/>
       <c r="AG271" s="37"/>
       <c r="AH271" s="37" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AI271" s="37"/>
       <c r="AJ271" s="37"/>
@@ -15804,7 +15778,7 @@
         <v>75</v>
       </c>
       <c r="B272" s="33" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C272" s="40" t="s">
         <v>38</v>
@@ -15827,7 +15801,7 @@
       <c r="S272" s="34"/>
       <c r="T272" s="34"/>
       <c r="U272" s="37" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="V272" s="34"/>
       <c r="W272" s="34"/>
@@ -15842,7 +15816,7 @@
       <c r="AF272" s="37"/>
       <c r="AG272" s="37"/>
       <c r="AH272" s="37" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="AI272" s="37"/>
       <c r="AJ272" s="37"/>
@@ -15852,7 +15826,7 @@
         <v>75</v>
       </c>
       <c r="B273" s="33" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C273" s="40" t="s">
         <v>38</v>
@@ -15875,7 +15849,7 @@
       <c r="S273" s="34"/>
       <c r="T273" s="34"/>
       <c r="U273" s="37" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="V273" s="34"/>
       <c r="W273" s="34"/>
@@ -15890,7 +15864,7 @@
       <c r="AF273" s="37"/>
       <c r="AG273" s="37"/>
       <c r="AH273" s="37" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AI273" s="37"/>
       <c r="AJ273" s="37"/>
@@ -15900,7 +15874,7 @@
         <v>75</v>
       </c>
       <c r="B274" s="33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C274" s="40" t="s">
         <v>38</v>
@@ -15923,7 +15897,7 @@
       <c r="S274" s="34"/>
       <c r="T274" s="34"/>
       <c r="U274" s="37" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="V274" s="34"/>
       <c r="W274" s="34"/>
@@ -15938,7 +15912,7 @@
       <c r="AF274" s="37"/>
       <c r="AG274" s="37"/>
       <c r="AH274" s="37" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="AI274" s="37"/>
       <c r="AJ274" s="37"/>
@@ -15948,7 +15922,7 @@
         <v>75</v>
       </c>
       <c r="B275" s="33" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C275" s="40" t="s">
         <v>38</v>
@@ -15971,7 +15945,7 @@
       <c r="S275" s="34"/>
       <c r="T275" s="34"/>
       <c r="U275" s="37" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="V275" s="34"/>
       <c r="W275" s="34"/>
@@ -15986,7 +15960,7 @@
       <c r="AF275" s="37"/>
       <c r="AG275" s="37"/>
       <c r="AH275" s="37" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="AI275" s="37"/>
       <c r="AJ275" s="37"/>
@@ -15996,7 +15970,7 @@
         <v>75</v>
       </c>
       <c r="B276" s="33" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C276" s="40" t="s">
         <v>38</v>
@@ -16019,7 +15993,7 @@
       <c r="S276" s="34"/>
       <c r="T276" s="34"/>
       <c r="U276" s="37" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="V276" s="34"/>
       <c r="W276" s="34"/>
@@ -16034,7 +16008,7 @@
       <c r="AF276" s="37"/>
       <c r="AG276" s="37"/>
       <c r="AH276" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="AI276" s="37"/>
       <c r="AJ276" s="37"/>
@@ -16044,7 +16018,7 @@
         <v>75</v>
       </c>
       <c r="B277" s="33" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C277" s="40" t="s">
         <v>38</v>
@@ -16067,7 +16041,7 @@
       <c r="S277" s="34"/>
       <c r="T277" s="34"/>
       <c r="U277" s="37" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="V277" s="34"/>
       <c r="W277" s="34"/>
@@ -16082,7 +16056,7 @@
       <c r="AF277" s="37"/>
       <c r="AG277" s="37"/>
       <c r="AH277" s="37" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="AI277" s="37"/>
       <c r="AJ277" s="37"/>
@@ -16092,7 +16066,7 @@
         <v>75</v>
       </c>
       <c r="B278" s="33" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C278" s="40" t="s">
         <v>38</v>
@@ -16130,7 +16104,7 @@
       <c r="AF278" s="37"/>
       <c r="AG278" s="37"/>
       <c r="AH278" s="37" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="AI278" s="37"/>
       <c r="AJ278" s="37"/>
@@ -16140,7 +16114,7 @@
         <v>75</v>
       </c>
       <c r="B279" s="33" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C279" s="40" t="s">
         <v>38</v>
@@ -16178,7 +16152,7 @@
       <c r="AF279" s="37"/>
       <c r="AG279" s="37"/>
       <c r="AH279" s="37" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AI279" s="37"/>
       <c r="AJ279" s="37"/>
@@ -16188,7 +16162,7 @@
         <v>75</v>
       </c>
       <c r="B280" s="33" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C280" s="40" t="s">
         <v>38</v>
@@ -16211,7 +16185,7 @@
       <c r="S280" s="34"/>
       <c r="T280" s="34"/>
       <c r="U280" s="37" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="V280" s="34"/>
       <c r="W280" s="34"/>
@@ -16226,7 +16200,7 @@
       <c r="AF280" s="37"/>
       <c r="AG280" s="37"/>
       <c r="AH280" s="37" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AI280" s="37"/>
       <c r="AJ280" s="37"/>
@@ -16236,7 +16210,7 @@
         <v>75</v>
       </c>
       <c r="B281" s="33" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C281" s="40" t="s">
         <v>38</v>
@@ -16259,7 +16233,7 @@
       <c r="S281" s="34"/>
       <c r="T281" s="34"/>
       <c r="U281" s="37" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="V281" s="34"/>
       <c r="W281" s="34"/>
@@ -16274,7 +16248,7 @@
       <c r="AF281" s="37"/>
       <c r="AG281" s="37"/>
       <c r="AH281" s="37" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="AI281" s="37"/>
       <c r="AJ281" s="37"/>
@@ -16284,7 +16258,7 @@
         <v>75</v>
       </c>
       <c r="B282" s="33" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C282" s="40" t="s">
         <v>38</v>
@@ -16307,7 +16281,7 @@
       <c r="S282" s="34"/>
       <c r="T282" s="34"/>
       <c r="U282" s="37" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="V282" s="34"/>
       <c r="W282" s="34"/>
@@ -16322,7 +16296,7 @@
       <c r="AF282" s="37"/>
       <c r="AG282" s="37"/>
       <c r="AH282" s="37" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AI282" s="37"/>
       <c r="AJ282" s="37"/>
@@ -16332,7 +16306,7 @@
         <v>75</v>
       </c>
       <c r="B283" s="33" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C283" s="40" t="s">
         <v>38</v>
@@ -16355,7 +16329,7 @@
       <c r="S283" s="34"/>
       <c r="T283" s="34"/>
       <c r="U283" s="37" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="V283" s="34"/>
       <c r="W283" s="34"/>
@@ -16370,7 +16344,7 @@
       <c r="AF283" s="37"/>
       <c r="AG283" s="37"/>
       <c r="AH283" s="37" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="AI283" s="37"/>
       <c r="AJ283" s="37"/>
@@ -16380,7 +16354,7 @@
         <v>75</v>
       </c>
       <c r="B284" s="33" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C284" s="40" t="s">
         <v>38</v>
@@ -16403,7 +16377,7 @@
       <c r="S284" s="34"/>
       <c r="T284" s="34"/>
       <c r="U284" s="37" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="V284" s="34"/>
       <c r="W284" s="34"/>
@@ -16418,7 +16392,7 @@
       <c r="AF284" s="37"/>
       <c r="AG284" s="37"/>
       <c r="AH284" s="37" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="AI284" s="37"/>
       <c r="AJ284" s="37"/>
@@ -16428,7 +16402,7 @@
         <v>75</v>
       </c>
       <c r="B285" s="33" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C285" s="40" t="s">
         <v>38</v>
@@ -16451,7 +16425,7 @@
       <c r="S285" s="34"/>
       <c r="T285" s="34"/>
       <c r="U285" s="37" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="V285" s="34"/>
       <c r="W285" s="34"/>
@@ -16466,7 +16440,7 @@
       <c r="AF285" s="37"/>
       <c r="AG285" s="37"/>
       <c r="AH285" s="37" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AI285" s="37"/>
       <c r="AJ285" s="37"/>
@@ -16476,7 +16450,7 @@
         <v>75</v>
       </c>
       <c r="B286" s="33" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C286" s="40" t="s">
         <v>38</v>
@@ -16499,7 +16473,7 @@
       <c r="S286" s="34"/>
       <c r="T286" s="34"/>
       <c r="U286" s="37" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="V286" s="34"/>
       <c r="W286" s="34"/>
@@ -16514,7 +16488,7 @@
       <c r="AF286" s="37"/>
       <c r="AG286" s="37"/>
       <c r="AH286" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AI286" s="37"/>
       <c r="AJ286" s="37"/>
@@ -16524,7 +16498,7 @@
         <v>75</v>
       </c>
       <c r="B287" s="33" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C287" s="40" t="s">
         <v>38</v>
@@ -16547,7 +16521,7 @@
       <c r="S287" s="34"/>
       <c r="T287" s="34"/>
       <c r="U287" s="37" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="V287" s="34"/>
       <c r="W287" s="34"/>
@@ -16562,7 +16536,7 @@
       <c r="AF287" s="37"/>
       <c r="AG287" s="37"/>
       <c r="AH287" s="37" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="AI287" s="37"/>
       <c r="AJ287" s="37"/>
@@ -16572,7 +16546,7 @@
         <v>75</v>
       </c>
       <c r="B288" s="33" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C288" s="40" t="s">
         <v>38</v>
@@ -16595,7 +16569,7 @@
       <c r="S288" s="34"/>
       <c r="T288" s="34"/>
       <c r="U288" s="37" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="V288" s="34"/>
       <c r="W288" s="34"/>
@@ -16610,7 +16584,7 @@
       <c r="AF288" s="37"/>
       <c r="AG288" s="37"/>
       <c r="AH288" s="37" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AI288" s="37"/>
       <c r="AJ288" s="37"/>
@@ -16620,7 +16594,7 @@
         <v>75</v>
       </c>
       <c r="B289" s="33" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C289" s="40" t="s">
         <v>38</v>
@@ -16643,7 +16617,7 @@
       <c r="S289" s="34"/>
       <c r="T289" s="34"/>
       <c r="U289" s="37" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="V289" s="34"/>
       <c r="W289" s="34"/>
@@ -16658,7 +16632,7 @@
       <c r="AF289" s="37"/>
       <c r="AG289" s="37"/>
       <c r="AH289" s="37" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="AI289" s="37"/>
       <c r="AJ289" s="37"/>
@@ -16668,7 +16642,7 @@
         <v>75</v>
       </c>
       <c r="B290" s="33" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C290" s="40" t="s">
         <v>38</v>
@@ -16691,7 +16665,7 @@
       <c r="S290" s="34"/>
       <c r="T290" s="34"/>
       <c r="U290" s="37" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="V290" s="34"/>
       <c r="W290" s="34"/>
@@ -16706,7 +16680,7 @@
       <c r="AF290" s="37"/>
       <c r="AG290" s="37"/>
       <c r="AH290" s="37" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="AI290" s="37"/>
       <c r="AJ290" s="37"/>
@@ -16716,7 +16690,7 @@
         <v>75</v>
       </c>
       <c r="B291" s="33" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C291" s="40" t="s">
         <v>38</v>
@@ -16739,7 +16713,7 @@
       <c r="S291" s="34"/>
       <c r="T291" s="34"/>
       <c r="U291" s="37" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="V291" s="34"/>
       <c r="W291" s="34"/>
@@ -16754,7 +16728,7 @@
       <c r="AF291" s="37"/>
       <c r="AG291" s="37"/>
       <c r="AH291" s="37" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="AI291" s="37"/>
       <c r="AJ291" s="37"/>
@@ -16764,7 +16738,7 @@
         <v>36</v>
       </c>
       <c r="B292" s="33" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C292" s="40" t="s">
         <v>38</v>
@@ -16808,7 +16782,7 @@
         <v>75</v>
       </c>
       <c r="B293" s="33" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C293" s="40" t="s">
         <v>38</v>
@@ -16831,7 +16805,7 @@
       <c r="S293" s="34"/>
       <c r="T293" s="34"/>
       <c r="U293" s="40" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="V293" s="34"/>
       <c r="W293" s="34"/>
@@ -16846,7 +16820,7 @@
       <c r="AF293" s="37"/>
       <c r="AG293" s="37"/>
       <c r="AH293" s="40" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="AI293" s="37"/>
       <c r="AJ293" s="37"/>
@@ -16856,7 +16830,7 @@
         <v>75</v>
       </c>
       <c r="B294" s="33" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C294" s="40" t="s">
         <v>38</v>
@@ -16879,7 +16853,7 @@
       <c r="S294" s="34"/>
       <c r="T294" s="34"/>
       <c r="U294" s="40" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="V294" s="34"/>
       <c r="W294" s="34"/>
@@ -16904,7 +16878,7 @@
         <v>75</v>
       </c>
       <c r="B295" s="33" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C295" s="40" t="s">
         <v>38</v>
@@ -16927,7 +16901,7 @@
       <c r="S295" s="34"/>
       <c r="T295" s="34"/>
       <c r="U295" s="40" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="V295" s="34"/>
       <c r="W295" s="34"/>
@@ -16942,7 +16916,7 @@
       <c r="AF295" s="37"/>
       <c r="AG295" s="37"/>
       <c r="AH295" s="40" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="AI295" s="37"/>
       <c r="AJ295" s="37"/>
@@ -16952,7 +16926,7 @@
         <v>75</v>
       </c>
       <c r="B296" s="33" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C296" s="40" t="s">
         <v>38</v>
@@ -16975,7 +16949,7 @@
       <c r="S296" s="34"/>
       <c r="T296" s="34"/>
       <c r="U296" s="40" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="V296" s="34"/>
       <c r="W296" s="34"/>
@@ -17000,7 +16974,7 @@
         <v>75</v>
       </c>
       <c r="B297" s="33" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C297" s="40" t="s">
         <v>38</v>
@@ -17023,7 +16997,7 @@
       <c r="S297" s="34"/>
       <c r="T297" s="34"/>
       <c r="U297" s="40" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="V297" s="34"/>
       <c r="W297" s="34"/>
@@ -17038,7 +17012,7 @@
       <c r="AF297" s="37"/>
       <c r="AG297" s="37"/>
       <c r="AH297" s="40" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="AI297" s="37"/>
       <c r="AJ297" s="37"/>
@@ -17048,7 +17022,7 @@
         <v>75</v>
       </c>
       <c r="B298" s="33" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C298" s="40" t="s">
         <v>38</v>
@@ -17071,7 +17045,7 @@
       <c r="S298" s="34"/>
       <c r="T298" s="34"/>
       <c r="U298" s="37" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="V298" s="34"/>
       <c r="W298" s="34"/>
@@ -17086,7 +17060,7 @@
       <c r="AF298" s="37"/>
       <c r="AG298" s="37"/>
       <c r="AH298" s="40" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AI298" s="37"/>
       <c r="AJ298" s="37"/>
@@ -17096,7 +17070,7 @@
         <v>55</v>
       </c>
       <c r="B299" s="33" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C299" s="34"/>
       <c r="D299" s="35"/>
@@ -17138,7 +17112,7 @@
         <v>55</v>
       </c>
       <c r="B300" s="33" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C300" s="34"/>
       <c r="D300" s="35"/>
@@ -17222,7 +17196,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{002700AA-00D7-4C35-98DB-000A00E800DF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00D3006B-00A8-468D-95F7-00F200E000EE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -17231,7 +17205,7 @@
           </x14:formula2>
           <xm:sqref>J2:J43 J45:J291 J293:J301</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00ED00F2-0002-4BC3-8FEF-000E00F1006F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00CF0043-0030-41D2-91B1-001F00DE0047}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -17266,7 +17240,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="41" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B1" s="41" t="s">
         <v>1</v>
@@ -17293,7 +17267,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="49" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="K1" s="49"/>
       <c r="L1" s="49"/>
@@ -17313,13 +17287,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="49" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B2" s="49" t="s">
         <v>102</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -17346,13 +17320,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="49" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B3" s="49" t="s">
         <v>138</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -17406,13 +17380,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="49" t="s">
+        <v>587</v>
+      </c>
+      <c r="B5" s="49" t="s">
         <v>588</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="C5" s="10" t="s">
         <v>589</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>590</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -17439,13 +17413,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="49" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B6" s="49" t="s">
+        <v>590</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>591</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>592</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -17499,13 +17473,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="49" t="s">
+        <v>592</v>
+      </c>
+      <c r="B8" s="49" t="s">
         <v>593</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="C8" s="10" t="s">
         <v>594</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>595</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -17532,13 +17506,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="49" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B9" s="49" t="s">
+        <v>595</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>596</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>597</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -17565,13 +17539,13 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="49" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B10" s="49" t="s">
+        <v>597</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>598</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>599</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -17625,10 +17599,10 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="49" t="s">
+        <v>599</v>
+      </c>
+      <c r="B12" s="49" t="s">
         <v>600</v>
-      </c>
-      <c r="B12" s="49" t="s">
-        <v>601</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>382</v>
@@ -17658,10 +17632,10 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="49" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>386</v>
@@ -17691,10 +17665,10 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="49" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B14" s="49" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>389</v>
@@ -17751,10 +17725,10 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="49" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>382</v>
@@ -17784,10 +17758,10 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="49" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>386</v>
@@ -17844,13 +17818,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="49" t="s">
+        <v>604</v>
+      </c>
+      <c r="B19" s="49" t="s">
         <v>605</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="C19" s="49" t="s">
         <v>606</v>
-      </c>
-      <c r="C19" s="49" t="s">
-        <v>607</v>
       </c>
       <c r="D19" s="49"/>
       <c r="E19" s="49"/>
@@ -17877,13 +17851,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="49" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B20" s="49" t="s">
+        <v>607</v>
+      </c>
+      <c r="C20" s="49" t="s">
         <v>608</v>
-      </c>
-      <c r="C20" s="49" t="s">
-        <v>609</v>
       </c>
       <c r="D20" s="49"/>
       <c r="E20" s="49"/>
@@ -17910,13 +17884,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="49" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B21" s="49" t="s">
+        <v>597</v>
+      </c>
+      <c r="C21" s="49" t="s">
         <v>598</v>
-      </c>
-      <c r="C21" s="49" t="s">
-        <v>599</v>
       </c>
       <c r="D21" s="49"/>
       <c r="E21" s="49"/>
@@ -18072,10 +18046,10 @@
         <v>178</v>
       </c>
       <c r="B26" s="10" t="s">
+        <v>597</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>598</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>599</v>
       </c>
       <c r="D26" s="49"/>
       <c r="E26" s="49"/>
@@ -18299,10 +18273,10 @@
         <v>186</v>
       </c>
       <c r="B33" s="49" t="s">
+        <v>597</v>
+      </c>
+      <c r="C33" s="10" t="s">
         <v>598</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>599</v>
       </c>
       <c r="D33" s="49"/>
       <c r="E33" s="49"/>
@@ -18358,13 +18332,13 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="49" t="s">
+        <v>609</v>
+      </c>
+      <c r="B35" s="49" t="s">
         <v>610</v>
       </c>
-      <c r="B35" s="49" t="s">
+      <c r="C35" s="10" t="s">
         <v>611</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>612</v>
       </c>
       <c r="D35" s="49"/>
       <c r="E35" s="49"/>
@@ -18391,13 +18365,13 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="49" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B36" s="49" t="s">
+        <v>612</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>613</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>614</v>
       </c>
       <c r="D36" s="49"/>
       <c r="E36" s="49"/>
@@ -18451,13 +18425,13 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="49" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B38" s="49" t="s">
         <v>138</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D38" s="49"/>
       <c r="E38" s="49"/>
@@ -18484,13 +18458,13 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="49" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B39" s="49" t="s">
         <v>102</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D39" s="49"/>
       <c r="E39" s="49"/>
@@ -18544,13 +18518,13 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="49" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B41" s="49" t="s">
         <v>138</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D41" s="49"/>
       <c r="E41" s="49"/>
@@ -18577,13 +18551,13 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="49" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B42" s="49" t="s">
         <v>102</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D42" s="49"/>
       <c r="E42" s="49"/>
@@ -18637,13 +18611,13 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="49" t="s">
+        <v>619</v>
+      </c>
+      <c r="B44" s="49" t="s">
         <v>620</v>
       </c>
-      <c r="B44" s="49" t="s">
+      <c r="C44" s="10" t="s">
         <v>621</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>622</v>
       </c>
       <c r="D44" s="49"/>
       <c r="E44" s="49"/>
@@ -18670,13 +18644,13 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="49" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B45" s="49" t="s">
+        <v>622</v>
+      </c>
+      <c r="C45" s="10" t="s">
         <v>623</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>624</v>
       </c>
       <c r="D45" s="49"/>
       <c r="E45" s="49"/>
@@ -18703,13 +18677,13 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="49" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B46" s="49" t="s">
+        <v>624</v>
+      </c>
+      <c r="C46" s="10" t="s">
         <v>625</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>626</v>
       </c>
       <c r="D46" s="49"/>
       <c r="E46" s="49"/>
@@ -18736,13 +18710,13 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="49" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B47" s="49" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D47" s="49"/>
       <c r="E47" s="49"/>
@@ -18799,10 +18773,10 @@
         <v>352</v>
       </c>
       <c r="B49" s="49" t="s">
+        <v>627</v>
+      </c>
+      <c r="C49" s="49" t="s">
         <v>628</v>
-      </c>
-      <c r="C49" s="49" t="s">
-        <v>629</v>
       </c>
       <c r="D49" s="49"/>
       <c r="E49" s="49"/>
@@ -18834,10 +18808,10 @@
         <v>352</v>
       </c>
       <c r="B50" s="49" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D50" s="49"/>
       <c r="E50" s="49"/>
@@ -18869,10 +18843,10 @@
         <v>352</v>
       </c>
       <c r="B51" s="49" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D51" s="49"/>
       <c r="E51" s="49"/>
@@ -18904,10 +18878,10 @@
         <v>352</v>
       </c>
       <c r="B52" s="49" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D52" s="49"/>
       <c r="E52" s="49"/>
@@ -18939,10 +18913,10 @@
         <v>352</v>
       </c>
       <c r="B53" s="49" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D53" s="49"/>
       <c r="E53" s="49"/>
@@ -18998,13 +18972,13 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="49" t="s">
+        <v>633</v>
+      </c>
+      <c r="B55" s="49" t="s">
         <v>634</v>
       </c>
-      <c r="B55" s="49" t="s">
+      <c r="C55" s="10" t="s">
         <v>635</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>636</v>
       </c>
       <c r="D55" s="49"/>
       <c r="E55" s="49"/>
@@ -19031,13 +19005,13 @@
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="49" t="s">
+        <v>636</v>
+      </c>
+      <c r="B56" s="49" t="s">
         <v>637</v>
       </c>
-      <c r="B56" s="49" t="s">
+      <c r="C56" s="10" t="s">
         <v>638</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>639</v>
       </c>
       <c r="D56" s="49"/>
       <c r="E56" s="49"/>
@@ -20576,25 +20550,25 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="50" t="s">
+        <v>639</v>
+      </c>
+      <c r="B1" s="50" t="s">
         <v>640</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="C1" s="50" t="s">
         <v>641</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="D1" s="50" t="s">
         <v>642</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="E1" s="50" t="s">
         <v>643</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="F1" s="50" t="s">
         <v>644</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="G1" s="51" t="s">
         <v>645</v>
-      </c>
-      <c r="G1" s="51" t="s">
-        <v>646</v>
       </c>
       <c r="H1" s="50"/>
       <c r="I1" s="50"/>
@@ -20618,24 +20592,24 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="52" t="s">
+        <v>646</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>647</v>
-      </c>
-      <c r="B2" s="52" t="s">
-        <v>648</v>
       </c>
       <c r="C2" s="53" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-06-14 15-07</v>
+        <v xml:space="preserve">2022-08-23 13-48</v>
       </c>
       <c r="D2" s="54" t="s">
+        <v>648</v>
+      </c>
+      <c r="E2" s="54" t="s">
+        <v>490</v>
+      </c>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55" t="s">
         <v>649</v>
-      </c>
-      <c r="E2" s="54" t="s">
-        <v>491</v>
-      </c>
-      <c r="F2" s="55"/>
-      <c r="G2" s="56" t="s">
-        <v>650</v>
       </c>
       <c r="H2" s="55"/>
       <c r="I2" s="55"/>
@@ -20685,30 +20659,30 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="50" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="G1" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="62" t="s">
+      <c r="H1" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="63" t="s">
+      <c r="I1" s="62" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="55"/>
@@ -20727,1078 +20701,1078 @@
       <c r="W1" s="55"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="63" t="s">
+        <v>584</v>
+      </c>
+      <c r="B2" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="63" t="s">
         <v>585</v>
       </c>
-      <c r="B2" s="64" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="64" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="63"/>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="63" t="s">
+        <v>584</v>
+      </c>
+      <c r="B3" s="63" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="63" t="s">
         <v>586</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="64"/>
-      <c r="U2" s="64"/>
-      <c r="V2" s="64"/>
-      <c r="W2" s="64"/>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="64" t="s">
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="63"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="63"/>
+      <c r="U3" s="63"/>
+      <c r="V3" s="63"/>
+      <c r="W3" s="63"/>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="63"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="63"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="63"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="63"/>
+      <c r="T4" s="63"/>
+      <c r="U4" s="63"/>
+      <c r="V4" s="63"/>
+      <c r="W4" s="63"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="63" t="s">
+        <v>650</v>
+      </c>
+      <c r="B5" s="63" t="s">
+        <v>651</v>
+      </c>
+      <c r="C5" s="63" t="s">
+        <v>652</v>
+      </c>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="63"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="63"/>
+      <c r="U5" s="63"/>
+      <c r="V5" s="63"/>
+      <c r="W5" s="63"/>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="63" t="s">
+        <v>650</v>
+      </c>
+      <c r="B6" s="63" t="s">
+        <v>653</v>
+      </c>
+      <c r="C6" s="63" t="s">
+        <v>654</v>
+      </c>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="63"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
+      <c r="V6" s="63"/>
+      <c r="W6" s="63"/>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="63" t="s">
+        <v>650</v>
+      </c>
+      <c r="B7" s="63" t="s">
+        <v>655</v>
+      </c>
+      <c r="C7" s="63" t="s">
+        <v>656</v>
+      </c>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="63"/>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="63"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="63"/>
+      <c r="W7" s="63"/>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="63" t="s">
+        <v>650</v>
+      </c>
+      <c r="B8" s="63" t="s">
+        <v>657</v>
+      </c>
+      <c r="C8" s="63" t="s">
+        <v>658</v>
+      </c>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63"/>
+      <c r="N8" s="63"/>
+      <c r="O8" s="63"/>
+      <c r="P8" s="63"/>
+      <c r="Q8" s="63"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="63"/>
+      <c r="U8" s="63"/>
+      <c r="V8" s="63"/>
+      <c r="W8" s="63"/>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="63" t="s">
+        <v>650</v>
+      </c>
+      <c r="B9" s="63" t="s">
+        <v>659</v>
+      </c>
+      <c r="C9" s="63" t="s">
+        <v>660</v>
+      </c>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="63"/>
+      <c r="P9" s="63"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="63"/>
+      <c r="V9" s="63"/>
+      <c r="W9" s="63"/>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="63"/>
+      <c r="P10" s="63"/>
+      <c r="Q10" s="63"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="63"/>
+      <c r="U10" s="63"/>
+      <c r="V10" s="63"/>
+      <c r="W10" s="63"/>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="63" t="s">
+        <v>661</v>
+      </c>
+      <c r="B11" s="63" t="s">
+        <v>662</v>
+      </c>
+      <c r="C11" s="63" t="s">
+        <v>663</v>
+      </c>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="63"/>
+      <c r="N11" s="63"/>
+      <c r="O11" s="63"/>
+      <c r="P11" s="63"/>
+      <c r="Q11" s="63"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="63"/>
+      <c r="T11" s="63"/>
+      <c r="U11" s="63"/>
+      <c r="V11" s="63"/>
+      <c r="W11" s="63"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="63" t="s">
+        <v>661</v>
+      </c>
+      <c r="B12" s="63" t="s">
+        <v>664</v>
+      </c>
+      <c r="C12" s="63" t="s">
+        <v>665</v>
+      </c>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="63"/>
+      <c r="P12" s="63"/>
+      <c r="Q12" s="63"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="63"/>
+      <c r="V12" s="63"/>
+      <c r="W12" s="63"/>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="63" t="s">
+        <v>661</v>
+      </c>
+      <c r="B13" s="63" t="s">
+        <v>666</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>667</v>
+      </c>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="63"/>
+      <c r="O13" s="63"/>
+      <c r="P13" s="63"/>
+      <c r="Q13" s="63"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="63"/>
+      <c r="U13" s="63"/>
+      <c r="V13" s="63"/>
+      <c r="W13" s="63"/>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="63" t="s">
+        <v>661</v>
+      </c>
+      <c r="B14" s="63" t="s">
+        <v>668</v>
+      </c>
+      <c r="C14" s="63" t="s">
+        <v>669</v>
+      </c>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="63"/>
+      <c r="N14" s="63"/>
+      <c r="O14" s="63"/>
+      <c r="P14" s="63"/>
+      <c r="Q14" s="63"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="63"/>
+      <c r="U14" s="63"/>
+      <c r="V14" s="63"/>
+      <c r="W14" s="63"/>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="63" t="s">
+        <v>661</v>
+      </c>
+      <c r="B15" s="63" t="s">
+        <v>670</v>
+      </c>
+      <c r="C15" s="63" t="s">
+        <v>671</v>
+      </c>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="63"/>
+      <c r="O15" s="63"/>
+      <c r="P15" s="63"/>
+      <c r="Q15" s="63"/>
+      <c r="R15" s="63"/>
+      <c r="S15" s="63"/>
+      <c r="T15" s="63"/>
+      <c r="U15" s="63"/>
+      <c r="V15" s="63"/>
+      <c r="W15" s="63"/>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="63" t="s">
+        <v>661</v>
+      </c>
+      <c r="B16" s="63" t="s">
+        <v>672</v>
+      </c>
+      <c r="C16" s="63" t="s">
+        <v>673</v>
+      </c>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="63"/>
+      <c r="L16" s="63"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="63"/>
+      <c r="O16" s="63"/>
+      <c r="P16" s="63"/>
+      <c r="Q16" s="63"/>
+      <c r="R16" s="63"/>
+      <c r="S16" s="63"/>
+      <c r="T16" s="63"/>
+      <c r="U16" s="63"/>
+      <c r="V16" s="63"/>
+      <c r="W16" s="63"/>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="63"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="63"/>
+      <c r="O17" s="63"/>
+      <c r="P17" s="63"/>
+      <c r="Q17" s="63"/>
+      <c r="R17" s="63"/>
+      <c r="S17" s="63"/>
+      <c r="T17" s="63"/>
+      <c r="U17" s="63"/>
+      <c r="V17" s="63"/>
+      <c r="W17" s="63"/>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="63" t="s">
+        <v>674</v>
+      </c>
+      <c r="B18" s="63" t="s">
+        <v>662</v>
+      </c>
+      <c r="C18" s="63" t="s">
+        <v>663</v>
+      </c>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="63"/>
+      <c r="N18" s="63"/>
+      <c r="O18" s="63"/>
+      <c r="P18" s="63"/>
+      <c r="Q18" s="63"/>
+      <c r="R18" s="63"/>
+      <c r="S18" s="63"/>
+      <c r="T18" s="63"/>
+      <c r="U18" s="63"/>
+      <c r="V18" s="63"/>
+      <c r="W18" s="63"/>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="63" t="s">
+        <v>674</v>
+      </c>
+      <c r="B19" s="63" t="s">
+        <v>664</v>
+      </c>
+      <c r="C19" s="63" t="s">
+        <v>665</v>
+      </c>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="63"/>
+      <c r="O19" s="63"/>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="63"/>
+      <c r="R19" s="63"/>
+      <c r="S19" s="63"/>
+      <c r="T19" s="63"/>
+      <c r="U19" s="63"/>
+      <c r="V19" s="63"/>
+      <c r="W19" s="63"/>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="63" t="s">
+        <v>674</v>
+      </c>
+      <c r="B20" s="63" t="s">
+        <v>666</v>
+      </c>
+      <c r="C20" s="63" t="s">
+        <v>667</v>
+      </c>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="63"/>
+      <c r="P20" s="63"/>
+      <c r="Q20" s="63"/>
+      <c r="R20" s="63"/>
+      <c r="S20" s="63"/>
+      <c r="T20" s="63"/>
+      <c r="U20" s="63"/>
+      <c r="V20" s="63"/>
+      <c r="W20" s="63"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="63" t="s">
+        <v>674</v>
+      </c>
+      <c r="B21" s="63" t="s">
+        <v>668</v>
+      </c>
+      <c r="C21" s="63" t="s">
+        <v>669</v>
+      </c>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="63"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="63"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="63"/>
+      <c r="L21" s="63"/>
+      <c r="M21" s="63"/>
+      <c r="N21" s="63"/>
+      <c r="O21" s="63"/>
+      <c r="P21" s="63"/>
+      <c r="Q21" s="63"/>
+      <c r="R21" s="63"/>
+      <c r="S21" s="63"/>
+      <c r="T21" s="63"/>
+      <c r="U21" s="63"/>
+      <c r="V21" s="63"/>
+      <c r="W21" s="63"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="63" t="s">
+        <v>674</v>
+      </c>
+      <c r="B22" s="63" t="s">
+        <v>672</v>
+      </c>
+      <c r="C22" s="63" t="s">
+        <v>673</v>
+      </c>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="63"/>
+      <c r="J22" s="63"/>
+      <c r="K22" s="63"/>
+      <c r="L22" s="63"/>
+      <c r="M22" s="63"/>
+      <c r="N22" s="63"/>
+      <c r="O22" s="63"/>
+      <c r="P22" s="63"/>
+      <c r="Q22" s="63"/>
+      <c r="R22" s="63"/>
+      <c r="S22" s="63"/>
+      <c r="T22" s="63"/>
+      <c r="U22" s="63"/>
+      <c r="V22" s="63"/>
+      <c r="W22" s="63"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="63" t="s">
+        <v>674</v>
+      </c>
+      <c r="B23" s="63" t="s">
+        <v>675</v>
+      </c>
+      <c r="C23" s="63" t="s">
+        <v>676</v>
+      </c>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="63"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="63"/>
+      <c r="M23" s="63"/>
+      <c r="N23" s="63"/>
+      <c r="O23" s="63"/>
+      <c r="P23" s="63"/>
+      <c r="Q23" s="63"/>
+      <c r="R23" s="63"/>
+      <c r="S23" s="63"/>
+      <c r="T23" s="63"/>
+      <c r="U23" s="63"/>
+      <c r="V23" s="63"/>
+      <c r="W23" s="63"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="63"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="63"/>
+      <c r="G24" s="63"/>
+      <c r="H24" s="63"/>
+      <c r="I24" s="63"/>
+      <c r="J24" s="63"/>
+      <c r="K24" s="63"/>
+      <c r="L24" s="63"/>
+      <c r="M24" s="63"/>
+      <c r="N24" s="63"/>
+      <c r="O24" s="63"/>
+      <c r="P24" s="63"/>
+      <c r="Q24" s="63"/>
+      <c r="R24" s="63"/>
+      <c r="S24" s="63"/>
+      <c r="T24" s="63"/>
+      <c r="U24" s="63"/>
+      <c r="V24" s="63"/>
+      <c r="W24" s="63"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="63" t="s">
+        <v>677</v>
+      </c>
+      <c r="B25" s="63" t="s">
+        <v>678</v>
+      </c>
+      <c r="C25" s="63" t="s">
+        <v>679</v>
+      </c>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="63"/>
+      <c r="J25" s="63"/>
+      <c r="K25" s="63"/>
+      <c r="L25" s="63"/>
+      <c r="M25" s="63"/>
+      <c r="N25" s="63"/>
+      <c r="O25" s="63"/>
+      <c r="P25" s="63"/>
+      <c r="Q25" s="63"/>
+      <c r="R25" s="63"/>
+      <c r="S25" s="63"/>
+      <c r="T25" s="63"/>
+      <c r="U25" s="63"/>
+      <c r="V25" s="63"/>
+      <c r="W25" s="63"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="63" t="s">
+        <v>677</v>
+      </c>
+      <c r="B26" s="63" t="s">
+        <v>680</v>
+      </c>
+      <c r="C26" s="63" t="s">
+        <v>681</v>
+      </c>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="63"/>
+      <c r="J26" s="63"/>
+      <c r="K26" s="63"/>
+      <c r="L26" s="63"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="63"/>
+      <c r="O26" s="63"/>
+      <c r="P26" s="63"/>
+      <c r="Q26" s="63"/>
+      <c r="R26" s="63"/>
+      <c r="S26" s="63"/>
+      <c r="T26" s="63"/>
+      <c r="U26" s="63"/>
+      <c r="V26" s="63"/>
+      <c r="W26" s="63"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="63" t="s">
+        <v>677</v>
+      </c>
+      <c r="B27" s="63" t="s">
+        <v>682</v>
+      </c>
+      <c r="C27" s="63" t="s">
+        <v>683</v>
+      </c>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="63"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="63"/>
+      <c r="P27" s="63"/>
+      <c r="Q27" s="63"/>
+      <c r="R27" s="63"/>
+      <c r="S27" s="63"/>
+      <c r="T27" s="63"/>
+      <c r="U27" s="63"/>
+      <c r="V27" s="63"/>
+      <c r="W27" s="63"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="63" t="s">
+        <v>677</v>
+      </c>
+      <c r="B28" s="63" t="s">
+        <v>684</v>
+      </c>
+      <c r="C28" s="63" t="s">
+        <v>685</v>
+      </c>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="63"/>
+      <c r="J28" s="63"/>
+      <c r="K28" s="63"/>
+      <c r="L28" s="63"/>
+      <c r="M28" s="63"/>
+      <c r="N28" s="63"/>
+      <c r="O28" s="63"/>
+      <c r="P28" s="63"/>
+      <c r="Q28" s="63"/>
+      <c r="R28" s="63"/>
+      <c r="S28" s="63"/>
+      <c r="T28" s="63"/>
+      <c r="U28" s="63"/>
+      <c r="V28" s="63"/>
+      <c r="W28" s="63"/>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="63" t="s">
+        <v>677</v>
+      </c>
+      <c r="B29" s="63" t="s">
+        <v>597</v>
+      </c>
+      <c r="C29" s="63" t="s">
+        <v>598</v>
+      </c>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="63"/>
+      <c r="J29" s="63"/>
+      <c r="K29" s="63"/>
+      <c r="L29" s="63"/>
+      <c r="M29" s="63"/>
+      <c r="N29" s="63"/>
+      <c r="O29" s="63"/>
+      <c r="P29" s="63"/>
+      <c r="Q29" s="63"/>
+      <c r="R29" s="63"/>
+      <c r="S29" s="63"/>
+      <c r="T29" s="63"/>
+      <c r="U29" s="63"/>
+      <c r="V29" s="63"/>
+      <c r="W29" s="63"/>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="63"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="63"/>
+      <c r="K30" s="63"/>
+      <c r="L30" s="63"/>
+      <c r="M30" s="63"/>
+      <c r="N30" s="63"/>
+      <c r="O30" s="63"/>
+      <c r="P30" s="63"/>
+      <c r="Q30" s="63"/>
+      <c r="R30" s="63"/>
+      <c r="S30" s="63"/>
+      <c r="T30" s="63"/>
+      <c r="U30" s="63"/>
+      <c r="V30" s="63"/>
+      <c r="W30" s="63"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="63" t="s">
+        <v>686</v>
+      </c>
+      <c r="B31" s="63" t="s">
+        <v>687</v>
+      </c>
+      <c r="C31" s="63" t="s">
         <v>585</v>
       </c>
-      <c r="B3" s="64" t="s">
-        <v>138</v>
-      </c>
-      <c r="C3" s="64" t="s">
-        <v>587</v>
-      </c>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="64"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
-      <c r="O4" s="64"/>
-      <c r="P4" s="64"/>
-      <c r="Q4" s="64"/>
-      <c r="R4" s="64"/>
-      <c r="S4" s="64"/>
-      <c r="T4" s="64"/>
-      <c r="U4" s="64"/>
-      <c r="V4" s="64"/>
-      <c r="W4" s="64"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="64" t="s">
-        <v>651</v>
-      </c>
-      <c r="B5" s="64" t="s">
-        <v>652</v>
-      </c>
-      <c r="C5" s="64" t="s">
-        <v>653</v>
-      </c>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="64"/>
-      <c r="N5" s="64"/>
-      <c r="O5" s="64"/>
-      <c r="P5" s="64"/>
-      <c r="Q5" s="64"/>
-      <c r="R5" s="64"/>
-      <c r="S5" s="64"/>
-      <c r="T5" s="64"/>
-      <c r="U5" s="64"/>
-      <c r="V5" s="64"/>
-      <c r="W5" s="64"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="64" t="s">
-        <v>651</v>
-      </c>
-      <c r="B6" s="64" t="s">
-        <v>654</v>
-      </c>
-      <c r="C6" s="64" t="s">
-        <v>655</v>
-      </c>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="64"/>
-      <c r="N6" s="64"/>
-      <c r="O6" s="64"/>
-      <c r="P6" s="64"/>
-      <c r="Q6" s="64"/>
-      <c r="R6" s="64"/>
-      <c r="S6" s="64"/>
-      <c r="T6" s="64"/>
-      <c r="U6" s="64"/>
-      <c r="V6" s="64"/>
-      <c r="W6" s="64"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="64" t="s">
-        <v>651</v>
-      </c>
-      <c r="B7" s="64" t="s">
-        <v>656</v>
-      </c>
-      <c r="C7" s="64" t="s">
-        <v>657</v>
-      </c>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="64"/>
-      <c r="M7" s="64"/>
-      <c r="N7" s="64"/>
-      <c r="O7" s="64"/>
-      <c r="P7" s="64"/>
-      <c r="Q7" s="64"/>
-      <c r="R7" s="64"/>
-      <c r="S7" s="64"/>
-      <c r="T7" s="64"/>
-      <c r="U7" s="64"/>
-      <c r="V7" s="64"/>
-      <c r="W7" s="64"/>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="64" t="s">
-        <v>651</v>
-      </c>
-      <c r="B8" s="64" t="s">
-        <v>658</v>
-      </c>
-      <c r="C8" s="64" t="s">
-        <v>659</v>
-      </c>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="64"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="64"/>
-      <c r="N8" s="64"/>
-      <c r="O8" s="64"/>
-      <c r="P8" s="64"/>
-      <c r="Q8" s="64"/>
-      <c r="R8" s="64"/>
-      <c r="S8" s="64"/>
-      <c r="T8" s="64"/>
-      <c r="U8" s="64"/>
-      <c r="V8" s="64"/>
-      <c r="W8" s="64"/>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="64" t="s">
-        <v>651</v>
-      </c>
-      <c r="B9" s="64" t="s">
-        <v>660</v>
-      </c>
-      <c r="C9" s="64" t="s">
-        <v>661</v>
-      </c>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="64"/>
-      <c r="N9" s="64"/>
-      <c r="O9" s="64"/>
-      <c r="P9" s="64"/>
-      <c r="Q9" s="64"/>
-      <c r="R9" s="64"/>
-      <c r="S9" s="64"/>
-      <c r="T9" s="64"/>
-      <c r="U9" s="64"/>
-      <c r="V9" s="64"/>
-      <c r="W9" s="64"/>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="64"/>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="64"/>
-      <c r="N10" s="64"/>
-      <c r="O10" s="64"/>
-      <c r="P10" s="64"/>
-      <c r="Q10" s="64"/>
-      <c r="R10" s="64"/>
-      <c r="S10" s="64"/>
-      <c r="T10" s="64"/>
-      <c r="U10" s="64"/>
-      <c r="V10" s="64"/>
-      <c r="W10" s="64"/>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="64" t="s">
-        <v>662</v>
-      </c>
-      <c r="B11" s="64" t="s">
-        <v>663</v>
-      </c>
-      <c r="C11" s="64" t="s">
-        <v>664</v>
-      </c>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="64"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="64"/>
-      <c r="N11" s="64"/>
-      <c r="O11" s="64"/>
-      <c r="P11" s="64"/>
-      <c r="Q11" s="64"/>
-      <c r="R11" s="64"/>
-      <c r="S11" s="64"/>
-      <c r="T11" s="64"/>
-      <c r="U11" s="64"/>
-      <c r="V11" s="64"/>
-      <c r="W11" s="64"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="64" t="s">
-        <v>662</v>
-      </c>
-      <c r="B12" s="64" t="s">
-        <v>665</v>
-      </c>
-      <c r="C12" s="64" t="s">
-        <v>666</v>
-      </c>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="64"/>
-      <c r="K12" s="64"/>
-      <c r="L12" s="64"/>
-      <c r="M12" s="64"/>
-      <c r="N12" s="64"/>
-      <c r="O12" s="64"/>
-      <c r="P12" s="64"/>
-      <c r="Q12" s="64"/>
-      <c r="R12" s="64"/>
-      <c r="S12" s="64"/>
-      <c r="T12" s="64"/>
-      <c r="U12" s="64"/>
-      <c r="V12" s="64"/>
-      <c r="W12" s="64"/>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="64" t="s">
-        <v>662</v>
-      </c>
-      <c r="B13" s="64" t="s">
-        <v>667</v>
-      </c>
-      <c r="C13" s="64" t="s">
-        <v>668</v>
-      </c>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="64"/>
-      <c r="M13" s="64"/>
-      <c r="N13" s="64"/>
-      <c r="O13" s="64"/>
-      <c r="P13" s="64"/>
-      <c r="Q13" s="64"/>
-      <c r="R13" s="64"/>
-      <c r="S13" s="64"/>
-      <c r="T13" s="64"/>
-      <c r="U13" s="64"/>
-      <c r="V13" s="64"/>
-      <c r="W13" s="64"/>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="64" t="s">
-        <v>662</v>
-      </c>
-      <c r="B14" s="64" t="s">
-        <v>669</v>
-      </c>
-      <c r="C14" s="64" t="s">
-        <v>670</v>
-      </c>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="64"/>
-      <c r="J14" s="64"/>
-      <c r="K14" s="64"/>
-      <c r="L14" s="64"/>
-      <c r="M14" s="64"/>
-      <c r="N14" s="64"/>
-      <c r="O14" s="64"/>
-      <c r="P14" s="64"/>
-      <c r="Q14" s="64"/>
-      <c r="R14" s="64"/>
-      <c r="S14" s="64"/>
-      <c r="T14" s="64"/>
-      <c r="U14" s="64"/>
-      <c r="V14" s="64"/>
-      <c r="W14" s="64"/>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="64" t="s">
-        <v>662</v>
-      </c>
-      <c r="B15" s="64" t="s">
-        <v>671</v>
-      </c>
-      <c r="C15" s="64" t="s">
-        <v>672</v>
-      </c>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="64"/>
-      <c r="N15" s="64"/>
-      <c r="O15" s="64"/>
-      <c r="P15" s="64"/>
-      <c r="Q15" s="64"/>
-      <c r="R15" s="64"/>
-      <c r="S15" s="64"/>
-      <c r="T15" s="64"/>
-      <c r="U15" s="64"/>
-      <c r="V15" s="64"/>
-      <c r="W15" s="64"/>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="64" t="s">
-        <v>662</v>
-      </c>
-      <c r="B16" s="64" t="s">
-        <v>673</v>
-      </c>
-      <c r="C16" s="64" t="s">
-        <v>674</v>
-      </c>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="64"/>
-      <c r="I16" s="64"/>
-      <c r="J16" s="64"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="64"/>
-      <c r="M16" s="64"/>
-      <c r="N16" s="64"/>
-      <c r="O16" s="64"/>
-      <c r="P16" s="64"/>
-      <c r="Q16" s="64"/>
-      <c r="R16" s="64"/>
-      <c r="S16" s="64"/>
-      <c r="T16" s="64"/>
-      <c r="U16" s="64"/>
-      <c r="V16" s="64"/>
-      <c r="W16" s="64"/>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="64"/>
-      <c r="B17" s="64"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="64"/>
-      <c r="J17" s="64"/>
-      <c r="K17" s="64"/>
-      <c r="L17" s="64"/>
-      <c r="M17" s="64"/>
-      <c r="N17" s="64"/>
-      <c r="O17" s="64"/>
-      <c r="P17" s="64"/>
-      <c r="Q17" s="64"/>
-      <c r="R17" s="64"/>
-      <c r="S17" s="64"/>
-      <c r="T17" s="64"/>
-      <c r="U17" s="64"/>
-      <c r="V17" s="64"/>
-      <c r="W17" s="64"/>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="64" t="s">
-        <v>675</v>
-      </c>
-      <c r="B18" s="64" t="s">
-        <v>663</v>
-      </c>
-      <c r="C18" s="64" t="s">
-        <v>664</v>
-      </c>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="64"/>
-      <c r="L18" s="64"/>
-      <c r="M18" s="64"/>
-      <c r="N18" s="64"/>
-      <c r="O18" s="64"/>
-      <c r="P18" s="64"/>
-      <c r="Q18" s="64"/>
-      <c r="R18" s="64"/>
-      <c r="S18" s="64"/>
-      <c r="T18" s="64"/>
-      <c r="U18" s="64"/>
-      <c r="V18" s="64"/>
-      <c r="W18" s="64"/>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="64" t="s">
-        <v>675</v>
-      </c>
-      <c r="B19" s="64" t="s">
-        <v>665</v>
-      </c>
-      <c r="C19" s="64" t="s">
-        <v>666</v>
-      </c>
-      <c r="D19" s="64"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="64"/>
-      <c r="H19" s="64"/>
-      <c r="I19" s="64"/>
-      <c r="J19" s="64"/>
-      <c r="K19" s="64"/>
-      <c r="L19" s="64"/>
-      <c r="M19" s="64"/>
-      <c r="N19" s="64"/>
-      <c r="O19" s="64"/>
-      <c r="P19" s="64"/>
-      <c r="Q19" s="64"/>
-      <c r="R19" s="64"/>
-      <c r="S19" s="64"/>
-      <c r="T19" s="64"/>
-      <c r="U19" s="64"/>
-      <c r="V19" s="64"/>
-      <c r="W19" s="64"/>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="64" t="s">
-        <v>675</v>
-      </c>
-      <c r="B20" s="64" t="s">
-        <v>667</v>
-      </c>
-      <c r="C20" s="64" t="s">
-        <v>668</v>
-      </c>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
-      <c r="J20" s="64"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="64"/>
-      <c r="M20" s="64"/>
-      <c r="N20" s="64"/>
-      <c r="O20" s="64"/>
-      <c r="P20" s="64"/>
-      <c r="Q20" s="64"/>
-      <c r="R20" s="64"/>
-      <c r="S20" s="64"/>
-      <c r="T20" s="64"/>
-      <c r="U20" s="64"/>
-      <c r="V20" s="64"/>
-      <c r="W20" s="64"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="64" t="s">
-        <v>675</v>
-      </c>
-      <c r="B21" s="64" t="s">
-        <v>669</v>
-      </c>
-      <c r="C21" s="64" t="s">
-        <v>670</v>
-      </c>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="64"/>
-      <c r="J21" s="64"/>
-      <c r="K21" s="64"/>
-      <c r="L21" s="64"/>
-      <c r="M21" s="64"/>
-      <c r="N21" s="64"/>
-      <c r="O21" s="64"/>
-      <c r="P21" s="64"/>
-      <c r="Q21" s="64"/>
-      <c r="R21" s="64"/>
-      <c r="S21" s="64"/>
-      <c r="T21" s="64"/>
-      <c r="U21" s="64"/>
-      <c r="V21" s="64"/>
-      <c r="W21" s="64"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="64" t="s">
-        <v>675</v>
-      </c>
-      <c r="B22" s="64" t="s">
-        <v>673</v>
-      </c>
-      <c r="C22" s="64" t="s">
-        <v>674</v>
-      </c>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="64"/>
-      <c r="K22" s="64"/>
-      <c r="L22" s="64"/>
-      <c r="M22" s="64"/>
-      <c r="N22" s="64"/>
-      <c r="O22" s="64"/>
-      <c r="P22" s="64"/>
-      <c r="Q22" s="64"/>
-      <c r="R22" s="64"/>
-      <c r="S22" s="64"/>
-      <c r="T22" s="64"/>
-      <c r="U22" s="64"/>
-      <c r="V22" s="64"/>
-      <c r="W22" s="64"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="64" t="s">
-        <v>675</v>
-      </c>
-      <c r="B23" s="64" t="s">
-        <v>676</v>
-      </c>
-      <c r="C23" s="64" t="s">
-        <v>677</v>
-      </c>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="64"/>
-      <c r="J23" s="64"/>
-      <c r="K23" s="64"/>
-      <c r="L23" s="64"/>
-      <c r="M23" s="64"/>
-      <c r="N23" s="64"/>
-      <c r="O23" s="64"/>
-      <c r="P23" s="64"/>
-      <c r="Q23" s="64"/>
-      <c r="R23" s="64"/>
-      <c r="S23" s="64"/>
-      <c r="T23" s="64"/>
-      <c r="U23" s="64"/>
-      <c r="V23" s="64"/>
-      <c r="W23" s="64"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="64"/>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="64"/>
-      <c r="G24" s="64"/>
-      <c r="H24" s="64"/>
-      <c r="I24" s="64"/>
-      <c r="J24" s="64"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="64"/>
-      <c r="M24" s="64"/>
-      <c r="N24" s="64"/>
-      <c r="O24" s="64"/>
-      <c r="P24" s="64"/>
-      <c r="Q24" s="64"/>
-      <c r="R24" s="64"/>
-      <c r="S24" s="64"/>
-      <c r="T24" s="64"/>
-      <c r="U24" s="64"/>
-      <c r="V24" s="64"/>
-      <c r="W24" s="64"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="64" t="s">
-        <v>678</v>
-      </c>
-      <c r="B25" s="64" t="s">
-        <v>679</v>
-      </c>
-      <c r="C25" s="64" t="s">
-        <v>680</v>
-      </c>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="64"/>
-      <c r="H25" s="64"/>
-      <c r="I25" s="64"/>
-      <c r="J25" s="64"/>
-      <c r="K25" s="64"/>
-      <c r="L25" s="64"/>
-      <c r="M25" s="64"/>
-      <c r="N25" s="64"/>
-      <c r="O25" s="64"/>
-      <c r="P25" s="64"/>
-      <c r="Q25" s="64"/>
-      <c r="R25" s="64"/>
-      <c r="S25" s="64"/>
-      <c r="T25" s="64"/>
-      <c r="U25" s="64"/>
-      <c r="V25" s="64"/>
-      <c r="W25" s="64"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="64" t="s">
-        <v>678</v>
-      </c>
-      <c r="B26" s="64" t="s">
-        <v>681</v>
-      </c>
-      <c r="C26" s="64" t="s">
-        <v>682</v>
-      </c>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="64"/>
-      <c r="I26" s="64"/>
-      <c r="J26" s="64"/>
-      <c r="K26" s="64"/>
-      <c r="L26" s="64"/>
-      <c r="M26" s="64"/>
-      <c r="N26" s="64"/>
-      <c r="O26" s="64"/>
-      <c r="P26" s="64"/>
-      <c r="Q26" s="64"/>
-      <c r="R26" s="64"/>
-      <c r="S26" s="64"/>
-      <c r="T26" s="64"/>
-      <c r="U26" s="64"/>
-      <c r="V26" s="64"/>
-      <c r="W26" s="64"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="64" t="s">
-        <v>678</v>
-      </c>
-      <c r="B27" s="64" t="s">
-        <v>683</v>
-      </c>
-      <c r="C27" s="64" t="s">
-        <v>684</v>
-      </c>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="64"/>
-      <c r="I27" s="64"/>
-      <c r="J27" s="64"/>
-      <c r="K27" s="64"/>
-      <c r="L27" s="64"/>
-      <c r="M27" s="64"/>
-      <c r="N27" s="64"/>
-      <c r="O27" s="64"/>
-      <c r="P27" s="64"/>
-      <c r="Q27" s="64"/>
-      <c r="R27" s="64"/>
-      <c r="S27" s="64"/>
-      <c r="T27" s="64"/>
-      <c r="U27" s="64"/>
-      <c r="V27" s="64"/>
-      <c r="W27" s="64"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="64" t="s">
-        <v>678</v>
-      </c>
-      <c r="B28" s="64" t="s">
-        <v>685</v>
-      </c>
-      <c r="C28" s="64" t="s">
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="63"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="63"/>
+      <c r="K31" s="63"/>
+      <c r="L31" s="63"/>
+      <c r="M31" s="63"/>
+      <c r="N31" s="63"/>
+      <c r="O31" s="63"/>
+      <c r="P31" s="63"/>
+      <c r="Q31" s="63"/>
+      <c r="R31" s="63"/>
+      <c r="S31" s="63"/>
+      <c r="T31" s="63"/>
+      <c r="U31" s="63"/>
+      <c r="V31" s="63"/>
+      <c r="W31" s="63"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="63" t="s">
         <v>686</v>
       </c>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="64"/>
-      <c r="I28" s="64"/>
-      <c r="J28" s="64"/>
-      <c r="K28" s="64"/>
-      <c r="L28" s="64"/>
-      <c r="M28" s="64"/>
-      <c r="N28" s="64"/>
-      <c r="O28" s="64"/>
-      <c r="P28" s="64"/>
-      <c r="Q28" s="64"/>
-      <c r="R28" s="64"/>
-      <c r="S28" s="64"/>
-      <c r="T28" s="64"/>
-      <c r="U28" s="64"/>
-      <c r="V28" s="64"/>
-      <c r="W28" s="64"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="64" t="s">
-        <v>678</v>
-      </c>
-      <c r="B29" s="64" t="s">
-        <v>598</v>
-      </c>
-      <c r="C29" s="64" t="s">
-        <v>599</v>
-      </c>
-      <c r="D29" s="64"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="64"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="64"/>
-      <c r="I29" s="64"/>
-      <c r="J29" s="64"/>
-      <c r="K29" s="64"/>
-      <c r="L29" s="64"/>
-      <c r="M29" s="64"/>
-      <c r="N29" s="64"/>
-      <c r="O29" s="64"/>
-      <c r="P29" s="64"/>
-      <c r="Q29" s="64"/>
-      <c r="R29" s="64"/>
-      <c r="S29" s="64"/>
-      <c r="T29" s="64"/>
-      <c r="U29" s="64"/>
-      <c r="V29" s="64"/>
-      <c r="W29" s="64"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="64"/>
-      <c r="B30" s="64"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="64"/>
-      <c r="J30" s="64"/>
-      <c r="K30" s="64"/>
-      <c r="L30" s="64"/>
-      <c r="M30" s="64"/>
-      <c r="N30" s="64"/>
-      <c r="O30" s="64"/>
-      <c r="P30" s="64"/>
-      <c r="Q30" s="64"/>
-      <c r="R30" s="64"/>
-      <c r="S30" s="64"/>
-      <c r="T30" s="64"/>
-      <c r="U30" s="64"/>
-      <c r="V30" s="64"/>
-      <c r="W30" s="64"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="64" t="s">
-        <v>687</v>
-      </c>
-      <c r="B31" s="64" t="s">
+      <c r="B32" s="63" t="s">
         <v>688</v>
       </c>
-      <c r="C31" s="64" t="s">
+      <c r="C32" s="63" t="s">
         <v>586</v>
       </c>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="64"/>
-      <c r="I31" s="64"/>
-      <c r="J31" s="64"/>
-      <c r="K31" s="64"/>
-      <c r="L31" s="64"/>
-      <c r="M31" s="64"/>
-      <c r="N31" s="64"/>
-      <c r="O31" s="64"/>
-      <c r="P31" s="64"/>
-      <c r="Q31" s="64"/>
-      <c r="R31" s="64"/>
-      <c r="S31" s="64"/>
-      <c r="T31" s="64"/>
-      <c r="U31" s="64"/>
-      <c r="V31" s="64"/>
-      <c r="W31" s="64"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="64" t="s">
-        <v>687</v>
-      </c>
-      <c r="B32" s="64" t="s">
-        <v>689</v>
-      </c>
-      <c r="C32" s="64" t="s">
-        <v>587</v>
-      </c>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="64"/>
-      <c r="J32" s="64"/>
-      <c r="K32" s="64"/>
-      <c r="L32" s="64"/>
-      <c r="M32" s="64"/>
-      <c r="N32" s="64"/>
-      <c r="O32" s="64"/>
-      <c r="P32" s="64"/>
-      <c r="Q32" s="64"/>
-      <c r="R32" s="64"/>
-      <c r="S32" s="64"/>
-      <c r="T32" s="64"/>
-      <c r="U32" s="64"/>
-      <c r="V32" s="64"/>
-      <c r="W32" s="64"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="63"/>
+      <c r="O32" s="63"/>
+      <c r="P32" s="63"/>
+      <c r="Q32" s="63"/>
+      <c r="R32" s="63"/>
+      <c r="S32" s="63"/>
+      <c r="T32" s="63"/>
+      <c r="U32" s="63"/>
+      <c r="V32" s="63"/>
+      <c r="W32" s="63"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="64"/>
-      <c r="B33" s="64"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="64"/>
-      <c r="I33" s="64"/>
-      <c r="J33" s="64"/>
-      <c r="K33" s="64"/>
-      <c r="L33" s="64"/>
-      <c r="M33" s="64"/>
-      <c r="N33" s="64"/>
-      <c r="O33" s="64"/>
-      <c r="P33" s="64"/>
-      <c r="Q33" s="64"/>
-      <c r="R33" s="64"/>
-      <c r="S33" s="64"/>
-      <c r="T33" s="64"/>
-      <c r="U33" s="64"/>
-      <c r="V33" s="64"/>
-      <c r="W33" s="64"/>
+      <c r="A33" s="63"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="63"/>
+      <c r="M33" s="63"/>
+      <c r="N33" s="63"/>
+      <c r="O33" s="63"/>
+      <c r="P33" s="63"/>
+      <c r="Q33" s="63"/>
+      <c r="R33" s="63"/>
+      <c r="S33" s="63"/>
+      <c r="T33" s="63"/>
+      <c r="U33" s="63"/>
+      <c r="V33" s="63"/>
+      <c r="W33" s="63"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" ref="B34:B47" si="0">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C34, "(", ""), ")", "")), " ", "_")</f>
         <v>combined_oral_contraceptives</v>
       </c>
       <c r="C34" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
         <v>progesterone_only_pills</v>
       </c>
       <c r="C35" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
         <v>injectibles</v>
       </c>
       <c r="C36" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
         <v>implants_1_rod</v>
       </c>
       <c r="C37" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
         <v>implants_2_rods</v>
       </c>
       <c r="C38" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
         <v>iud</v>
       </c>
       <c r="C39" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
         <v>condoms</v>
       </c>
       <c r="C40" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
         <v>tubal_ligation</v>
       </c>
       <c r="C41" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>cycle_beads</v>
       </c>
       <c r="C42" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B43" t="s">
+        <v>597</v>
+      </c>
+      <c r="C43" t="s">
         <v>598</v>
-      </c>
-      <c r="C43" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -21809,26 +21783,26 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
         <v>wants_to_get_pregnant</v>
       </c>
       <c r="C45" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
         <v>did_not_want_fp</v>
       </c>
       <c r="C46" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -21838,25 +21812,25 @@
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="65" t="s">
+      <c r="A48" s="54" t="s">
+        <v>702</v>
+      </c>
+      <c r="B48" s="54" t="s">
         <v>703</v>
       </c>
-      <c r="B48" s="65" t="s">
+      <c r="C48" s="54" t="s">
         <v>704</v>
       </c>
-      <c r="C48" s="65" t="s">
-        <v>705</v>
-      </c>
-      <c r="D48" s="65"/>
-      <c r="E48" s="65"/>
-      <c r="F48" s="65"/>
-      <c r="G48" s="65"/>
-      <c r="H48" s="65"/>
-      <c r="I48" s="65"/>
-      <c r="J48" s="65"/>
-      <c r="K48" s="65"/>
-      <c r="L48" s="65"/>
-      <c r="M48" s="65"/>
+      <c r="D48" s="54"/>
+      <c r="E48" s="54"/>
+      <c r="F48" s="54"/>
+      <c r="G48" s="54"/>
+      <c r="H48" s="54"/>
+      <c r="I48" s="54"/>
+      <c r="J48" s="54"/>
+      <c r="K48" s="54"/>
+      <c r="L48" s="54"/>
+      <c r="M48" s="54"/>
       <c r="N48" s="55"/>
       <c r="O48" s="55"/>
       <c r="P48" s="55"/>
@@ -21869,25 +21843,25 @@
       <c r="W48" s="55"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="65" t="s">
-        <v>703</v>
-      </c>
-      <c r="B49" s="65" t="s">
+      <c r="A49" s="54" t="s">
+        <v>702</v>
+      </c>
+      <c r="B49" s="54" t="s">
+        <v>705</v>
+      </c>
+      <c r="C49" s="54" t="s">
         <v>706</v>
       </c>
-      <c r="C49" s="65" t="s">
-        <v>707</v>
-      </c>
-      <c r="D49" s="65"/>
-      <c r="E49" s="65"/>
-      <c r="F49" s="65"/>
-      <c r="G49" s="65"/>
-      <c r="H49" s="65"/>
-      <c r="I49" s="65"/>
-      <c r="J49" s="65"/>
-      <c r="K49" s="65"/>
-      <c r="L49" s="65"/>
-      <c r="M49" s="65"/>
+      <c r="D49" s="54"/>
+      <c r="E49" s="54"/>
+      <c r="F49" s="54"/>
+      <c r="G49" s="54"/>
+      <c r="H49" s="54"/>
+      <c r="I49" s="54"/>
+      <c r="J49" s="54"/>
+      <c r="K49" s="54"/>
+      <c r="L49" s="54"/>
+      <c r="M49" s="54"/>
       <c r="N49" s="55"/>
       <c r="O49" s="55"/>
       <c r="P49" s="55"/>
@@ -21901,222 +21875,222 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" t="s">
+        <v>707</v>
+      </c>
+      <c r="B51" t="s">
         <v>708</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>709</v>
-      </c>
-      <c r="C51" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B52" t="s">
+        <v>710</v>
+      </c>
+      <c r="C52" t="s">
         <v>711</v>
-      </c>
-      <c r="C52" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B53" t="s">
+        <v>712</v>
+      </c>
+      <c r="C53" t="s">
         <v>713</v>
-      </c>
-      <c r="C53" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B54" t="s">
+        <v>714</v>
+      </c>
+      <c r="C54" t="s">
         <v>715</v>
-      </c>
-      <c r="C54" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B55" t="s">
+        <v>716</v>
+      </c>
+      <c r="C55" t="s">
         <v>717</v>
-      </c>
-      <c r="C55" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B56" t="s">
+        <v>597</v>
+      </c>
+      <c r="C56" t="s">
         <v>598</v>
       </c>
-      <c r="C56" t="s">
-        <v>599</v>
-      </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="65" t="s">
+      <c r="A58" s="54" t="s">
+        <v>718</v>
+      </c>
+      <c r="B58" s="54" t="s">
         <v>719</v>
       </c>
-      <c r="B58" s="65" t="s">
+      <c r="C58" s="54" t="s">
         <v>720</v>
       </c>
-      <c r="C58" s="65" t="s">
+    </row>
+    <row r="59" ht="15.75" customHeight="1">
+      <c r="A59" s="54" t="s">
+        <v>718</v>
+      </c>
+      <c r="B59" s="54" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="65" t="s">
-        <v>719</v>
-      </c>
-      <c r="B59" s="65" t="s">
+      <c r="C59" s="54" t="s">
         <v>722</v>
       </c>
-      <c r="C59" s="65" t="s">
+    </row>
+    <row r="60" ht="15.75" customHeight="1">
+      <c r="A60" s="54" t="s">
+        <v>718</v>
+      </c>
+      <c r="B60" s="54" t="s">
         <v>723</v>
       </c>
-    </row>
-    <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="65" t="s">
-        <v>719</v>
-      </c>
-      <c r="B60" s="65" t="s">
+      <c r="C60" s="54" t="s">
         <v>724</v>
       </c>
-      <c r="C60" s="65" t="s">
-        <v>725</v>
-      </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="65" t="s">
-        <v>719</v>
-      </c>
-      <c r="B61" s="65" t="s">
+      <c r="A61" s="54" t="s">
+        <v>718</v>
+      </c>
+      <c r="B61" s="54" t="s">
+        <v>597</v>
+      </c>
+      <c r="C61" s="54" t="s">
         <v>598</v>
-      </c>
-      <c r="C61" s="65" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="55" t="s">
+        <v>725</v>
+      </c>
+      <c r="B63" s="55" t="s">
         <v>726</v>
       </c>
-      <c r="B63" s="55" t="s">
+      <c r="C63" s="54" t="s">
         <v>727</v>
-      </c>
-      <c r="C63" s="65" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="55" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B64" s="55" t="s">
+        <v>728</v>
+      </c>
+      <c r="C64" s="54" t="s">
         <v>729</v>
-      </c>
-      <c r="C64" s="65" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="55" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B65" s="55" t="s">
+        <v>730</v>
+      </c>
+      <c r="C65" s="54" t="s">
         <v>731</v>
-      </c>
-      <c r="C65" s="65" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="55" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B66" s="55" t="s">
+        <v>732</v>
+      </c>
+      <c r="C66" s="54" t="s">
         <v>733</v>
-      </c>
-      <c r="C66" s="65" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="55" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B67" s="55" t="s">
-        <v>627</v>
-      </c>
-      <c r="C67" s="65" t="s">
-        <v>633</v>
+        <v>626</v>
+      </c>
+      <c r="C67" s="54" t="s">
+        <v>632</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" t="s">
+        <v>734</v>
+      </c>
+      <c r="B69" t="s">
         <v>735</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>736</v>
-      </c>
-      <c r="C69" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B70" t="s">
+        <v>737</v>
+      </c>
+      <c r="C70" t="s">
         <v>738</v>
-      </c>
-      <c r="C70" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" t="s">
+        <v>739</v>
+      </c>
+      <c r="B72" t="s">
         <v>740</v>
       </c>
-      <c r="B72" t="s">
-        <v>741</v>
-      </c>
-      <c r="C72" s="66" t="s">
-        <v>701</v>
+      <c r="C72" s="64" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B73" t="s">
+        <v>741</v>
+      </c>
+      <c r="C73" t="s">
         <v>742</v>
-      </c>
-      <c r="C73" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B74" t="s">
+        <v>597</v>
+      </c>
+      <c r="C74" t="s">
         <v>598</v>
-      </c>
-      <c r="C74" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Update default app forms
</commit_message>
<xml_diff>
--- a/config/default/forms/app/delivery.xlsx
+++ b/config/default/forms/app/delivery.xlsx
@@ -439,7 +439,7 @@
     <t>t_danger_signs_referral_follow_up_date</t>
   </si>
   <si>
-    <t xml:space="preserve">date-time(floor(decimal-date-time(today())) + 3)</t>
+    <t xml:space="preserve">date-time(decimal-date-time(today()) + 3)</t>
   </si>
   <si>
     <t>condition</t>
@@ -540,7 +540,7 @@
     <t xml:space="preserve">Date of death</t>
   </si>
   <si>
-    <t xml:space="preserve">decimal-date-time(.) &lt;= decimal-date-time(today()) and difference-in-months( ., today() ) &lt; 1</t>
+    <t xml:space="preserve">. &lt;= now() and difference-in-months( ., today() ) &lt; 1</t>
   </si>
   <si>
     <t xml:space="preserve">Date cannot be in the future and older than a month from today.</t>
@@ -1268,7 +1268,7 @@
     <t>days</t>
   </si>
   <si>
-    <t xml:space="preserve">floor(decimal-date-time(today())) - floor(decimal-date-time(${delivery_date}))</t>
+    <t xml:space="preserve">floor(decimal-date-time(today()) - decimal-date-time(${delivery_date}))</t>
   </si>
   <si>
     <t>summary</t>
@@ -2834,7 +2834,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName=" " id="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}"/>
+  <person displayName=" " id="{6C409A6D-5981-1362-D5A6-271CC5B59A4E}"/>
 </personList>
 </file>
 
@@ -3250,7 +3250,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="U266" personId="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}" id="{0024000F-00D4-40FA-8C20-0081001200D2}" done="0">
+  <threadedComment ref="U266" personId="{6C409A6D-5981-1362-D5A6-271CC5B59A4E}" id="{0024000F-00D4-40FA-8C20-0081001200D2}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org is there a reason we are using .. instead of ${} for these? It would be more consistent if we could use $
 _Assigned to you_
 -Michael Kohn
@@ -3272,7 +3272,7 @@
 -Michael Kohn
 </text>
   </threadedComment>
-  <threadedComment ref="U294" personId="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}" id="{00800045-00BB-493D-B802-00C800B500C8}" done="0">
+  <threadedComment ref="U294" personId="{6C409A6D-5981-1362-D5A6-271CC5B59A4E}" id="{00800045-00BB-493D-B802-00C800B500C8}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org in some of the other forms i see this as ../../patient_id instead, not sure if it matters but feel like we should be consistent. I can update it based on your input. Also not sure why some of the ones below have ../../inputs and this one is ../inputs.
 _Assigned to you_
 -Michael Kohn
@@ -3285,7 +3285,7 @@
 -Michael Kohn
 </text>
   </threadedComment>
-  <threadedComment ref="U298" personId="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}" id="{00660081-00F5-41A0-8991-00C6004C00A7}" done="0">
+  <threadedComment ref="U298" personId="{6C409A6D-5981-1362-D5A6-271CC5B59A4E}" id="{00660081-00F5-41A0-8991-00C6004C00A7}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org in other forms there is a calculate field called pregnancy_uuid_ctx. To be consistent, it feels like we should either add that calculate field to this form and use that for this calculation, or update the other forms to use the "instance('contact-summary'......)" notation. I'd actually prefer to update the other forms to use the "instance('contact-summary'....)" notation because in general i was trying to avoid referencing those top level calculate fields in the data section (there are exceptions). Do you have a preference?
 _Assigned to you_
 -Michael Kohn
@@ -3295,7 +3295,7 @@
 -Marc Abbyad
 </text>
   </threadedComment>
-  <threadedComment ref="AI1" personId="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}" id="{00A000D4-0058-42D9-AAD4-004A00F70029}" done="0">
+  <threadedComment ref="AI1" personId="{6C409A6D-5981-1362-D5A6-271CC5B59A4E}" id="{00A000D4-0058-42D9-AAD4-004A00F70029}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org just FYI i moved these "instance" columns to be after the cht::notes column so that all forms have the same columns in the same order up to AH. Personally I'd probably prefer that all forms have the same exact columns in the same order, even if not all columns are needed for that form.
 _Assigned to you_
 -Michael Kohn
@@ -17196,7 +17196,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00D3006B-00A8-468D-95F7-00F200E000EE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00D9004A-00D4-491E-A903-0017004200C3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -17205,7 +17205,7 @@
           </x14:formula2>
           <xm:sqref>J2:J43 J45:J291 J293:J301</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00CF0043-0030-41D2-91B1-001F00DE0047}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00D4007B-00AB-4896-B480-005100E5007A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -20599,7 +20599,7 @@
       </c>
       <c r="C2" s="53" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-08-23 13-48</v>
+        <v xml:space="preserve">2022-09-26 12-11</v>
       </c>
       <c r="D2" s="54" t="s">
         <v>648</v>

</xml_diff>

<commit_message>
Remove custom today XPath function (#7821)
</commit_message>
<xml_diff>
--- a/config/default/forms/app/delivery.xlsx
+++ b/config/default/forms/app/delivery.xlsx
@@ -439,7 +439,7 @@
     <t>t_danger_signs_referral_follow_up_date</t>
   </si>
   <si>
-    <t xml:space="preserve">date-time(floor(decimal-date-time(today())) + 3)</t>
+    <t xml:space="preserve">date-time(decimal-date-time(today()) + 3)</t>
   </si>
   <si>
     <t>condition</t>
@@ -540,7 +540,7 @@
     <t xml:space="preserve">Date of death</t>
   </si>
   <si>
-    <t xml:space="preserve">decimal-date-time(.) &lt;= decimal-date-time(today()) and difference-in-months( ., today() ) &lt; 1</t>
+    <t xml:space="preserve">. &lt;= now() and difference-in-months( ., today() ) &lt; 1</t>
   </si>
   <si>
     <t xml:space="preserve">Date cannot be in the future and older than a month from today.</t>
@@ -1268,7 +1268,7 @@
     <t>days</t>
   </si>
   <si>
-    <t xml:space="preserve">floor(decimal-date-time(today())) - floor(decimal-date-time(${delivery_date}))</t>
+    <t xml:space="preserve">floor(decimal-date-time(today()) - decimal-date-time(${delivery_date}))</t>
   </si>
   <si>
     <t>summary</t>
@@ -2834,7 +2834,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName=" " id="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}"/>
+  <person displayName=" " id="{6C409A6D-5981-1362-D5A6-271CC5B59A4E}"/>
 </personList>
 </file>
 
@@ -3250,7 +3250,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="U266" personId="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}" id="{0024000F-00D4-40FA-8C20-0081001200D2}" done="0">
+  <threadedComment ref="U266" personId="{6C409A6D-5981-1362-D5A6-271CC5B59A4E}" id="{0024000F-00D4-40FA-8C20-0081001200D2}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org is there a reason we are using .. instead of ${} for these? It would be more consistent if we could use $
 _Assigned to you_
 -Michael Kohn
@@ -3272,7 +3272,7 @@
 -Michael Kohn
 </text>
   </threadedComment>
-  <threadedComment ref="U294" personId="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}" id="{00800045-00BB-493D-B802-00C800B500C8}" done="0">
+  <threadedComment ref="U294" personId="{6C409A6D-5981-1362-D5A6-271CC5B59A4E}" id="{00800045-00BB-493D-B802-00C800B500C8}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org in some of the other forms i see this as ../../patient_id instead, not sure if it matters but feel like we should be consistent. I can update it based on your input. Also not sure why some of the ones below have ../../inputs and this one is ../inputs.
 _Assigned to you_
 -Michael Kohn
@@ -3285,7 +3285,7 @@
 -Michael Kohn
 </text>
   </threadedComment>
-  <threadedComment ref="U298" personId="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}" id="{00660081-00F5-41A0-8991-00C6004C00A7}" done="0">
+  <threadedComment ref="U298" personId="{6C409A6D-5981-1362-D5A6-271CC5B59A4E}" id="{00660081-00F5-41A0-8991-00C6004C00A7}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org in other forms there is a calculate field called pregnancy_uuid_ctx. To be consistent, it feels like we should either add that calculate field to this form and use that for this calculation, or update the other forms to use the "instance('contact-summary'......)" notation. I'd actually prefer to update the other forms to use the "instance('contact-summary'....)" notation because in general i was trying to avoid referencing those top level calculate fields in the data section (there are exceptions). Do you have a preference?
 _Assigned to you_
 -Michael Kohn
@@ -3295,7 +3295,7 @@
 -Marc Abbyad
 </text>
   </threadedComment>
-  <threadedComment ref="AI1" personId="{4D87ED22-6D4B-FB2F-9760-400F6740D22E}" id="{00A000D4-0058-42D9-AAD4-004A00F70029}" done="0">
+  <threadedComment ref="AI1" personId="{6C409A6D-5981-1362-D5A6-271CC5B59A4E}" id="{00A000D4-0058-42D9-AAD4-004A00F70029}" done="0">
     <text xml:space="preserve">+marc@medicmobile.org just FYI i moved these "instance" columns to be after the cht::notes column so that all forms have the same columns in the same order up to AH. Personally I'd probably prefer that all forms have the same exact columns in the same order, even if not all columns are needed for that form.
 _Assigned to you_
 -Michael Kohn
@@ -17196,7 +17196,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00D3006B-00A8-468D-95F7-00F200E000EE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00D9004A-00D4-491E-A903-0017004200C3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"yes,no"</xm:f>
           </x14:formula1>
@@ -17205,7 +17205,7 @@
           </x14:formula2>
           <xm:sqref>J2:J43 J45:J291 J293:J301</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00CF0043-0030-41D2-91B1-001F00DE0047}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00D4007B-00AB-4896-B480-005100E5007A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</xm:f>
           </x14:formula1>
@@ -20599,7 +20599,7 @@
       </c>
       <c r="C2" s="53" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-08-23 13-48</v>
+        <v xml:space="preserve">2022-09-26 12-11</v>
       </c>
       <c r="D2" s="54" t="s">
         <v>648</v>

</xml_diff>

<commit_message>
Update default form to have "valid" child_count
</commit_message>
<xml_diff>
--- a/config/default/forms/app/delivery.xlsx
+++ b/config/default/forms/app/delivery.xlsx
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="742">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="741">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -1173,9 +1173,6 @@
   </si>
   <si>
     <t xml:space="preserve">child_doc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“”</t>
   </si>
   <si>
     <t xml:space="preserve">${baby_profile}</t>
@@ -3102,10 +3099,10 @@
   <dimension ref="A1:AJ301"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M173" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="N163" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="A173" activeCellId="0" sqref="A173"/>
+      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="bottomLeft" activeCell="A163" activeCellId="0" sqref="A163"/>
       <selection pane="bottomRight" activeCell="U191" activeCellId="0" sqref="U191"/>
     </sheetView>
   </sheetViews>
@@ -8832,7 +8829,7 @@
       <c r="S125" s="22"/>
       <c r="T125" s="22"/>
       <c r="U125" s="25" t="s">
-        <v>243</v>
+        <v>169</v>
       </c>
       <c r="V125" s="23"/>
       <c r="W125" s="22"/>
@@ -11833,7 +11830,7 @@
       <c r="AH190" s="23"/>
       <c r="AI190" s="23"/>
       <c r="AJ190" s="23" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11925,7 +11922,7 @@
         <v>74</v>
       </c>
       <c r="B193" s="21" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C193" s="22" t="s">
         <v>38</v>
@@ -11948,7 +11945,7 @@
       <c r="S193" s="22"/>
       <c r="T193" s="22"/>
       <c r="U193" s="22" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="V193" s="23"/>
       <c r="W193" s="22"/>
@@ -11971,7 +11968,7 @@
         <v>74</v>
       </c>
       <c r="B194" s="21" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C194" s="22" t="s">
         <v>38</v>
@@ -11994,7 +11991,7 @@
       <c r="S194" s="22"/>
       <c r="T194" s="22"/>
       <c r="U194" s="22" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="V194" s="23"/>
       <c r="W194" s="22"/>
@@ -12095,10 +12092,10 @@
         <v>36</v>
       </c>
       <c r="B197" s="21" t="s">
+        <v>337</v>
+      </c>
+      <c r="C197" s="22" t="s">
         <v>338</v>
-      </c>
-      <c r="C197" s="22" t="s">
-        <v>339</v>
       </c>
       <c r="D197" s="23"/>
       <c r="E197" s="23"/>
@@ -12111,7 +12108,7 @@
         <v>248</v>
       </c>
       <c r="L197" s="23" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M197" s="23"/>
       <c r="N197" s="22"/>
@@ -12145,10 +12142,10 @@
         <v>105</v>
       </c>
       <c r="B198" s="21" t="s">
+        <v>340</v>
+      </c>
+      <c r="C198" s="22" t="s">
         <v>341</v>
-      </c>
-      <c r="C198" s="22" t="s">
-        <v>342</v>
       </c>
       <c r="D198" s="23"/>
       <c r="E198" s="23"/>
@@ -12189,10 +12186,10 @@
         <v>105</v>
       </c>
       <c r="B199" s="21" t="s">
+        <v>342</v>
+      </c>
+      <c r="C199" s="22" t="s">
         <v>343</v>
-      </c>
-      <c r="C199" s="22" t="s">
-        <v>344</v>
       </c>
       <c r="D199" s="23"/>
       <c r="E199" s="23"/>
@@ -12233,10 +12230,10 @@
         <v>105</v>
       </c>
       <c r="B200" s="21" t="s">
+        <v>344</v>
+      </c>
+      <c r="C200" s="22" t="s">
         <v>345</v>
-      </c>
-      <c r="C200" s="22" t="s">
-        <v>346</v>
       </c>
       <c r="D200" s="23"/>
       <c r="E200" s="23"/>
@@ -12277,10 +12274,10 @@
         <v>105</v>
       </c>
       <c r="B201" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="C201" s="22" t="s">
         <v>347</v>
-      </c>
-      <c r="C201" s="22" t="s">
-        <v>348</v>
       </c>
       <c r="D201" s="23"/>
       <c r="E201" s="23"/>
@@ -12321,10 +12318,10 @@
         <v>105</v>
       </c>
       <c r="B202" s="21" t="s">
+        <v>348</v>
+      </c>
+      <c r="C202" s="22" t="s">
         <v>349</v>
-      </c>
-      <c r="C202" s="22" t="s">
-        <v>350</v>
       </c>
       <c r="D202" s="23"/>
       <c r="E202" s="23"/>
@@ -12443,10 +12440,10 @@
         <v>36</v>
       </c>
       <c r="B205" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="C205" s="22" t="s">
         <v>351</v>
-      </c>
-      <c r="C205" s="22" t="s">
-        <v>352</v>
       </c>
       <c r="D205" s="23"/>
       <c r="E205" s="23"/>
@@ -12456,7 +12453,7 @@
       <c r="I205" s="23"/>
       <c r="J205" s="23"/>
       <c r="K205" s="22" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L205" s="23" t="s">
         <v>40</v>
@@ -12491,10 +12488,10 @@
         <v>105</v>
       </c>
       <c r="B206" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="C206" s="22" t="s">
         <v>354</v>
-      </c>
-      <c r="C206" s="22" t="s">
-        <v>355</v>
       </c>
       <c r="D206" s="23"/>
       <c r="E206" s="23"/>
@@ -12534,13 +12531,13 @@
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A207" s="21" t="s">
+        <v>355</v>
+      </c>
+      <c r="B207" s="21" t="s">
         <v>356</v>
       </c>
-      <c r="B207" s="21" t="s">
+      <c r="C207" s="22" t="s">
         <v>357</v>
-      </c>
-      <c r="C207" s="22" t="s">
-        <v>358</v>
       </c>
       <c r="D207" s="23"/>
       <c r="E207" s="23"/>
@@ -12554,7 +12551,7 @@
       <c r="K207" s="23"/>
       <c r="L207" s="23"/>
       <c r="M207" s="23" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="N207" s="23"/>
       <c r="O207" s="22"/>
@@ -12565,7 +12562,7 @@
       <c r="T207" s="22"/>
       <c r="U207" s="22"/>
       <c r="V207" s="22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="W207" s="22"/>
       <c r="X207" s="23"/>
@@ -12587,10 +12584,10 @@
         <v>179</v>
       </c>
       <c r="B208" s="21" t="s">
+        <v>360</v>
+      </c>
+      <c r="C208" s="22" t="s">
         <v>361</v>
-      </c>
-      <c r="C208" s="22" t="s">
-        <v>362</v>
       </c>
       <c r="D208" s="23"/>
       <c r="E208" s="23"/>
@@ -12604,10 +12601,10 @@
       <c r="K208" s="23"/>
       <c r="L208" s="22"/>
       <c r="M208" s="23" t="s">
+        <v>362</v>
+      </c>
+      <c r="N208" s="22" t="s">
         <v>363</v>
-      </c>
-      <c r="N208" s="22" t="s">
-        <v>364</v>
       </c>
       <c r="O208" s="23"/>
       <c r="P208" s="23"/>
@@ -12637,7 +12634,7 @@
         <v>74</v>
       </c>
       <c r="B209" s="21" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C209" s="22" t="s">
         <v>38</v>
@@ -12660,7 +12657,7 @@
       <c r="S209" s="23"/>
       <c r="T209" s="23"/>
       <c r="U209" s="23" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="V209" s="23"/>
       <c r="W209" s="23"/>
@@ -12763,7 +12760,7 @@
         <v>36</v>
       </c>
       <c r="B212" s="31" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C212" s="32" t="s">
         <v>38</v>
@@ -12777,7 +12774,7 @@
       <c r="J212" s="33"/>
       <c r="K212" s="33"/>
       <c r="L212" s="33" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M212" s="33"/>
       <c r="N212" s="32"/>
@@ -12811,10 +12808,10 @@
         <v>105</v>
       </c>
       <c r="B213" s="34" t="s">
+        <v>367</v>
+      </c>
+      <c r="C213" s="32" t="s">
         <v>368</v>
-      </c>
-      <c r="C213" s="32" t="s">
-        <v>369</v>
       </c>
       <c r="D213" s="33"/>
       <c r="E213" s="33"/>
@@ -12855,10 +12852,10 @@
         <v>105</v>
       </c>
       <c r="B214" s="31" t="s">
+        <v>369</v>
+      </c>
+      <c r="C214" s="32" t="s">
         <v>370</v>
-      </c>
-      <c r="C214" s="32" t="s">
-        <v>371</v>
       </c>
       <c r="D214" s="33"/>
       <c r="E214" s="33"/>
@@ -12869,7 +12866,7 @@
       <c r="J214" s="33"/>
       <c r="K214" s="33"/>
       <c r="L214" s="32" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="M214" s="33"/>
       <c r="N214" s="33"/>
@@ -12901,10 +12898,10 @@
         <v>105</v>
       </c>
       <c r="B215" s="31" t="s">
+        <v>372</v>
+      </c>
+      <c r="C215" s="32" t="s">
         <v>373</v>
-      </c>
-      <c r="C215" s="32" t="s">
-        <v>374</v>
       </c>
       <c r="D215" s="33"/>
       <c r="E215" s="33"/>
@@ -12945,10 +12942,10 @@
         <v>105</v>
       </c>
       <c r="B216" s="31" t="s">
+        <v>374</v>
+      </c>
+      <c r="C216" s="32" t="s">
         <v>375</v>
-      </c>
-      <c r="C216" s="32" t="s">
-        <v>376</v>
       </c>
       <c r="D216" s="33"/>
       <c r="E216" s="33"/>
@@ -12959,7 +12956,7 @@
       <c r="J216" s="33"/>
       <c r="K216" s="33"/>
       <c r="L216" s="32" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="M216" s="33"/>
       <c r="N216" s="33"/>
@@ -12991,10 +12988,10 @@
         <v>105</v>
       </c>
       <c r="B217" s="31" t="s">
+        <v>376</v>
+      </c>
+      <c r="C217" s="33" t="s">
         <v>377</v>
-      </c>
-      <c r="C217" s="33" t="s">
-        <v>378</v>
       </c>
       <c r="D217" s="33"/>
       <c r="E217" s="33"/>
@@ -13005,7 +13002,7 @@
       <c r="J217" s="33"/>
       <c r="K217" s="33"/>
       <c r="L217" s="32" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="M217" s="33"/>
       <c r="N217" s="33"/>
@@ -13037,10 +13034,10 @@
         <v>105</v>
       </c>
       <c r="B218" s="31" t="s">
+        <v>379</v>
+      </c>
+      <c r="C218" s="32" t="s">
         <v>380</v>
-      </c>
-      <c r="C218" s="32" t="s">
-        <v>381</v>
       </c>
       <c r="D218" s="33"/>
       <c r="E218" s="33"/>
@@ -13050,10 +13047,10 @@
       <c r="I218" s="33"/>
       <c r="J218" s="33"/>
       <c r="K218" s="32" t="s">
+        <v>381</v>
+      </c>
+      <c r="L218" s="33" t="s">
         <v>382</v>
-      </c>
-      <c r="L218" s="33" t="s">
-        <v>383</v>
       </c>
       <c r="M218" s="33"/>
       <c r="N218" s="32"/>
@@ -13085,10 +13082,10 @@
         <v>105</v>
       </c>
       <c r="B219" s="31" t="s">
+        <v>383</v>
+      </c>
+      <c r="C219" s="32" t="s">
         <v>384</v>
-      </c>
-      <c r="C219" s="32" t="s">
-        <v>385</v>
       </c>
       <c r="D219" s="33"/>
       <c r="E219" s="33"/>
@@ -13098,10 +13095,10 @@
       <c r="I219" s="33"/>
       <c r="J219" s="33"/>
       <c r="K219" s="32" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="L219" s="33" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M219" s="33"/>
       <c r="N219" s="32"/>
@@ -13133,10 +13130,10 @@
         <v>105</v>
       </c>
       <c r="B220" s="31" t="s">
+        <v>386</v>
+      </c>
+      <c r="C220" s="32" t="s">
         <v>387</v>
-      </c>
-      <c r="C220" s="32" t="s">
-        <v>388</v>
       </c>
       <c r="D220" s="33"/>
       <c r="E220" s="33"/>
@@ -13146,10 +13143,10 @@
       <c r="I220" s="33"/>
       <c r="J220" s="33"/>
       <c r="K220" s="32" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L220" s="33" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M220" s="33"/>
       <c r="N220" s="32"/>
@@ -13181,10 +13178,10 @@
         <v>105</v>
       </c>
       <c r="B221" s="31" t="s">
+        <v>389</v>
+      </c>
+      <c r="C221" s="33" t="s">
         <v>390</v>
-      </c>
-      <c r="C221" s="33" t="s">
-        <v>391</v>
       </c>
       <c r="D221" s="33"/>
       <c r="E221" s="33"/>
@@ -13194,10 +13191,10 @@
       <c r="I221" s="33"/>
       <c r="J221" s="33"/>
       <c r="K221" s="32" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L221" s="32" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="M221" s="33"/>
       <c r="N221" s="33"/>
@@ -13229,10 +13226,10 @@
         <v>105</v>
       </c>
       <c r="B222" s="31" t="s">
+        <v>391</v>
+      </c>
+      <c r="C222" s="32" t="s">
         <v>392</v>
-      </c>
-      <c r="C222" s="32" t="s">
-        <v>393</v>
       </c>
       <c r="D222" s="33"/>
       <c r="E222" s="33"/>
@@ -13242,10 +13239,10 @@
       <c r="I222" s="33"/>
       <c r="J222" s="33"/>
       <c r="K222" s="32" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L222" s="33" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M222" s="33"/>
       <c r="N222" s="32"/>
@@ -13277,10 +13274,10 @@
         <v>105</v>
       </c>
       <c r="B223" s="31" t="s">
+        <v>393</v>
+      </c>
+      <c r="C223" s="32" t="s">
         <v>394</v>
-      </c>
-      <c r="C223" s="32" t="s">
-        <v>395</v>
       </c>
       <c r="D223" s="33"/>
       <c r="E223" s="33"/>
@@ -13290,10 +13287,10 @@
       <c r="I223" s="33"/>
       <c r="J223" s="33"/>
       <c r="K223" s="32" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L223" s="33" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M223" s="33"/>
       <c r="N223" s="32"/>
@@ -13325,10 +13322,10 @@
         <v>105</v>
       </c>
       <c r="B224" s="31" t="s">
+        <v>395</v>
+      </c>
+      <c r="C224" s="33" t="s">
         <v>396</v>
-      </c>
-      <c r="C224" s="33" t="s">
-        <v>397</v>
       </c>
       <c r="D224" s="33"/>
       <c r="E224" s="33"/>
@@ -13338,10 +13335,10 @@
       <c r="I224" s="33"/>
       <c r="J224" s="33"/>
       <c r="K224" s="32" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="L224" s="32" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="M224" s="33"/>
       <c r="N224" s="33"/>
@@ -13373,10 +13370,10 @@
         <v>105</v>
       </c>
       <c r="B225" s="31" t="s">
+        <v>398</v>
+      </c>
+      <c r="C225" s="32" t="s">
         <v>399</v>
-      </c>
-      <c r="C225" s="32" t="s">
-        <v>400</v>
       </c>
       <c r="D225" s="33"/>
       <c r="E225" s="33"/>
@@ -13386,10 +13383,10 @@
       <c r="I225" s="33"/>
       <c r="J225" s="33"/>
       <c r="K225" s="33" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="L225" s="33" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M225" s="33"/>
       <c r="N225" s="32"/>
@@ -13421,10 +13418,10 @@
         <v>105</v>
       </c>
       <c r="B226" s="31" t="s">
+        <v>401</v>
+      </c>
+      <c r="C226" s="32" t="s">
         <v>402</v>
-      </c>
-      <c r="C226" s="32" t="s">
-        <v>403</v>
       </c>
       <c r="D226" s="33"/>
       <c r="E226" s="33"/>
@@ -13434,10 +13431,10 @@
       <c r="I226" s="33"/>
       <c r="J226" s="33"/>
       <c r="K226" s="33" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="L226" s="33" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M226" s="33"/>
       <c r="N226" s="32"/>
@@ -13469,10 +13466,10 @@
         <v>105</v>
       </c>
       <c r="B227" s="31" t="s">
+        <v>404</v>
+      </c>
+      <c r="C227" s="32" t="s">
         <v>405</v>
-      </c>
-      <c r="C227" s="32" t="s">
-        <v>406</v>
       </c>
       <c r="D227" s="33"/>
       <c r="E227" s="33"/>
@@ -13482,10 +13479,10 @@
       <c r="I227" s="33"/>
       <c r="J227" s="33"/>
       <c r="K227" s="33" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="L227" s="33" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M227" s="33"/>
       <c r="N227" s="32"/>
@@ -13517,10 +13514,10 @@
         <v>105</v>
       </c>
       <c r="B228" s="31" t="s">
+        <v>407</v>
+      </c>
+      <c r="C228" s="32" t="s">
         <v>408</v>
-      </c>
-      <c r="C228" s="32" t="s">
-        <v>409</v>
       </c>
       <c r="D228" s="33"/>
       <c r="E228" s="33"/>
@@ -13530,10 +13527,10 @@
       <c r="I228" s="33"/>
       <c r="J228" s="33"/>
       <c r="K228" s="33" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="L228" s="33" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M228" s="33"/>
       <c r="N228" s="32"/>
@@ -13565,10 +13562,10 @@
         <v>105</v>
       </c>
       <c r="B229" s="31" t="s">
+        <v>410</v>
+      </c>
+      <c r="C229" s="32" t="s">
         <v>411</v>
-      </c>
-      <c r="C229" s="32" t="s">
-        <v>412</v>
       </c>
       <c r="D229" s="33"/>
       <c r="E229" s="33"/>
@@ -13578,10 +13575,10 @@
       <c r="I229" s="33"/>
       <c r="J229" s="33"/>
       <c r="K229" s="32" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L229" s="32" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="M229" s="33"/>
       <c r="N229" s="32"/>
@@ -13613,7 +13610,7 @@
         <v>105</v>
       </c>
       <c r="B230" s="31" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C230" s="32" t="s">
         <v>110</v>
@@ -13626,10 +13623,10 @@
       <c r="I230" s="33"/>
       <c r="J230" s="33"/>
       <c r="K230" s="32" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="L230" s="32" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M230" s="33"/>
       <c r="N230" s="33"/>
@@ -13661,7 +13658,7 @@
         <v>105</v>
       </c>
       <c r="B231" s="31" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C231" s="32" t="s">
         <v>112</v>
@@ -13674,10 +13671,10 @@
       <c r="I231" s="33"/>
       <c r="J231" s="33"/>
       <c r="K231" s="32" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L231" s="32" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M231" s="33"/>
       <c r="N231" s="33"/>
@@ -13709,7 +13706,7 @@
         <v>105</v>
       </c>
       <c r="B232" s="31" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C232" s="32" t="s">
         <v>114</v>
@@ -13722,10 +13719,10 @@
       <c r="I232" s="33"/>
       <c r="J232" s="33"/>
       <c r="K232" s="32" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="L232" s="32" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M232" s="33"/>
       <c r="N232" s="33"/>
@@ -13757,7 +13754,7 @@
         <v>105</v>
       </c>
       <c r="B233" s="31" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C233" s="32" t="s">
         <v>116</v>
@@ -13770,10 +13767,10 @@
       <c r="I233" s="33"/>
       <c r="J233" s="33"/>
       <c r="K233" s="32" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="L233" s="32" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M233" s="33"/>
       <c r="N233" s="33"/>
@@ -13805,7 +13802,7 @@
         <v>105</v>
       </c>
       <c r="B234" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C234" s="32" t="s">
         <v>118</v>
@@ -13818,10 +13815,10 @@
       <c r="I234" s="33"/>
       <c r="J234" s="33"/>
       <c r="K234" s="32" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L234" s="32" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M234" s="33"/>
       <c r="N234" s="33"/>
@@ -13853,10 +13850,10 @@
         <v>105</v>
       </c>
       <c r="B235" s="31" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C235" s="32" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D235" s="33"/>
       <c r="E235" s="33"/>
@@ -13866,10 +13863,10 @@
       <c r="I235" s="33"/>
       <c r="J235" s="33"/>
       <c r="K235" s="32" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="L235" s="32" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="M235" s="33"/>
       <c r="N235" s="33"/>
@@ -13901,10 +13898,10 @@
         <v>105</v>
       </c>
       <c r="B236" s="31" t="s">
+        <v>425</v>
+      </c>
+      <c r="C236" s="32" t="s">
         <v>426</v>
-      </c>
-      <c r="C236" s="32" t="s">
-        <v>427</v>
       </c>
       <c r="D236" s="33"/>
       <c r="E236" s="33"/>
@@ -13914,7 +13911,7 @@
       <c r="I236" s="33"/>
       <c r="J236" s="33"/>
       <c r="K236" s="32" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="L236" s="33"/>
       <c r="M236" s="33"/>
@@ -13947,10 +13944,10 @@
         <v>105</v>
       </c>
       <c r="B237" s="31" t="s">
+        <v>427</v>
+      </c>
+      <c r="C237" s="32" t="s">
         <v>428</v>
-      </c>
-      <c r="C237" s="32" t="s">
-        <v>429</v>
       </c>
       <c r="D237" s="33"/>
       <c r="E237" s="33"/>
@@ -13960,10 +13957,10 @@
       <c r="I237" s="33"/>
       <c r="J237" s="33"/>
       <c r="K237" s="33" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="L237" s="33" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M237" s="33"/>
       <c r="N237" s="32"/>
@@ -13995,10 +13992,10 @@
         <v>105</v>
       </c>
       <c r="B238" s="31" t="s">
+        <v>430</v>
+      </c>
+      <c r="C238" s="32" t="s">
         <v>431</v>
-      </c>
-      <c r="C238" s="32" t="s">
-        <v>432</v>
       </c>
       <c r="D238" s="33"/>
       <c r="E238" s="33"/>
@@ -14008,10 +14005,10 @@
       <c r="I238" s="33"/>
       <c r="J238" s="33"/>
       <c r="K238" s="33" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="L238" s="33" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M238" s="33"/>
       <c r="N238" s="32"/>
@@ -14043,10 +14040,10 @@
         <v>105</v>
       </c>
       <c r="B239" s="31" t="s">
+        <v>433</v>
+      </c>
+      <c r="C239" s="32" t="s">
         <v>434</v>
-      </c>
-      <c r="C239" s="32" t="s">
-        <v>435</v>
       </c>
       <c r="D239" s="33"/>
       <c r="E239" s="33"/>
@@ -14056,10 +14053,10 @@
       <c r="I239" s="33"/>
       <c r="J239" s="33"/>
       <c r="K239" s="33" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="L239" s="33" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M239" s="33"/>
       <c r="N239" s="32"/>
@@ -14091,10 +14088,10 @@
         <v>105</v>
       </c>
       <c r="B240" s="31" t="s">
+        <v>436</v>
+      </c>
+      <c r="C240" s="32" t="s">
         <v>437</v>
-      </c>
-      <c r="C240" s="32" t="s">
-        <v>438</v>
       </c>
       <c r="D240" s="33"/>
       <c r="E240" s="33"/>
@@ -14104,10 +14101,10 @@
       <c r="I240" s="33"/>
       <c r="J240" s="33"/>
       <c r="K240" s="33" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L240" s="33" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M240" s="33"/>
       <c r="N240" s="32"/>
@@ -14139,10 +14136,10 @@
         <v>105</v>
       </c>
       <c r="B241" s="31" t="s">
+        <v>439</v>
+      </c>
+      <c r="C241" s="32" t="s">
         <v>440</v>
-      </c>
-      <c r="C241" s="32" t="s">
-        <v>441</v>
       </c>
       <c r="D241" s="33"/>
       <c r="E241" s="33"/>
@@ -14152,10 +14149,10 @@
       <c r="I241" s="33"/>
       <c r="J241" s="33"/>
       <c r="K241" s="32" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="L241" s="33" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M241" s="33"/>
       <c r="N241" s="32"/>
@@ -14187,10 +14184,10 @@
         <v>105</v>
       </c>
       <c r="B242" s="31" t="s">
+        <v>442</v>
+      </c>
+      <c r="C242" s="32" t="s">
         <v>443</v>
-      </c>
-      <c r="C242" s="32" t="s">
-        <v>444</v>
       </c>
       <c r="D242" s="33"/>
       <c r="E242" s="33"/>
@@ -14200,7 +14197,7 @@
       <c r="I242" s="33"/>
       <c r="J242" s="33"/>
       <c r="K242" s="33" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="L242" s="33"/>
       <c r="M242" s="33"/>
@@ -14233,10 +14230,10 @@
         <v>105</v>
       </c>
       <c r="B243" s="31" t="s">
+        <v>445</v>
+      </c>
+      <c r="C243" s="32" t="s">
         <v>446</v>
-      </c>
-      <c r="C243" s="32" t="s">
-        <v>447</v>
       </c>
       <c r="D243" s="33"/>
       <c r="E243" s="33"/>
@@ -14246,10 +14243,10 @@
       <c r="I243" s="33"/>
       <c r="J243" s="33"/>
       <c r="K243" s="32" t="s">
+        <v>447</v>
+      </c>
+      <c r="L243" s="32" t="s">
         <v>448</v>
-      </c>
-      <c r="L243" s="32" t="s">
-        <v>449</v>
       </c>
       <c r="M243" s="33"/>
       <c r="N243" s="33"/>
@@ -14281,10 +14278,10 @@
         <v>105</v>
       </c>
       <c r="B244" s="31" t="s">
+        <v>449</v>
+      </c>
+      <c r="C244" s="32" t="s">
         <v>450</v>
-      </c>
-      <c r="C244" s="32" t="s">
-        <v>451</v>
       </c>
       <c r="D244" s="33"/>
       <c r="E244" s="33"/>
@@ -14294,7 +14291,7 @@
       <c r="I244" s="33"/>
       <c r="J244" s="33"/>
       <c r="K244" s="32" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="L244" s="32"/>
       <c r="M244" s="33"/>
@@ -14327,10 +14324,10 @@
         <v>105</v>
       </c>
       <c r="B245" s="31" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C245" s="32" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D245" s="33"/>
       <c r="E245" s="33"/>
@@ -14340,10 +14337,10 @@
       <c r="I245" s="33"/>
       <c r="J245" s="33"/>
       <c r="K245" s="32" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L245" s="32" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M245" s="33"/>
       <c r="N245" s="33"/>
@@ -14375,10 +14372,10 @@
         <v>105</v>
       </c>
       <c r="B246" s="31" t="s">
+        <v>453</v>
+      </c>
+      <c r="C246" s="32" t="s">
         <v>454</v>
-      </c>
-      <c r="C246" s="32" t="s">
-        <v>455</v>
       </c>
       <c r="D246" s="33"/>
       <c r="E246" s="33"/>
@@ -14388,10 +14385,10 @@
       <c r="I246" s="33"/>
       <c r="J246" s="33"/>
       <c r="K246" s="32" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="L246" s="33" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M246" s="33"/>
       <c r="N246" s="32"/>
@@ -14423,10 +14420,10 @@
         <v>105</v>
       </c>
       <c r="B247" s="31" t="s">
+        <v>455</v>
+      </c>
+      <c r="C247" s="32" t="s">
         <v>456</v>
-      </c>
-      <c r="C247" s="32" t="s">
-        <v>457</v>
       </c>
       <c r="D247" s="33"/>
       <c r="E247" s="33"/>
@@ -14436,7 +14433,7 @@
       <c r="I247" s="33"/>
       <c r="J247" s="33"/>
       <c r="K247" s="32" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="L247" s="33"/>
       <c r="M247" s="33"/>
@@ -14469,10 +14466,10 @@
         <v>105</v>
       </c>
       <c r="B248" s="31" t="s">
+        <v>457</v>
+      </c>
+      <c r="C248" s="32" t="s">
         <v>458</v>
-      </c>
-      <c r="C248" s="32" t="s">
-        <v>459</v>
       </c>
       <c r="D248" s="33"/>
       <c r="E248" s="33"/>
@@ -14482,7 +14479,7 @@
       <c r="I248" s="33"/>
       <c r="J248" s="33"/>
       <c r="K248" s="32" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="L248" s="33"/>
       <c r="M248" s="33"/>
@@ -14515,10 +14512,10 @@
         <v>105</v>
       </c>
       <c r="B249" s="31" t="s">
+        <v>459</v>
+      </c>
+      <c r="C249" s="32" t="s">
         <v>460</v>
-      </c>
-      <c r="C249" s="32" t="s">
-        <v>461</v>
       </c>
       <c r="D249" s="33"/>
       <c r="E249" s="33"/>
@@ -14528,10 +14525,10 @@
       <c r="I249" s="33"/>
       <c r="J249" s="33"/>
       <c r="K249" s="32" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L249" s="32" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="M249" s="33"/>
       <c r="N249" s="33"/>
@@ -14563,10 +14560,10 @@
         <v>105</v>
       </c>
       <c r="B250" s="31" t="s">
+        <v>462</v>
+      </c>
+      <c r="C250" s="32" t="s">
         <v>463</v>
-      </c>
-      <c r="C250" s="32" t="s">
-        <v>464</v>
       </c>
       <c r="D250" s="33"/>
       <c r="E250" s="33"/>
@@ -14576,7 +14573,7 @@
       <c r="I250" s="33"/>
       <c r="J250" s="33"/>
       <c r="K250" s="32" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L250" s="32"/>
       <c r="M250" s="33"/>
@@ -14609,10 +14606,10 @@
         <v>105</v>
       </c>
       <c r="B251" s="31" t="s">
+        <v>464</v>
+      </c>
+      <c r="C251" s="32" t="s">
         <v>465</v>
-      </c>
-      <c r="C251" s="32" t="s">
-        <v>466</v>
       </c>
       <c r="D251" s="33"/>
       <c r="E251" s="33"/>
@@ -14622,7 +14619,7 @@
       <c r="I251" s="33"/>
       <c r="J251" s="33"/>
       <c r="K251" s="32" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L251" s="32"/>
       <c r="M251" s="33"/>
@@ -14655,10 +14652,10 @@
         <v>105</v>
       </c>
       <c r="B252" s="31" t="s">
+        <v>466</v>
+      </c>
+      <c r="C252" s="32" t="s">
         <v>467</v>
-      </c>
-      <c r="C252" s="32" t="s">
-        <v>468</v>
       </c>
       <c r="D252" s="33"/>
       <c r="E252" s="33"/>
@@ -14668,7 +14665,7 @@
       <c r="I252" s="33"/>
       <c r="J252" s="33"/>
       <c r="K252" s="32" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="L252" s="32"/>
       <c r="M252" s="33"/>
@@ -14701,7 +14698,7 @@
         <v>36</v>
       </c>
       <c r="B253" s="31" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C253" s="32" t="s">
         <v>38</v>
@@ -14746,10 +14743,10 @@
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A254" s="31" t="s">
+        <v>470</v>
+      </c>
+      <c r="B254" s="31" t="s">
         <v>471</v>
-      </c>
-      <c r="B254" s="31" t="s">
-        <v>472</v>
       </c>
       <c r="C254" s="32" t="s">
         <v>38</v>
@@ -14772,7 +14769,7 @@
       <c r="S254" s="32"/>
       <c r="T254" s="32"/>
       <c r="U254" s="32" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="V254" s="33"/>
       <c r="W254" s="32"/>
@@ -14795,7 +14792,7 @@
         <v>74</v>
       </c>
       <c r="B255" s="31" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C255" s="32" t="s">
         <v>38</v>
@@ -14818,7 +14815,7 @@
       <c r="S255" s="32"/>
       <c r="T255" s="32"/>
       <c r="U255" s="32" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="V255" s="33"/>
       <c r="W255" s="32"/>
@@ -14838,10 +14835,10 @@
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A256" s="31" t="s">
+        <v>475</v>
+      </c>
+      <c r="B256" s="31" t="s">
         <v>476</v>
-      </c>
-      <c r="B256" s="31" t="s">
-        <v>477</v>
       </c>
       <c r="C256" s="32" t="s">
         <v>38</v>
@@ -14864,7 +14861,7 @@
       <c r="S256" s="32"/>
       <c r="T256" s="32"/>
       <c r="U256" s="32" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="V256" s="33"/>
       <c r="W256" s="32"/>
@@ -14887,7 +14884,7 @@
         <v>74</v>
       </c>
       <c r="B257" s="31" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C257" s="32" t="s">
         <v>38</v>
@@ -14910,7 +14907,7 @@
       <c r="S257" s="32"/>
       <c r="T257" s="32"/>
       <c r="U257" s="32" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="V257" s="33"/>
       <c r="W257" s="32"/>
@@ -14933,7 +14930,7 @@
         <v>129</v>
       </c>
       <c r="B258" s="31" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C258" s="32" t="s">
         <v>38</v>
@@ -14956,7 +14953,7 @@
       <c r="S258" s="33"/>
       <c r="T258" s="33"/>
       <c r="U258" s="32" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="V258" s="33"/>
       <c r="W258" s="33"/>
@@ -14979,7 +14976,7 @@
         <v>74</v>
       </c>
       <c r="B259" s="31" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C259" s="32" t="s">
         <v>38</v>
@@ -15002,7 +14999,7 @@
       <c r="S259" s="33"/>
       <c r="T259" s="33"/>
       <c r="U259" s="32" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="V259" s="33"/>
       <c r="W259" s="33"/>
@@ -15025,7 +15022,7 @@
         <v>129</v>
       </c>
       <c r="B260" s="31" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C260" s="32" t="s">
         <v>38</v>
@@ -15048,7 +15045,7 @@
       <c r="S260" s="33"/>
       <c r="T260" s="33"/>
       <c r="U260" s="32" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="V260" s="33"/>
       <c r="W260" s="33"/>
@@ -15071,7 +15068,7 @@
         <v>74</v>
       </c>
       <c r="B261" s="31" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C261" s="32" t="s">
         <v>38</v>
@@ -15094,7 +15091,7 @@
       <c r="S261" s="33"/>
       <c r="T261" s="33"/>
       <c r="U261" s="32" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="V261" s="33"/>
       <c r="W261" s="33"/>
@@ -15235,7 +15232,7 @@
         <v>36</v>
       </c>
       <c r="B265" s="35" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C265" s="36" t="s">
         <v>38</v>
@@ -15283,7 +15280,7 @@
         <v>74</v>
       </c>
       <c r="B266" s="35" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C266" s="42" t="s">
         <v>38</v>
@@ -15306,7 +15303,7 @@
       <c r="S266" s="36"/>
       <c r="T266" s="36"/>
       <c r="U266" s="39" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="V266" s="36"/>
       <c r="W266" s="36"/>
@@ -15321,7 +15318,7 @@
       <c r="AF266" s="39"/>
       <c r="AG266" s="39"/>
       <c r="AH266" s="39" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="AI266" s="39"/>
       <c r="AJ266" s="39"/>
@@ -15331,7 +15328,7 @@
         <v>74</v>
       </c>
       <c r="B267" s="35" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C267" s="42" t="s">
         <v>38</v>
@@ -15354,7 +15351,7 @@
       <c r="S267" s="36"/>
       <c r="T267" s="36"/>
       <c r="U267" s="39" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="V267" s="36"/>
       <c r="W267" s="36"/>
@@ -15369,7 +15366,7 @@
       <c r="AF267" s="39"/>
       <c r="AG267" s="39"/>
       <c r="AH267" s="39" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="AI267" s="39"/>
       <c r="AJ267" s="39"/>
@@ -15379,7 +15376,7 @@
         <v>74</v>
       </c>
       <c r="B268" s="35" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C268" s="42" t="s">
         <v>38</v>
@@ -15402,7 +15399,7 @@
       <c r="S268" s="36"/>
       <c r="T268" s="36"/>
       <c r="U268" s="39" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V268" s="36"/>
       <c r="W268" s="36"/>
@@ -15417,7 +15414,7 @@
       <c r="AF268" s="39"/>
       <c r="AG268" s="39"/>
       <c r="AH268" s="39" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="AI268" s="39"/>
       <c r="AJ268" s="39"/>
@@ -15427,7 +15424,7 @@
         <v>74</v>
       </c>
       <c r="B269" s="35" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C269" s="42" t="s">
         <v>38</v>
@@ -15450,7 +15447,7 @@
       <c r="S269" s="36"/>
       <c r="T269" s="36"/>
       <c r="U269" s="39" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="V269" s="36"/>
       <c r="W269" s="36"/>
@@ -15465,7 +15462,7 @@
       <c r="AF269" s="39"/>
       <c r="AG269" s="39"/>
       <c r="AH269" s="39" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="AI269" s="39"/>
       <c r="AJ269" s="39"/>
@@ -15475,7 +15472,7 @@
         <v>74</v>
       </c>
       <c r="B270" s="35" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C270" s="42" t="s">
         <v>38</v>
@@ -15498,7 +15495,7 @@
       <c r="S270" s="36"/>
       <c r="T270" s="36"/>
       <c r="U270" s="39" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="V270" s="36"/>
       <c r="W270" s="36"/>
@@ -15513,7 +15510,7 @@
       <c r="AF270" s="39"/>
       <c r="AG270" s="39"/>
       <c r="AH270" s="39" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="AI270" s="39"/>
       <c r="AJ270" s="39"/>
@@ -15523,7 +15520,7 @@
         <v>74</v>
       </c>
       <c r="B271" s="35" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C271" s="42" t="s">
         <v>38</v>
@@ -15546,7 +15543,7 @@
       <c r="S271" s="36"/>
       <c r="T271" s="36"/>
       <c r="U271" s="39" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="V271" s="36"/>
       <c r="W271" s="36"/>
@@ -15561,7 +15558,7 @@
       <c r="AF271" s="39"/>
       <c r="AG271" s="39"/>
       <c r="AH271" s="39" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="AI271" s="39"/>
       <c r="AJ271" s="39"/>
@@ -15571,7 +15568,7 @@
         <v>74</v>
       </c>
       <c r="B272" s="35" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C272" s="42" t="s">
         <v>38</v>
@@ -15594,7 +15591,7 @@
       <c r="S272" s="36"/>
       <c r="T272" s="36"/>
       <c r="U272" s="39" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="V272" s="36"/>
       <c r="W272" s="36"/>
@@ -15609,7 +15606,7 @@
       <c r="AF272" s="39"/>
       <c r="AG272" s="39"/>
       <c r="AH272" s="39" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="AI272" s="39"/>
       <c r="AJ272" s="39"/>
@@ -15619,7 +15616,7 @@
         <v>74</v>
       </c>
       <c r="B273" s="35" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C273" s="42" t="s">
         <v>38</v>
@@ -15642,7 +15639,7 @@
       <c r="S273" s="36"/>
       <c r="T273" s="36"/>
       <c r="U273" s="39" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="V273" s="36"/>
       <c r="W273" s="36"/>
@@ -15657,7 +15654,7 @@
       <c r="AF273" s="39"/>
       <c r="AG273" s="39"/>
       <c r="AH273" s="39" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="AI273" s="39"/>
       <c r="AJ273" s="39"/>
@@ -15667,7 +15664,7 @@
         <v>74</v>
       </c>
       <c r="B274" s="35" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C274" s="42" t="s">
         <v>38</v>
@@ -15690,7 +15687,7 @@
       <c r="S274" s="36"/>
       <c r="T274" s="36"/>
       <c r="U274" s="39" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="V274" s="36"/>
       <c r="W274" s="36"/>
@@ -15705,7 +15702,7 @@
       <c r="AF274" s="39"/>
       <c r="AG274" s="39"/>
       <c r="AH274" s="39" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AI274" s="39"/>
       <c r="AJ274" s="39"/>
@@ -15715,7 +15712,7 @@
         <v>74</v>
       </c>
       <c r="B275" s="35" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C275" s="42" t="s">
         <v>38</v>
@@ -15738,7 +15735,7 @@
       <c r="S275" s="36"/>
       <c r="T275" s="36"/>
       <c r="U275" s="39" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="V275" s="36"/>
       <c r="W275" s="36"/>
@@ -15753,7 +15750,7 @@
       <c r="AF275" s="39"/>
       <c r="AG275" s="39"/>
       <c r="AH275" s="39" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AI275" s="39"/>
       <c r="AJ275" s="39"/>
@@ -15763,7 +15760,7 @@
         <v>74</v>
       </c>
       <c r="B276" s="35" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C276" s="42" t="s">
         <v>38</v>
@@ -15786,7 +15783,7 @@
       <c r="S276" s="36"/>
       <c r="T276" s="36"/>
       <c r="U276" s="39" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="V276" s="36"/>
       <c r="W276" s="36"/>
@@ -15801,7 +15798,7 @@
       <c r="AF276" s="39"/>
       <c r="AG276" s="39"/>
       <c r="AH276" s="39" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="AI276" s="39"/>
       <c r="AJ276" s="39"/>
@@ -15811,7 +15808,7 @@
         <v>74</v>
       </c>
       <c r="B277" s="35" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C277" s="42" t="s">
         <v>38</v>
@@ -15834,7 +15831,7 @@
       <c r="S277" s="36"/>
       <c r="T277" s="36"/>
       <c r="U277" s="39" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="V277" s="36"/>
       <c r="W277" s="36"/>
@@ -15849,7 +15846,7 @@
       <c r="AF277" s="39"/>
       <c r="AG277" s="39"/>
       <c r="AH277" s="39" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="AI277" s="39"/>
       <c r="AJ277" s="39"/>
@@ -15859,7 +15856,7 @@
         <v>74</v>
       </c>
       <c r="B278" s="35" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C278" s="42" t="s">
         <v>38</v>
@@ -15897,7 +15894,7 @@
       <c r="AF278" s="39"/>
       <c r="AG278" s="39"/>
       <c r="AH278" s="39" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="AI278" s="39"/>
       <c r="AJ278" s="39"/>
@@ -15907,7 +15904,7 @@
         <v>74</v>
       </c>
       <c r="B279" s="35" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C279" s="42" t="s">
         <v>38</v>
@@ -15945,7 +15942,7 @@
       <c r="AF279" s="39"/>
       <c r="AG279" s="39"/>
       <c r="AH279" s="39" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="AI279" s="39"/>
       <c r="AJ279" s="39"/>
@@ -15955,7 +15952,7 @@
         <v>74</v>
       </c>
       <c r="B280" s="35" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C280" s="42" t="s">
         <v>38</v>
@@ -15978,7 +15975,7 @@
       <c r="S280" s="36"/>
       <c r="T280" s="36"/>
       <c r="U280" s="39" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="V280" s="36"/>
       <c r="W280" s="36"/>
@@ -15993,7 +15990,7 @@
       <c r="AF280" s="39"/>
       <c r="AG280" s="39"/>
       <c r="AH280" s="39" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="AI280" s="39"/>
       <c r="AJ280" s="39"/>
@@ -16003,7 +16000,7 @@
         <v>74</v>
       </c>
       <c r="B281" s="35" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C281" s="42" t="s">
         <v>38</v>
@@ -16026,7 +16023,7 @@
       <c r="S281" s="36"/>
       <c r="T281" s="36"/>
       <c r="U281" s="39" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="V281" s="36"/>
       <c r="W281" s="36"/>
@@ -16041,7 +16038,7 @@
       <c r="AF281" s="39"/>
       <c r="AG281" s="39"/>
       <c r="AH281" s="39" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AI281" s="39"/>
       <c r="AJ281" s="39"/>
@@ -16051,7 +16048,7 @@
         <v>74</v>
       </c>
       <c r="B282" s="35" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C282" s="42" t="s">
         <v>38</v>
@@ -16074,7 +16071,7 @@
       <c r="S282" s="36"/>
       <c r="T282" s="36"/>
       <c r="U282" s="39" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="V282" s="36"/>
       <c r="W282" s="36"/>
@@ -16089,7 +16086,7 @@
       <c r="AF282" s="39"/>
       <c r="AG282" s="39"/>
       <c r="AH282" s="39" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="AI282" s="39"/>
       <c r="AJ282" s="39"/>
@@ -16099,7 +16096,7 @@
         <v>74</v>
       </c>
       <c r="B283" s="35" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C283" s="42" t="s">
         <v>38</v>
@@ -16122,7 +16119,7 @@
       <c r="S283" s="36"/>
       <c r="T283" s="36"/>
       <c r="U283" s="39" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="V283" s="36"/>
       <c r="W283" s="36"/>
@@ -16137,7 +16134,7 @@
       <c r="AF283" s="39"/>
       <c r="AG283" s="39"/>
       <c r="AH283" s="39" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AI283" s="39"/>
       <c r="AJ283" s="39"/>
@@ -16147,7 +16144,7 @@
         <v>74</v>
       </c>
       <c r="B284" s="35" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C284" s="42" t="s">
         <v>38</v>
@@ -16170,7 +16167,7 @@
       <c r="S284" s="36"/>
       <c r="T284" s="36"/>
       <c r="U284" s="39" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="V284" s="36"/>
       <c r="W284" s="36"/>
@@ -16185,7 +16182,7 @@
       <c r="AF284" s="39"/>
       <c r="AG284" s="39"/>
       <c r="AH284" s="39" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AI284" s="39"/>
       <c r="AJ284" s="39"/>
@@ -16195,7 +16192,7 @@
         <v>74</v>
       </c>
       <c r="B285" s="35" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C285" s="42" t="s">
         <v>38</v>
@@ -16218,7 +16215,7 @@
       <c r="S285" s="36"/>
       <c r="T285" s="36"/>
       <c r="U285" s="39" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="V285" s="36"/>
       <c r="W285" s="36"/>
@@ -16233,7 +16230,7 @@
       <c r="AF285" s="39"/>
       <c r="AG285" s="39"/>
       <c r="AH285" s="39" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="AI285" s="39"/>
       <c r="AJ285" s="39"/>
@@ -16243,7 +16240,7 @@
         <v>74</v>
       </c>
       <c r="B286" s="35" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C286" s="42" t="s">
         <v>38</v>
@@ -16266,7 +16263,7 @@
       <c r="S286" s="36"/>
       <c r="T286" s="36"/>
       <c r="U286" s="39" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="V286" s="36"/>
       <c r="W286" s="36"/>
@@ -16281,7 +16278,7 @@
       <c r="AF286" s="39"/>
       <c r="AG286" s="39"/>
       <c r="AH286" s="39" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AI286" s="39"/>
       <c r="AJ286" s="39"/>
@@ -16291,7 +16288,7 @@
         <v>74</v>
       </c>
       <c r="B287" s="35" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C287" s="42" t="s">
         <v>38</v>
@@ -16314,7 +16311,7 @@
       <c r="S287" s="36"/>
       <c r="T287" s="36"/>
       <c r="U287" s="39" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="V287" s="36"/>
       <c r="W287" s="36"/>
@@ -16329,7 +16326,7 @@
       <c r="AF287" s="39"/>
       <c r="AG287" s="39"/>
       <c r="AH287" s="39" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="AI287" s="39"/>
       <c r="AJ287" s="39"/>
@@ -16339,7 +16336,7 @@
         <v>74</v>
       </c>
       <c r="B288" s="35" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C288" s="42" t="s">
         <v>38</v>
@@ -16362,7 +16359,7 @@
       <c r="S288" s="36"/>
       <c r="T288" s="36"/>
       <c r="U288" s="39" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="V288" s="36"/>
       <c r="W288" s="36"/>
@@ -16377,7 +16374,7 @@
       <c r="AF288" s="39"/>
       <c r="AG288" s="39"/>
       <c r="AH288" s="39" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="AI288" s="39"/>
       <c r="AJ288" s="39"/>
@@ -16387,7 +16384,7 @@
         <v>74</v>
       </c>
       <c r="B289" s="35" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C289" s="42" t="s">
         <v>38</v>
@@ -16410,7 +16407,7 @@
       <c r="S289" s="36"/>
       <c r="T289" s="36"/>
       <c r="U289" s="39" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="V289" s="36"/>
       <c r="W289" s="36"/>
@@ -16425,7 +16422,7 @@
       <c r="AF289" s="39"/>
       <c r="AG289" s="39"/>
       <c r="AH289" s="39" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="AI289" s="39"/>
       <c r="AJ289" s="39"/>
@@ -16435,7 +16432,7 @@
         <v>74</v>
       </c>
       <c r="B290" s="35" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C290" s="42" t="s">
         <v>38</v>
@@ -16458,7 +16455,7 @@
       <c r="S290" s="36"/>
       <c r="T290" s="36"/>
       <c r="U290" s="39" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="V290" s="36"/>
       <c r="W290" s="36"/>
@@ -16473,7 +16470,7 @@
       <c r="AF290" s="39"/>
       <c r="AG290" s="39"/>
       <c r="AH290" s="39" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="AI290" s="39"/>
       <c r="AJ290" s="39"/>
@@ -16483,7 +16480,7 @@
         <v>74</v>
       </c>
       <c r="B291" s="35" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C291" s="42" t="s">
         <v>38</v>
@@ -16506,7 +16503,7 @@
       <c r="S291" s="36"/>
       <c r="T291" s="36"/>
       <c r="U291" s="39" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="V291" s="36"/>
       <c r="W291" s="36"/>
@@ -16521,7 +16518,7 @@
       <c r="AF291" s="39"/>
       <c r="AG291" s="39"/>
       <c r="AH291" s="39" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AI291" s="39"/>
       <c r="AJ291" s="39"/>
@@ -16531,7 +16528,7 @@
         <v>36</v>
       </c>
       <c r="B292" s="35" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C292" s="42" t="s">
         <v>38</v>
@@ -16575,7 +16572,7 @@
         <v>74</v>
       </c>
       <c r="B293" s="35" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C293" s="42" t="s">
         <v>38</v>
@@ -16598,7 +16595,7 @@
       <c r="S293" s="36"/>
       <c r="T293" s="36"/>
       <c r="U293" s="42" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="V293" s="36"/>
       <c r="W293" s="36"/>
@@ -16613,7 +16610,7 @@
       <c r="AF293" s="39"/>
       <c r="AG293" s="39"/>
       <c r="AH293" s="42" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="AI293" s="39"/>
       <c r="AJ293" s="39"/>
@@ -16623,7 +16620,7 @@
         <v>74</v>
       </c>
       <c r="B294" s="35" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C294" s="42" t="s">
         <v>38</v>
@@ -16646,7 +16643,7 @@
       <c r="S294" s="36"/>
       <c r="T294" s="36"/>
       <c r="U294" s="42" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="V294" s="36"/>
       <c r="W294" s="36"/>
@@ -16671,7 +16668,7 @@
         <v>74</v>
       </c>
       <c r="B295" s="35" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C295" s="42" t="s">
         <v>38</v>
@@ -16694,7 +16691,7 @@
       <c r="S295" s="36"/>
       <c r="T295" s="36"/>
       <c r="U295" s="42" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="V295" s="36"/>
       <c r="W295" s="36"/>
@@ -16709,7 +16706,7 @@
       <c r="AF295" s="39"/>
       <c r="AG295" s="39"/>
       <c r="AH295" s="42" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="AI295" s="39"/>
       <c r="AJ295" s="39"/>
@@ -16719,7 +16716,7 @@
         <v>74</v>
       </c>
       <c r="B296" s="35" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C296" s="42" t="s">
         <v>38</v>
@@ -16742,7 +16739,7 @@
       <c r="S296" s="36"/>
       <c r="T296" s="36"/>
       <c r="U296" s="42" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="V296" s="36"/>
       <c r="W296" s="36"/>
@@ -16767,7 +16764,7 @@
         <v>74</v>
       </c>
       <c r="B297" s="35" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C297" s="42" t="s">
         <v>38</v>
@@ -16790,7 +16787,7 @@
       <c r="S297" s="36"/>
       <c r="T297" s="36"/>
       <c r="U297" s="42" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="V297" s="36"/>
       <c r="W297" s="36"/>
@@ -16805,7 +16802,7 @@
       <c r="AF297" s="39"/>
       <c r="AG297" s="39"/>
       <c r="AH297" s="42" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="AI297" s="39"/>
       <c r="AJ297" s="39"/>
@@ -16815,7 +16812,7 @@
         <v>74</v>
       </c>
       <c r="B298" s="35" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C298" s="42" t="s">
         <v>38</v>
@@ -16838,7 +16835,7 @@
       <c r="S298" s="36"/>
       <c r="T298" s="36"/>
       <c r="U298" s="39" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="V298" s="36"/>
       <c r="W298" s="36"/>
@@ -16853,7 +16850,7 @@
       <c r="AF298" s="39"/>
       <c r="AG298" s="39"/>
       <c r="AH298" s="42" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="AI298" s="39"/>
       <c r="AJ298" s="39"/>
@@ -16863,7 +16860,7 @@
         <v>55</v>
       </c>
       <c r="B299" s="35" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C299" s="36"/>
       <c r="D299" s="37"/>
@@ -16905,7 +16902,7 @@
         <v>55</v>
       </c>
       <c r="B300" s="35" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C300" s="36"/>
       <c r="D300" s="37"/>
@@ -17023,7 +17020,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="43" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B1" s="43" t="s">
         <v>1</v>
@@ -17050,7 +17047,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="51" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="K1" s="51"/>
       <c r="L1" s="51"/>
@@ -17070,13 +17067,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="51" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B2" s="51" t="s">
         <v>101</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
@@ -17103,13 +17100,13 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="51" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B3" s="51" t="s">
         <v>137</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -17163,13 +17160,13 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="51" t="s">
+        <v>585</v>
+      </c>
+      <c r="B5" s="51" t="s">
         <v>586</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="C5" s="11" t="s">
         <v>587</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>588</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
@@ -17196,13 +17193,13 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="51" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B6" s="51" t="s">
+        <v>588</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>589</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>590</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -17256,13 +17253,13 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="51" t="s">
+        <v>590</v>
+      </c>
+      <c r="B8" s="51" t="s">
         <v>591</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="C8" s="11" t="s">
         <v>592</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>593</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
@@ -17289,13 +17286,13 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="51" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B9" s="51" t="s">
+        <v>593</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>594</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>595</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -17322,13 +17319,13 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="51" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B10" s="51" t="s">
+        <v>595</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>596</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>597</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
@@ -17382,13 +17379,13 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="51" t="s">
+        <v>597</v>
+      </c>
+      <c r="B12" s="51" t="s">
         <v>598</v>
       </c>
-      <c r="B12" s="51" t="s">
-        <v>599</v>
-      </c>
       <c r="C12" s="11" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
@@ -17415,13 +17412,13 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="51" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
@@ -17448,13 +17445,13 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="51" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
@@ -17508,13 +17505,13 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="51" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D16" s="51"/>
       <c r="E16" s="51"/>
@@ -17541,13 +17538,13 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="51" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D17" s="51"/>
       <c r="E17" s="51"/>
@@ -17601,13 +17598,13 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="51" t="s">
+        <v>602</v>
+      </c>
+      <c r="B19" s="51" t="s">
         <v>603</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="C19" s="51" t="s">
         <v>604</v>
-      </c>
-      <c r="C19" s="51" t="s">
-        <v>605</v>
       </c>
       <c r="D19" s="51"/>
       <c r="E19" s="51"/>
@@ -17634,13 +17631,13 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="51" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B20" s="51" t="s">
+        <v>605</v>
+      </c>
+      <c r="C20" s="51" t="s">
         <v>606</v>
-      </c>
-      <c r="C20" s="51" t="s">
-        <v>607</v>
       </c>
       <c r="D20" s="51"/>
       <c r="E20" s="51"/>
@@ -17667,13 +17664,13 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="51" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B21" s="51" t="s">
+        <v>595</v>
+      </c>
+      <c r="C21" s="51" t="s">
         <v>596</v>
-      </c>
-      <c r="C21" s="51" t="s">
-        <v>597</v>
       </c>
       <c r="D21" s="51"/>
       <c r="E21" s="51"/>
@@ -17829,10 +17826,10 @@
         <v>177</v>
       </c>
       <c r="B26" s="11" t="s">
+        <v>595</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>596</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>597</v>
       </c>
       <c r="D26" s="51"/>
       <c r="E26" s="51"/>
@@ -18056,10 +18053,10 @@
         <v>185</v>
       </c>
       <c r="B33" s="51" t="s">
+        <v>595</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>596</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>597</v>
       </c>
       <c r="D33" s="51"/>
       <c r="E33" s="51"/>
@@ -18115,13 +18112,13 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="51" t="s">
+        <v>607</v>
+      </c>
+      <c r="B35" s="51" t="s">
         <v>608</v>
       </c>
-      <c r="B35" s="51" t="s">
+      <c r="C35" s="11" t="s">
         <v>609</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>610</v>
       </c>
       <c r="D35" s="51"/>
       <c r="E35" s="51"/>
@@ -18148,13 +18145,13 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="51" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B36" s="51" t="s">
+        <v>610</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>611</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>612</v>
       </c>
       <c r="D36" s="51"/>
       <c r="E36" s="51"/>
@@ -18208,13 +18205,13 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="51" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B38" s="51" t="s">
         <v>137</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D38" s="51"/>
       <c r="E38" s="51"/>
@@ -18241,13 +18238,13 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="51" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B39" s="51" t="s">
         <v>101</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D39" s="51"/>
       <c r="E39" s="51"/>
@@ -18301,13 +18298,13 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="51" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B41" s="51" t="s">
         <v>137</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D41" s="51"/>
       <c r="E41" s="51"/>
@@ -18334,13 +18331,13 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="51" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B42" s="51" t="s">
         <v>101</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D42" s="51"/>
       <c r="E42" s="51"/>
@@ -18394,13 +18391,13 @@
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="51" t="s">
+        <v>617</v>
+      </c>
+      <c r="B44" s="51" t="s">
         <v>618</v>
       </c>
-      <c r="B44" s="51" t="s">
+      <c r="C44" s="11" t="s">
         <v>619</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>620</v>
       </c>
       <c r="D44" s="51"/>
       <c r="E44" s="51"/>
@@ -18427,13 +18424,13 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="51" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B45" s="51" t="s">
+        <v>620</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>621</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>622</v>
       </c>
       <c r="D45" s="51"/>
       <c r="E45" s="51"/>
@@ -18460,13 +18457,13 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="51" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B46" s="51" t="s">
+        <v>622</v>
+      </c>
+      <c r="C46" s="11" t="s">
         <v>623</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>624</v>
       </c>
       <c r="D46" s="51"/>
       <c r="E46" s="51"/>
@@ -18493,13 +18490,13 @@
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="51" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B47" s="51" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D47" s="51"/>
       <c r="E47" s="51"/>
@@ -18553,13 +18550,13 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="51" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B49" s="51" t="s">
+        <v>625</v>
+      </c>
+      <c r="C49" s="51" t="s">
         <v>626</v>
-      </c>
-      <c r="C49" s="51" t="s">
-        <v>627</v>
       </c>
       <c r="D49" s="51"/>
       <c r="E49" s="51"/>
@@ -18588,13 +18585,13 @@
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="51" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B50" s="51" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D50" s="51"/>
       <c r="E50" s="51"/>
@@ -18623,13 +18620,13 @@
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="51" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B51" s="51" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D51" s="51"/>
       <c r="E51" s="51"/>
@@ -18658,13 +18655,13 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="51" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B52" s="51" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D52" s="51"/>
       <c r="E52" s="51"/>
@@ -18693,13 +18690,13 @@
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="51" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B53" s="51" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D53" s="51"/>
       <c r="E53" s="51"/>
@@ -18755,13 +18752,13 @@
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="51" t="s">
+        <v>631</v>
+      </c>
+      <c r="B55" s="51" t="s">
         <v>632</v>
       </c>
-      <c r="B55" s="51" t="s">
+      <c r="C55" s="11" t="s">
         <v>633</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>634</v>
       </c>
       <c r="D55" s="51"/>
       <c r="E55" s="51"/>
@@ -18788,13 +18785,13 @@
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="51" t="s">
+        <v>634</v>
+      </c>
+      <c r="B56" s="51" t="s">
         <v>635</v>
       </c>
-      <c r="B56" s="51" t="s">
+      <c r="C56" s="11" t="s">
         <v>636</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>637</v>
       </c>
       <c r="D56" s="51"/>
       <c r="E56" s="51"/>
@@ -20337,25 +20334,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="52" t="s">
+        <v>637</v>
+      </c>
+      <c r="B1" s="52" t="s">
         <v>638</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="C1" s="52" t="s">
         <v>639</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="D1" s="52" t="s">
         <v>640</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="E1" s="52" t="s">
         <v>641</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="F1" s="52" t="s">
         <v>642</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="G1" s="53" t="s">
         <v>643</v>
-      </c>
-      <c r="G1" s="53" t="s">
-        <v>644</v>
       </c>
       <c r="H1" s="52"/>
       <c r="I1" s="52"/>
@@ -20379,24 +20376,24 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="B2" s="54" t="s">
         <v>645</v>
-      </c>
-      <c r="B2" s="54" t="s">
-        <v>646</v>
       </c>
       <c r="C2" s="55" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2025-09-05  13-33</v>
+        <v>2025-10-22  10-35</v>
       </c>
       <c r="D2" s="56" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F2" s="57"/>
       <c r="G2" s="57" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H2" s="57"/>
       <c r="I2" s="57"/>
@@ -20450,7 +20447,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="52" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>1</v>
@@ -20493,13 +20490,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="65" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B2" s="65" t="s">
         <v>101</v>
       </c>
       <c r="C2" s="65" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D2" s="65"/>
       <c r="E2" s="65"/>
@@ -20524,13 +20521,13 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="65" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B3" s="65" t="s">
         <v>137</v>
       </c>
       <c r="C3" s="65" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D3" s="65"/>
       <c r="E3" s="65"/>
@@ -20580,13 +20577,13 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="65" t="s">
+        <v>648</v>
+      </c>
+      <c r="B5" s="65" t="s">
         <v>649</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="C5" s="65" t="s">
         <v>650</v>
-      </c>
-      <c r="C5" s="65" t="s">
-        <v>651</v>
       </c>
       <c r="D5" s="65"/>
       <c r="E5" s="65"/>
@@ -20611,13 +20608,13 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="65" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B6" s="65" t="s">
+        <v>651</v>
+      </c>
+      <c r="C6" s="65" t="s">
         <v>652</v>
-      </c>
-      <c r="C6" s="65" t="s">
-        <v>653</v>
       </c>
       <c r="D6" s="65"/>
       <c r="E6" s="65"/>
@@ -20642,13 +20639,13 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="65" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B7" s="65" t="s">
+        <v>653</v>
+      </c>
+      <c r="C7" s="65" t="s">
         <v>654</v>
-      </c>
-      <c r="C7" s="65" t="s">
-        <v>655</v>
       </c>
       <c r="D7" s="65"/>
       <c r="E7" s="65"/>
@@ -20673,13 +20670,13 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="65" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B8" s="65" t="s">
+        <v>655</v>
+      </c>
+      <c r="C8" s="65" t="s">
         <v>656</v>
-      </c>
-      <c r="C8" s="65" t="s">
-        <v>657</v>
       </c>
       <c r="D8" s="65"/>
       <c r="E8" s="65"/>
@@ -20704,13 +20701,13 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="65" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B9" s="65" t="s">
+        <v>657</v>
+      </c>
+      <c r="C9" s="65" t="s">
         <v>658</v>
-      </c>
-      <c r="C9" s="65" t="s">
-        <v>659</v>
       </c>
       <c r="D9" s="65"/>
       <c r="E9" s="65"/>
@@ -20760,13 +20757,13 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="65" t="s">
+        <v>659</v>
+      </c>
+      <c r="B11" s="65" t="s">
         <v>660</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="C11" s="65" t="s">
         <v>661</v>
-      </c>
-      <c r="C11" s="65" t="s">
-        <v>662</v>
       </c>
       <c r="D11" s="65"/>
       <c r="E11" s="65"/>
@@ -20791,13 +20788,13 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="65" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B12" s="65" t="s">
+        <v>662</v>
+      </c>
+      <c r="C12" s="65" t="s">
         <v>663</v>
-      </c>
-      <c r="C12" s="65" t="s">
-        <v>664</v>
       </c>
       <c r="D12" s="65"/>
       <c r="E12" s="65"/>
@@ -20822,13 +20819,13 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="65" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B13" s="65" t="s">
+        <v>664</v>
+      </c>
+      <c r="C13" s="65" t="s">
         <v>665</v>
-      </c>
-      <c r="C13" s="65" t="s">
-        <v>666</v>
       </c>
       <c r="D13" s="65"/>
       <c r="E13" s="65"/>
@@ -20853,13 +20850,13 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="65" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B14" s="65" t="s">
+        <v>666</v>
+      </c>
+      <c r="C14" s="65" t="s">
         <v>667</v>
-      </c>
-      <c r="C14" s="65" t="s">
-        <v>668</v>
       </c>
       <c r="D14" s="65"/>
       <c r="E14" s="65"/>
@@ -20884,13 +20881,13 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="65" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B15" s="65" t="s">
+        <v>668</v>
+      </c>
+      <c r="C15" s="65" t="s">
         <v>669</v>
-      </c>
-      <c r="C15" s="65" t="s">
-        <v>670</v>
       </c>
       <c r="D15" s="65"/>
       <c r="E15" s="65"/>
@@ -20915,13 +20912,13 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="65" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B16" s="65" t="s">
+        <v>670</v>
+      </c>
+      <c r="C16" s="65" t="s">
         <v>671</v>
-      </c>
-      <c r="C16" s="65" t="s">
-        <v>672</v>
       </c>
       <c r="D16" s="65"/>
       <c r="E16" s="65"/>
@@ -20971,13 +20968,13 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="65" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B18" s="65" t="s">
+        <v>660</v>
+      </c>
+      <c r="C18" s="65" t="s">
         <v>661</v>
-      </c>
-      <c r="C18" s="65" t="s">
-        <v>662</v>
       </c>
       <c r="D18" s="65"/>
       <c r="E18" s="65"/>
@@ -21002,13 +20999,13 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="65" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B19" s="65" t="s">
+        <v>662</v>
+      </c>
+      <c r="C19" s="65" t="s">
         <v>663</v>
-      </c>
-      <c r="C19" s="65" t="s">
-        <v>664</v>
       </c>
       <c r="D19" s="65"/>
       <c r="E19" s="65"/>
@@ -21033,13 +21030,13 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="65" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B20" s="65" t="s">
+        <v>664</v>
+      </c>
+      <c r="C20" s="65" t="s">
         <v>665</v>
-      </c>
-      <c r="C20" s="65" t="s">
-        <v>666</v>
       </c>
       <c r="D20" s="65"/>
       <c r="E20" s="65"/>
@@ -21064,13 +21061,13 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="65" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B21" s="65" t="s">
+        <v>666</v>
+      </c>
+      <c r="C21" s="65" t="s">
         <v>667</v>
-      </c>
-      <c r="C21" s="65" t="s">
-        <v>668</v>
       </c>
       <c r="D21" s="65"/>
       <c r="E21" s="65"/>
@@ -21095,13 +21092,13 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="65" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B22" s="65" t="s">
+        <v>670</v>
+      </c>
+      <c r="C22" s="65" t="s">
         <v>671</v>
-      </c>
-      <c r="C22" s="65" t="s">
-        <v>672</v>
       </c>
       <c r="D22" s="65"/>
       <c r="E22" s="65"/>
@@ -21126,13 +21123,13 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="65" t="s">
+        <v>672</v>
+      </c>
+      <c r="B23" s="65" t="s">
         <v>673</v>
       </c>
-      <c r="B23" s="65" t="s">
+      <c r="C23" s="65" t="s">
         <v>674</v>
-      </c>
-      <c r="C23" s="65" t="s">
-        <v>675</v>
       </c>
       <c r="D23" s="65"/>
       <c r="E23" s="65"/>
@@ -21182,13 +21179,13 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="65" t="s">
+        <v>675</v>
+      </c>
+      <c r="B25" s="65" t="s">
         <v>676</v>
       </c>
-      <c r="B25" s="65" t="s">
+      <c r="C25" s="65" t="s">
         <v>677</v>
-      </c>
-      <c r="C25" s="65" t="s">
-        <v>678</v>
       </c>
       <c r="D25" s="65"/>
       <c r="E25" s="65"/>
@@ -21213,13 +21210,13 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="65" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B26" s="65" t="s">
+        <v>678</v>
+      </c>
+      <c r="C26" s="65" t="s">
         <v>679</v>
-      </c>
-      <c r="C26" s="65" t="s">
-        <v>680</v>
       </c>
       <c r="D26" s="65"/>
       <c r="E26" s="65"/>
@@ -21244,13 +21241,13 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="65" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B27" s="65" t="s">
+        <v>680</v>
+      </c>
+      <c r="C27" s="65" t="s">
         <v>681</v>
-      </c>
-      <c r="C27" s="65" t="s">
-        <v>682</v>
       </c>
       <c r="D27" s="65"/>
       <c r="E27" s="65"/>
@@ -21275,13 +21272,13 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="65" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B28" s="65" t="s">
+        <v>682</v>
+      </c>
+      <c r="C28" s="65" t="s">
         <v>683</v>
-      </c>
-      <c r="C28" s="65" t="s">
-        <v>684</v>
       </c>
       <c r="D28" s="65"/>
       <c r="E28" s="65"/>
@@ -21306,13 +21303,13 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="65" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B29" s="65" t="s">
+        <v>595</v>
+      </c>
+      <c r="C29" s="65" t="s">
         <v>596</v>
-      </c>
-      <c r="C29" s="65" t="s">
-        <v>597</v>
       </c>
       <c r="D29" s="65"/>
       <c r="E29" s="65"/>
@@ -21362,13 +21359,13 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="65" t="s">
+        <v>684</v>
+      </c>
+      <c r="B31" s="65" t="s">
         <v>685</v>
       </c>
-      <c r="B31" s="65" t="s">
-        <v>686</v>
-      </c>
       <c r="C31" s="65" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D31" s="65"/>
       <c r="E31" s="65"/>
@@ -21393,13 +21390,13 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="65" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B32" s="65" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C32" s="65" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D32" s="65"/>
       <c r="E32" s="65"/>
@@ -21449,14 +21446,14 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="66" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B34" s="66" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C34, "(", ""), ")", "")), " ", "_")</f>
         <v>combined_oral_contraceptives</v>
       </c>
       <c r="C34" s="66" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D34" s="66"/>
       <c r="E34" s="66"/>
@@ -21481,14 +21478,14 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="66" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B35" s="66" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C35, "(", ""), ")", "")), " ", "_")</f>
         <v>progesterone_only_pills</v>
       </c>
       <c r="C35" s="66" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D35" s="66"/>
       <c r="E35" s="66"/>
@@ -21513,14 +21510,14 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="66" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B36" s="66" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C36, "(", ""), ")", "")), " ", "_")</f>
         <v>injectibles</v>
       </c>
       <c r="C36" s="66" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D36" s="66"/>
       <c r="E36" s="66"/>
@@ -21545,14 +21542,14 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="66" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B37" s="66" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C37, "(", ""), ")", "")), " ", "_")</f>
         <v>implants_1_rod</v>
       </c>
       <c r="C37" s="66" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D37" s="66"/>
       <c r="E37" s="66"/>
@@ -21577,14 +21574,14 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="66" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B38" s="66" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C38, "(", ""), ")", "")), " ", "_")</f>
         <v>implants_2_rods</v>
       </c>
       <c r="C38" s="66" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D38" s="66"/>
       <c r="E38" s="66"/>
@@ -21609,14 +21606,14 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="66" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B39" s="66" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C39, "(", ""), ")", "")), " ", "_")</f>
         <v>iud</v>
       </c>
       <c r="C39" s="66" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D39" s="66"/>
       <c r="E39" s="66"/>
@@ -21641,14 +21638,14 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="66" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B40" s="66" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C40, "(", ""), ")", "")), " ", "_")</f>
         <v>condoms</v>
       </c>
       <c r="C40" s="66" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D40" s="66"/>
       <c r="E40" s="66"/>
@@ -21673,14 +21670,14 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="66" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B41" s="66" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C41, "(", ""), ")", "")), " ", "_")</f>
         <v>tubal_ligation</v>
       </c>
       <c r="C41" s="66" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D41" s="66"/>
       <c r="E41" s="66"/>
@@ -21705,14 +21702,14 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="66" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B42" s="66" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C42, "(", ""), ")", "")), " ", "_")</f>
         <v>cycle_beads</v>
       </c>
       <c r="C42" s="66" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D42" s="66"/>
       <c r="E42" s="66"/>
@@ -21737,13 +21734,13 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="66" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B43" s="66" t="s">
+        <v>595</v>
+      </c>
+      <c r="C43" s="66" t="s">
         <v>596</v>
-      </c>
-      <c r="C43" s="66" t="s">
-        <v>597</v>
       </c>
       <c r="D43" s="66"/>
       <c r="E43" s="66"/>
@@ -21774,14 +21771,14 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="66" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B45" s="66" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C45, "(", ""), ")", "")), " ", "_")</f>
         <v>wants_to_get_pregnant</v>
       </c>
       <c r="C45" s="66" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D45" s="66"/>
       <c r="E45" s="66"/>
@@ -21806,14 +21803,14 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="66" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B46" s="66" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C46, "(", ""), ")", "")), " ", "_")</f>
         <v>did_not_want_fp</v>
       </c>
       <c r="C46" s="66" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D46" s="66"/>
       <c r="E46" s="66"/>
@@ -21844,13 +21841,13 @@
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="56" t="s">
+        <v>700</v>
+      </c>
+      <c r="B48" s="56" t="s">
         <v>701</v>
       </c>
-      <c r="B48" s="56" t="s">
+      <c r="C48" s="56" t="s">
         <v>702</v>
-      </c>
-      <c r="C48" s="56" t="s">
-        <v>703</v>
       </c>
       <c r="D48" s="56"/>
       <c r="E48" s="56"/>
@@ -21875,13 +21872,13 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="56" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B49" s="56" t="s">
+        <v>703</v>
+      </c>
+      <c r="C49" s="56" t="s">
         <v>704</v>
-      </c>
-      <c r="C49" s="56" t="s">
-        <v>705</v>
       </c>
       <c r="D49" s="56"/>
       <c r="E49" s="56"/>
@@ -21906,13 +21903,13 @@
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="66" t="s">
+        <v>705</v>
+      </c>
+      <c r="B51" s="66" t="s">
         <v>706</v>
       </c>
-      <c r="B51" s="66" t="s">
+      <c r="C51" s="66" t="s">
         <v>707</v>
-      </c>
-      <c r="C51" s="66" t="s">
-        <v>708</v>
       </c>
       <c r="D51" s="66"/>
       <c r="E51" s="66"/>
@@ -21937,13 +21934,13 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="66" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B52" s="66" t="s">
+        <v>708</v>
+      </c>
+      <c r="C52" s="66" t="s">
         <v>709</v>
-      </c>
-      <c r="C52" s="66" t="s">
-        <v>710</v>
       </c>
       <c r="D52" s="66"/>
       <c r="E52" s="66"/>
@@ -21968,13 +21965,13 @@
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="66" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B53" s="66" t="s">
+        <v>710</v>
+      </c>
+      <c r="C53" s="66" t="s">
         <v>711</v>
-      </c>
-      <c r="C53" s="66" t="s">
-        <v>712</v>
       </c>
       <c r="D53" s="66"/>
       <c r="E53" s="66"/>
@@ -21999,13 +21996,13 @@
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="66" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B54" s="66" t="s">
+        <v>712</v>
+      </c>
+      <c r="C54" s="66" t="s">
         <v>713</v>
-      </c>
-      <c r="C54" s="66" t="s">
-        <v>714</v>
       </c>
       <c r="D54" s="66"/>
       <c r="E54" s="66"/>
@@ -22030,13 +22027,13 @@
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="66" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B55" s="66" t="s">
+        <v>714</v>
+      </c>
+      <c r="C55" s="66" t="s">
         <v>715</v>
-      </c>
-      <c r="C55" s="66" t="s">
-        <v>716</v>
       </c>
       <c r="D55" s="66"/>
       <c r="E55" s="66"/>
@@ -22061,13 +22058,13 @@
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="66" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B56" s="66" t="s">
+        <v>595</v>
+      </c>
+      <c r="C56" s="66" t="s">
         <v>596</v>
-      </c>
-      <c r="C56" s="66" t="s">
-        <v>597</v>
       </c>
       <c r="D56" s="66"/>
       <c r="E56" s="66"/>
@@ -22092,112 +22089,112 @@
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="56" t="s">
+        <v>716</v>
+      </c>
+      <c r="B58" s="56" t="s">
         <v>717</v>
       </c>
-      <c r="B58" s="56" t="s">
+      <c r="C58" s="56" t="s">
         <v>718</v>
-      </c>
-      <c r="C58" s="56" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="56" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B59" s="56" t="s">
+        <v>719</v>
+      </c>
+      <c r="C59" s="56" t="s">
         <v>720</v>
-      </c>
-      <c r="C59" s="56" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="56" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B60" s="56" t="s">
+        <v>721</v>
+      </c>
+      <c r="C60" s="56" t="s">
         <v>722</v>
-      </c>
-      <c r="C60" s="56" t="s">
-        <v>723</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="56" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B61" s="56" t="s">
+        <v>595</v>
+      </c>
+      <c r="C61" s="56" t="s">
         <v>596</v>
-      </c>
-      <c r="C61" s="56" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="57" t="s">
+        <v>723</v>
+      </c>
+      <c r="B63" s="57" t="s">
         <v>724</v>
       </c>
-      <c r="B63" s="57" t="s">
+      <c r="C63" s="56" t="s">
         <v>725</v>
-      </c>
-      <c r="C63" s="56" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="57" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B64" s="57" t="s">
+        <v>726</v>
+      </c>
+      <c r="C64" s="56" t="s">
         <v>727</v>
-      </c>
-      <c r="C64" s="56" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="57" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B65" s="57" t="s">
+        <v>728</v>
+      </c>
+      <c r="C65" s="56" t="s">
         <v>729</v>
-      </c>
-      <c r="C65" s="56" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="57" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B66" s="57" t="s">
+        <v>730</v>
+      </c>
+      <c r="C66" s="56" t="s">
         <v>731</v>
-      </c>
-      <c r="C66" s="56" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="57" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B67" s="57" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C67" s="56" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="66" t="s">
+        <v>732</v>
+      </c>
+      <c r="B69" s="66" t="s">
         <v>733</v>
       </c>
-      <c r="B69" s="66" t="s">
+      <c r="C69" s="66" t="s">
         <v>734</v>
-      </c>
-      <c r="C69" s="66" t="s">
-        <v>735</v>
       </c>
       <c r="D69" s="66"/>
       <c r="E69" s="66"/>
@@ -22222,13 +22219,13 @@
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="66" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B70" s="66" t="s">
+        <v>735</v>
+      </c>
+      <c r="C70" s="66" t="s">
         <v>736</v>
-      </c>
-      <c r="C70" s="66" t="s">
-        <v>737</v>
       </c>
       <c r="D70" s="66"/>
       <c r="E70" s="66"/>
@@ -22253,24 +22250,24 @@
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="66" t="s">
+        <v>737</v>
+      </c>
+      <c r="B72" s="66" t="s">
         <v>738</v>
       </c>
-      <c r="B72" s="66" t="s">
-        <v>739</v>
-      </c>
       <c r="C72" s="67" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="66" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B73" s="66" t="s">
+        <v>739</v>
+      </c>
+      <c r="C73" s="66" t="s">
         <v>740</v>
-      </c>
-      <c r="C73" s="66" t="s">
-        <v>741</v>
       </c>
       <c r="D73" s="66"/>
       <c r="E73" s="66"/>
@@ -22295,13 +22292,13 @@
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="66" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B74" s="66" t="s">
+        <v>595</v>
+      </c>
+      <c r="C74" s="66" t="s">
         <v>596</v>
-      </c>
-      <c r="C74" s="66" t="s">
-        <v>597</v>
       </c>
       <c r="D74" s="66"/>
       <c r="E74" s="66"/>

</xml_diff>